<commit_message>
PyPi NMR entries added, polishing
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{649C5C71-29A4-4342-8FCA-26FD323E74BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{02890DDC-40F3-7647-A223-C98F3938A77B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000"/>
+    <workbookView xWindow="440" yWindow="2820" windowWidth="25140" windowHeight="13120"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="196">
   <si>
     <t>name</t>
   </si>
@@ -94,9 +94,6 @@
     <t>NMR data acquisition &amp; processing (Varian instruments)</t>
   </si>
   <si>
-    <t>nD NMR</t>
-  </si>
-  <si>
     <t>nmrGlue</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t>1D NMR processing for metabolomics using [NMRProcFlow](https://nmrprocflow.org/)</t>
   </si>
   <si>
-    <t>1D NMR only (native R &amp; VM)</t>
-  </si>
-  <si>
     <t>TIMP</t>
   </si>
   <si>
@@ -362,6 +356,258 @@
   </si>
   <si>
     <t>repository</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/nmrstarlib/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/nmrsim/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/pybmrb/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/bionmr-utils/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/blochsimu/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/icoshift/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/paramagpy/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/chemex/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/famn-opt/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/pynmrstar/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/spike-py/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/drawnmr/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/biceps/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/peakipy/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/bfit/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/pySpecData/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/mwtab/</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/nmrml2isa/</t>
+  </si>
+  <si>
+    <t>nmrstarlib</t>
+  </si>
+  <si>
+    <t>https://github.com/MoseleyBioinformaticsLab/nmrstarlib</t>
+  </si>
+  <si>
+    <t>https://bmcbioinformatics.biomedcentral.com/articles/10.1186/s12859-017-1580-5</t>
+  </si>
+  <si>
+    <t>I/O NMR-STAR files to JSON used by BMRB</t>
+  </si>
+  <si>
+    <t>Solution NMR simulation</t>
+  </si>
+  <si>
+    <t>https://github.com/sametz/nmrsim</t>
+  </si>
+  <si>
+    <t>nmrsim</t>
+  </si>
+  <si>
+    <t>PyBMRB</t>
+  </si>
+  <si>
+    <t>https://github.com/uwbmrb/PyBMRB</t>
+  </si>
+  <si>
+    <t>Visualizations based on BMRB data</t>
+  </si>
+  <si>
+    <t>https://github.com/ahmohamed/nmrpro</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/nmrpro/</t>
+  </si>
+  <si>
+    <t>NMRpro</t>
+  </si>
+  <si>
+    <t>https://github.com/sizmailov/bionmr-utils</t>
+  </si>
+  <si>
+    <t>bionmr-utils</t>
+  </si>
+  <si>
+    <t>blochsimu</t>
+  </si>
+  <si>
+    <t>Simulation of Bloch equations</t>
+  </si>
+  <si>
+    <t>Biological NMR utilities</t>
+  </si>
+  <si>
+    <t>https://github.com/mfitzp/icoshift</t>
+  </si>
+  <si>
+    <t>icoshift</t>
+  </si>
+  <si>
+    <t>https://github.com/k7hoven/blochsimu</t>
+  </si>
+  <si>
+    <t>paramagpy</t>
+  </si>
+  <si>
+    <t>Calculation of protein NMR paramagnetic effects</t>
+  </si>
+  <si>
+    <t>https://github.com/henryorton/paramagpy</t>
+  </si>
+  <si>
+    <t>https://chemrxiv.org/articles/Paramagpy_Software_for_Fitting_Magnetic_Susceptibility_Tensors_Using_Paramagnetic_Effects_Measured_in_NMR_Spectra/9643154/1</t>
+  </si>
+  <si>
+    <t>Analysis of chemical exchange by NMR</t>
+  </si>
+  <si>
+    <t>ChemEx</t>
+  </si>
+  <si>
+    <t>https://github.com/gbouvignies/chemex</t>
+  </si>
+  <si>
+    <t>https://github.com/hcolaux/famn_opt</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/10.1021/jp505752c</t>
+  </si>
+  <si>
+    <t>FAM-N</t>
+  </si>
+  <si>
+    <t>PyNMR-STAR</t>
+  </si>
+  <si>
+    <t>I/O NMR-STAR files from BMRB</t>
+  </si>
+  <si>
+    <t>https://github.com/uwbmrb/PyNMRSTAR</t>
+  </si>
+  <si>
+    <t>SPIKE</t>
+  </si>
+  <si>
+    <t>Processing 1D/2D spectroscopic data</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/delsuc/spike/src/default/</t>
+  </si>
+  <si>
+    <t>drawnmr</t>
+  </si>
+  <si>
+    <t>Visualize NMR data</t>
+  </si>
+  <si>
+    <t>https://github.com/tlinnet/drawnmr</t>
+  </si>
+  <si>
+    <t>BICePs</t>
+  </si>
+  <si>
+    <t>Bayesian inference of conformational populations from NMR data</t>
+  </si>
+  <si>
+    <t>https://github.com/vvoelz/biceps/</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/10.1021/acs.jpcb.7b11871</t>
+  </si>
+  <si>
+    <t>Peakipy</t>
+  </si>
+  <si>
+    <t>Deconvolution of 2D NMR peaks</t>
+  </si>
+  <si>
+    <t>https://github.com/j-brady/peakipy</t>
+  </si>
+  <si>
+    <t>bfit</t>
+  </si>
+  <si>
+    <t>https://github.com/dfujim/bfit</t>
+  </si>
+  <si>
+    <t>https://github.com/jmfrancklab/pyspecdata</t>
+  </si>
+  <si>
+    <t>Process multidimensional data</t>
+  </si>
+  <si>
+    <t>NMR, ESR</t>
+  </si>
+  <si>
+    <t>pySpecData</t>
+  </si>
+  <si>
+    <t>mwTab</t>
+  </si>
+  <si>
+    <t>I/O mwTab files</t>
+  </si>
+  <si>
+    <t>https://github.com/MoseleyBioinformaticsLab/mwtab</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007%2Fs11306-018-1356-6</t>
+  </si>
+  <si>
+    <t>nmrml2isa</t>
+  </si>
+  <si>
+    <t>https://github.com/ISA-tools/nmrml2isa</t>
+  </si>
+  <si>
+    <t>Convert nmrML files to ISA-TAB [Qt interface](https://pypi.org/project/nmrml2isa-qt/)</t>
+  </si>
+  <si>
+    <t>nD NMR only</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nD NMR only</t>
+  </si>
+  <si>
+    <t>Process &amp; visualize NMR data (Django app available; uses nmrGlue)</t>
+  </si>
+  <si>
+    <t>1D NMR alignment via ICOSHIFT algorithm</t>
+  </si>
+  <si>
+    <t>Optimize composite pulses for MQMAS</t>
+  </si>
+  <si>
+    <t>Visualize NMR data (uses nmrGlue)</t>
   </si>
 </sst>
 </file>
@@ -1203,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1228,16 +1474,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1320,141 +1566,141 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -1462,90 +1708,90 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
         <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
         <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" t="s">
-        <v>75</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -1556,16 +1802,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
@@ -1573,124 +1819,504 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
         <v>82</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>83</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
         <v>87</v>
-      </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" t="s">
-        <v>89</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
         <v>91</v>
-      </c>
-      <c r="B21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" t="s">
-        <v>93</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
         <v>98</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>99</v>
-      </c>
-      <c r="C23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" t="s">
-        <v>101</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" t="s">
         <v>106</v>
-      </c>
-      <c r="B25" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" t="s">
-        <v>108</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>192</v>
+      </c>
+      <c r="G29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>146</v>
+      </c>
+      <c r="G31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>157</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" t="s">
+        <v>155</v>
+      </c>
+      <c r="G34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" t="s">
+        <v>194</v>
+      </c>
+      <c r="G35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>195</v>
+      </c>
+      <c r="G38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" t="s">
+        <v>173</v>
+      </c>
+      <c r="E39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>175</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" t="s">
+        <v>178</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s">
+        <v>180</v>
+      </c>
+      <c r="G42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
+        <v>185</v>
+      </c>
+      <c r="D43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s">
+        <v>184</v>
+      </c>
+      <c r="G43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>187</v>
+      </c>
+      <c r="B44" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s">
+        <v>189</v>
+      </c>
+      <c r="G44" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added basic URL checking
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{02890DDC-40F3-7647-A223-C98F3938A77B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AF664F-4BBA-AC48-B0AD-6A39356425C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="2820" windowWidth="25140" windowHeight="13120"/>
+    <workbookView xWindow="440" yWindow="2820" windowWidth="25140" windowHeight="13120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="198">
   <si>
     <t>name</t>
   </si>
@@ -608,12 +608,18 @@
   </si>
   <si>
     <t>Visualize NMR data (uses nmrGlue)</t>
+  </si>
+  <si>
+    <t>jcamp</t>
+  </si>
+  <si>
+    <t>Read JCAMP-DX files</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1448,11 +1454,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2319,6 +2325,17 @@
         <v>51</v>
       </c>
     </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>196</v>
+      </c>
+      <c r="E45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" t="s">
+        <v>197</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Polishing site & T-CI
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AF664F-4BBA-AC48-B0AD-6A39356425C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27861F42-6AD7-AE4C-B441-F3EB44E4206A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="2820" windowWidth="25140" windowHeight="13120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="201">
   <si>
     <t>name</t>
   </si>
@@ -614,6 +614,15 @@
   </si>
   <si>
     <t>Read JCAMP-DX files</t>
+  </si>
+  <si>
+    <t>https://bryanhanson.github.io/bad_page.html</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test entry</t>
   </si>
 </sst>
 </file>
@@ -1097,9 +1106,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1455,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2329,11 +2341,31 @@
       <c r="A45" t="s">
         <v>196</v>
       </c>
+      <c r="B45" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="E45" t="s">
         <v>28</v>
       </c>
       <c r="F45" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E46" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G46" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added simplerspec & nhazen/jcamp
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27861F42-6AD7-AE4C-B441-F3EB44E4206A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F49793-280E-F54E-834E-349B859937B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="2820" windowWidth="25140" windowHeight="13120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="2520" windowWidth="25140" windowHeight="13120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="205">
   <si>
     <t>name</t>
   </si>
@@ -623,6 +623,18 @@
   </si>
   <si>
     <t>test entry</t>
+  </si>
+  <si>
+    <t>simplerspec</t>
+  </si>
+  <si>
+    <t>https://github.com/philipp-baumann/simplerspec</t>
+  </si>
+  <si>
+    <t>https://github.com/philipp-baumann/simplerspec-pedometron-article</t>
+  </si>
+  <si>
+    <t>https://github.com/nzhagen/jcamp</t>
   </si>
 </sst>
 </file>
@@ -1467,16 +1479,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
     <col min="4" max="4" width="71.5" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
@@ -2341,8 +2353,9 @@
       <c r="A45" t="s">
         <v>196</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>198</v>
+      <c r="B45" s="2"/>
+      <c r="C45" t="s">
+        <v>204</v>
       </c>
       <c r="E45" t="s">
         <v>28</v>
@@ -2353,19 +2366,39 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>198</v>
       </c>
+      <c r="C46" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>199</v>
       </c>
       <c r="F46" t="s">
         <v>200</v>
       </c>
       <c r="G46" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>201</v>
+      </c>
+      <c r="B47" t="s">
+        <v>203</v>
+      </c>
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
polishing the input data
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC642CE7-BE7F-0E40-8C40-72782FA8B4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD7F6B9-9EE5-544E-A0CB-4135190A5847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27120" yWindow="1000" windowWidth="31620" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="250">
   <si>
     <t>name</t>
   </si>
@@ -28,9 +28,6 @@
     <t>website</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>ChemoSpec</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>EDA of 2D NMR</t>
   </si>
   <si>
-    <t>2D NMR only</t>
-  </si>
-  <si>
     <t>speaq</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>NMR data processing</t>
   </si>
   <si>
-    <t>1D NMR only</t>
-  </si>
-  <si>
     <t>OpenVnmrJ</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
     <t>https://link.springer.com/article/10.1007%2Fs10858-013-9718-x</t>
   </si>
   <si>
-    <t>Python</t>
-  </si>
-  <si>
     <t>NMR data processing, analysis, visualization &amp; conversion</t>
   </si>
   <si>
@@ -175,9 +163,6 @@
     <t>Markup language for sharing NMR data</t>
   </si>
   <si>
-    <t>NMR only</t>
-  </si>
-  <si>
     <t>rDolphin</t>
   </si>
   <si>
@@ -232,9 +217,6 @@
     <t>Vis and NIR</t>
   </si>
   <si>
-    <t>Vis-NIR only?</t>
-  </si>
-  <si>
     <t>resemble</t>
   </si>
   <si>
@@ -307,9 +289,6 @@
     <t>EDA of 1D NMR</t>
   </si>
   <si>
-    <t>1D NMR only?</t>
-  </si>
-  <si>
     <t>serrsBayes</t>
   </si>
   <si>
@@ -592,12 +571,6 @@
     <t>Convert nmrML files to ISA-TAB [Qt interface](https://pypi.org/project/nmrml2isa-qt/)</t>
   </si>
   <si>
-    <t>nD NMR only</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nD NMR only</t>
-  </si>
-  <si>
     <t>1D NMR alignment via ICOSHIFT algorithm</t>
   </si>
   <si>
@@ -631,9 +604,6 @@
     <t>Process &amp; visualize NMR data (Django app available; uses [nmrGlue](http://www.nmrglue.com/))</t>
   </si>
   <si>
-    <t>mid-IR and near-IR</t>
-  </si>
-  <si>
     <t>pavo</t>
   </si>
   <si>
@@ -643,12 +613,6 @@
     <t>https://github.com/rmaia/pavo/</t>
   </si>
   <si>
-    <t>Perceptual analysis, visualization and organization of spectral color data</t>
-  </si>
-  <si>
-    <t>visual pigments; input is spectra or images</t>
-  </si>
-  <si>
     <t>BATMAN</t>
   </si>
   <si>
@@ -667,12 +631,6 @@
     <t>tameNMR</t>
   </si>
   <si>
-    <t>Command line or runs in [Galaxy](https://galaxyproject.org/)</t>
-  </si>
-  <si>
-    <t>1H NMR metabolomics; uses [nmrglue]() and [speaq]()</t>
-  </si>
-  <si>
     <t>ssNAKE</t>
   </si>
   <si>
@@ -715,9 +673,6 @@
     <t>https://github.com/onemoonsci/nmrfxprocessorgui</t>
   </si>
   <si>
-    <t>Processing, visualization &amp; analsys of NMR data</t>
-  </si>
-  <si>
     <t>https://github.com/dcheshkov/ANATOLIA</t>
   </si>
   <si>
@@ -730,12 +685,6 @@
     <t>C++</t>
   </si>
   <si>
-    <t>Bruker NMR data only, standalone or from with TopSpin</t>
-  </si>
-  <si>
-    <t>NMR lineshhape analysis</t>
-  </si>
-  <si>
     <t>CARA</t>
   </si>
   <si>
@@ -749,6 +698,78 @@
   </si>
   <si>
     <t>Biomolecular NMR peak assignment</t>
+  </si>
+  <si>
+    <t>focus</t>
+  </si>
+  <si>
+    <t>Py</t>
+  </si>
+  <si>
+    <t>NMR (1D)</t>
+  </si>
+  <si>
+    <t>NMR (1D)?</t>
+  </si>
+  <si>
+    <t>NMR</t>
+  </si>
+  <si>
+    <t>NMR (2D)</t>
+  </si>
+  <si>
+    <t>NMR (nD)</t>
+  </si>
+  <si>
+    <t>NMR (SS)</t>
+  </si>
+  <si>
+    <t>NMR lineshape analysis</t>
+  </si>
+  <si>
+    <t>Processing, visualization &amp; analysis of NMR data</t>
+  </si>
+  <si>
+    <t>Data sharing</t>
+  </si>
+  <si>
+    <t>Data sharing (NMR)</t>
+  </si>
+  <si>
+    <t>NMR (13C)</t>
+  </si>
+  <si>
+    <t>Raman</t>
+  </si>
+  <si>
+    <t>Data Sharing</t>
+  </si>
+  <si>
+    <t>Vis-NIR</t>
+  </si>
+  <si>
+    <t>Vis-IR</t>
+  </si>
+  <si>
+    <t>NMR (Bruker)</t>
+  </si>
+  <si>
+    <t>Perceptual analysis, visualization and organization of spectral color data (incl images)</t>
+  </si>
+  <si>
+    <t>UV-Vis</t>
+  </si>
+  <si>
+    <t>Time series</t>
+  </si>
+  <si>
+    <t>Time series (NIR)</t>
+  </si>
+  <si>
+    <t>NIR-MIR</t>
+  </si>
+  <si>
+    <t>1H NMR metabolomics; uses [nmrglue]() and [speaq]() Command line or runs in [Galaxy](https://galaxyproject.org)</t>
   </si>
 </sst>
 </file>
@@ -1611,10 +1632,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1636,1052 +1657,1091 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
-      </c>
       <c r="G6" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>191</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" t="s">
-        <v>50</v>
-      </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
         <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>78</v>
+      </c>
+      <c r="G19" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="G21" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>100</v>
+        <v>93</v>
+      </c>
+      <c r="G23" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="G24" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F26" t="s">
-        <v>133</v>
+        <v>126</v>
+      </c>
+      <c r="G26" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F27" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G27" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F28" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F29" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F30" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F31" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F32" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G32" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F33" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="G33" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F34" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G34" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F35" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F36" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G36" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B37" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F37" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F38" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D39" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F39" t="s">
-        <v>171</v>
+        <v>164</v>
+      </c>
+      <c r="G39" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F40" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G40" t="s">
-        <v>12</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F41" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G41" t="s">
-        <v>95</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F42" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G42" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D43" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E43" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F43" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G43" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E44" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F44" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G44" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E45" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F45" t="s">
-        <v>196</v>
+        <v>187</v>
+      </c>
+      <c r="G45" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B46" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C46" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="G46" t="s">
-        <v>203</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C47" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>207</v>
+        <v>244</v>
       </c>
       <c r="G47" t="s">
-        <v>208</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B48" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C48" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="G48" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B49" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="G49" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B50" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="C50" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="D50" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="F50" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G50" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B51" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C51" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="D51" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="E51" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F51" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="G51" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C52" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" t="s">
+        <v>215</v>
+      </c>
+      <c r="F52" t="s">
+        <v>235</v>
+      </c>
+      <c r="G52" t="s">
         <v>230</v>
-      </c>
-      <c r="E52" t="s">
-        <v>229</v>
-      </c>
-      <c r="F52" t="s">
-        <v>231</v>
-      </c>
-      <c r="G52" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B53" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53" t="s">
+        <v>217</v>
+      </c>
+      <c r="E53" t="s">
+        <v>220</v>
+      </c>
+      <c r="F53" t="s">
         <v>234</v>
       </c>
-      <c r="C53" t="s">
-        <v>232</v>
-      </c>
-      <c r="E53" t="s">
-        <v>235</v>
-      </c>
-      <c r="F53" t="s">
-        <v>237</v>
-      </c>
       <c r="G53" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="B54" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="C54" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="E54" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="F54" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="G54" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New entries to data base
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ED6DFA-0AE2-F34D-8BCB-D95CFC3DC261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3FDE27-DDE0-2A49-B7C5-964E18E37827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="259">
   <si>
     <t>name</t>
   </si>
@@ -739,9 +739,6 @@
     <t>Raman</t>
   </si>
   <si>
-    <t>Vis-NIR</t>
-  </si>
-  <si>
     <t>Vis-IR</t>
   </si>
   <si>
@@ -757,16 +754,49 @@
     <t>Time series</t>
   </si>
   <si>
-    <t>Time series (NIR)</t>
-  </si>
-  <si>
-    <t>NIR-MIR</t>
-  </si>
-  <si>
     <t>1H NMR metabolomics; uses [nmrglue]() and [speaq]() Command line or runs in [Galaxy](https://galaxyproject.org)</t>
   </si>
   <si>
     <t>Data Sharing (NMR)</t>
+  </si>
+  <si>
+    <t>spectacles</t>
+  </si>
+  <si>
+    <t>https://github.com/pierreroudier/spectacles/</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=spectacles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storing, manipulation and analysis </t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=baseline</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>Baseline correction</t>
+  </si>
+  <si>
+    <t>geoSpectral</t>
+  </si>
+  <si>
+    <t>Workflow for data sets with space/time/spectral dimensions</t>
+  </si>
+  <si>
+    <t>Mid-Ir</t>
+  </si>
+  <si>
+    <t>Near-IR, Mid-IR</t>
+  </si>
+  <si>
+    <t>Vis-Near-IR</t>
+  </si>
+  <si>
+    <t>Time series (Near-IR)</t>
   </si>
 </sst>
 </file>
@@ -1627,12 +1657,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1935,7 +1965,7 @@
         <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1955,7 +1985,7 @@
         <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1975,7 +2005,7 @@
         <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2146,7 +2176,7 @@
         <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2169,7 +2199,7 @@
         <v>126</v>
       </c>
       <c r="G26" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2369,7 +2399,7 @@
         <v>155</v>
       </c>
       <c r="G36" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2572,7 +2602,7 @@
         <v>192</v>
       </c>
       <c r="G46" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2589,10 +2619,10 @@
         <v>5</v>
       </c>
       <c r="F47" t="s">
+        <v>241</v>
+      </c>
+      <c r="G47" t="s">
         <v>242</v>
-      </c>
-      <c r="G47" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2629,7 +2659,7 @@
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G49" t="s">
         <v>228</v>
@@ -2718,7 +2748,7 @@
         <v>233</v>
       </c>
       <c r="G53" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -2739,6 +2769,54 @@
       </c>
       <c r="G54" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>246</v>
+      </c>
+      <c r="B55" t="s">
+        <v>248</v>
+      </c>
+      <c r="C55" t="s">
+        <v>247</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>251</v>
+      </c>
+      <c r="B56" t="s">
+        <v>250</v>
+      </c>
+      <c r="E56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>253</v>
+      </c>
+      <c r="B57" t="s">
+        <v>250</v>
+      </c>
+      <c r="E57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" t="s">
+        <v>254</v>
+      </c>
+      <c r="G57" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved ANATOLIA pub to the right place
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DD4AEF-CF94-E34E-987E-21485415EDDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D089581-D20D-DB47-8193-E7EBE8EE1A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1680,7 +1680,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2739,9 +2739,6 @@
       <c r="C52" t="s">
         <v>216</v>
       </c>
-      <c r="D52" t="s">
-        <v>264</v>
-      </c>
       <c r="E52" t="s">
         <v>215</v>
       </c>
@@ -2761,6 +2758,9 @@
       </c>
       <c r="C53" t="s">
         <v>217</v>
+      </c>
+      <c r="D53" t="s">
+        <v>264</v>
       </c>
       <c r="E53" t="s">
         <v>220</v>

</xml_diff>

<commit_message>
fixed errors in xlsx
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D089581-D20D-DB47-8193-E7EBE8EE1A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B6355-B211-5F4A-BAEA-73B242C09004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24740" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="273">
   <si>
     <t>name</t>
   </si>
@@ -187,9 +187,6 @@
     <t>https://link.springer.com/article/10.1007/s11306-017-1178-y</t>
   </si>
   <si>
-    <t>1D NMR processing for metabolomics using [NMRProcFlow](https://nmrprocflow.org/)</t>
-  </si>
-  <si>
     <t>TIMP</t>
   </si>
   <si>
@@ -568,18 +565,12 @@
     <t>https://github.com/ISA-tools/nmrml2isa</t>
   </si>
   <si>
-    <t>Convert nmrML files to ISA-TAB [Qt interface](https://pypi.org/project/nmrml2isa-qt/)</t>
-  </si>
-  <si>
     <t>1D NMR alignment via ICOSHIFT algorithm</t>
   </si>
   <si>
     <t>Optimize composite pulses for MQMAS</t>
   </si>
   <si>
-    <t>Visualize NMR data (uses nmrGlue)</t>
-  </si>
-  <si>
     <t>jcamp</t>
   </si>
   <si>
@@ -598,12 +589,6 @@
     <t>https://github.com/nzhagen/jcamp</t>
   </si>
   <si>
-    <t>Spectral processing &amp; modeling [Uses prospectr in part](https://cran.r-project.org/package=prospectr)</t>
-  </si>
-  <si>
-    <t>Process &amp; visualize NMR data (Django app available; uses [nmrGlue](http://www.nmrglue.com/))</t>
-  </si>
-  <si>
     <t>pavo</t>
   </si>
   <si>
@@ -754,9 +739,6 @@
     <t>Time series</t>
   </si>
   <si>
-    <t>1H NMR metabolomics; uses [nmrglue]() and [speaq]() Command line or runs in [Galaxy](https://galaxyproject.org)</t>
-  </si>
-  <si>
     <t>Data Sharing (NMR)</t>
   </si>
   <si>
@@ -769,9 +751,6 @@
     <t>https://cran.r-project.org/package=spectacles</t>
   </si>
   <si>
-    <t xml:space="preserve">Storing, manipulation and analysis </t>
-  </si>
-  <si>
     <t>https://cran.r-project.org/package=baseline</t>
   </si>
   <si>
@@ -815,6 +794,51 @@
   </si>
   <si>
     <t>https://onlinelibrary.wiley.com/doi/abs/10.1002/mrc.4689</t>
+  </si>
+  <si>
+    <t>InSituAnalyze</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/10.1021/acs.analchem.9b03374?goto=supporting-info</t>
+  </si>
+  <si>
+    <t>https://github.com/JiaqiMEI/InSituAnalyze-Python</t>
+  </si>
+  <si>
+    <t>maintainer</t>
+  </si>
+  <si>
+    <t>yangzengling@cau.edu.cn</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>1H NMR metabolomics</t>
+  </si>
+  <si>
+    <t>Spectral processing &amp; modeling</t>
+  </si>
+  <si>
+    <t>Convert nmrML files to ISA-TAB</t>
+  </si>
+  <si>
+    <t>Process &amp; visualize NMR data</t>
+  </si>
+  <si>
+    <t>1D NMR processing for metabolomics</t>
+  </si>
+  <si>
+    <t>Spectral imaging</t>
+  </si>
+  <si>
+    <t>https://github.com/PranaGeo/geoSpectral</t>
+  </si>
+  <si>
+    <t>Storing, manipulation and analysis of spectroscopic data sets</t>
   </si>
 </sst>
 </file>
@@ -1675,12 +1699,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1691,10 +1715,11 @@
     <col min="4" max="4" width="71.5" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
     <col min="6" max="6" width="93.1640625" customWidth="1"/>
-    <col min="7" max="7" width="53.5" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1702,22 +1727,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1733,8 +1761,11 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1751,10 +1782,10 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1774,10 +1805,10 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1794,10 +1825,10 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1811,16 +1842,16 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1836,8 +1867,11 @@
       <c r="F7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1854,10 +1888,10 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1874,10 +1908,10 @@
         <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1894,10 +1928,10 @@
         <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1917,10 +1951,10 @@
         <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1937,10 +1971,10 @@
         <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1957,81 +1991,81 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
+        <v>269</v>
+      </c>
+      <c r="G13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>55</v>
       </c>
-      <c r="G13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>58</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>60</v>
       </c>
-      <c r="G14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="G15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
         <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -2039,828 +2073,872 @@
       <c r="F17" t="s">
         <v>6</v>
       </c>
+      <c r="G17" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
         <v>71</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>75</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>76</v>
-      </c>
-      <c r="D19" t="s">
-        <v>77</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
         <v>79</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>80</v>
-      </c>
-      <c r="C20" t="s">
-        <v>81</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>84</v>
-      </c>
-      <c r="C21" t="s">
-        <v>85</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
         <v>86</v>
-      </c>
-      <c r="B22" t="s">
-        <v>87</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
         <v>89</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>91</v>
-      </c>
-      <c r="D23" t="s">
-        <v>92</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G23" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
         <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>95</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
         <v>97</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>98</v>
-      </c>
-      <c r="D25" t="s">
-        <v>99</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
         <v>123</v>
       </c>
-      <c r="B26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>124</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
+        <v>222</v>
+      </c>
+      <c r="F26" t="s">
         <v>125</v>
       </c>
-      <c r="E26" t="s">
-        <v>227</v>
-      </c>
-      <c r="F26" t="s">
-        <v>126</v>
-      </c>
       <c r="G26" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G27" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
         <v>130</v>
       </c>
-      <c r="B28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
+        <v>222</v>
+      </c>
+      <c r="F28" t="s">
         <v>131</v>
       </c>
-      <c r="E28" t="s">
-        <v>227</v>
-      </c>
-      <c r="F28" t="s">
-        <v>132</v>
+      <c r="G28" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F29" t="s">
-        <v>193</v>
+        <v>268</v>
       </c>
       <c r="G29" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" t="s">
+        <v>222</v>
+      </c>
+      <c r="F31" t="s">
         <v>138</v>
       </c>
-      <c r="B31" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" t="s">
-        <v>143</v>
-      </c>
-      <c r="E31" t="s">
-        <v>227</v>
-      </c>
-      <c r="F31" t="s">
-        <v>139</v>
-      </c>
       <c r="G31" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G32" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
+        <v>222</v>
+      </c>
+      <c r="F33" t="s">
         <v>144</v>
       </c>
-      <c r="B33" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" t="s">
-        <v>227</v>
-      </c>
-      <c r="F33" t="s">
-        <v>145</v>
-      </c>
       <c r="G33" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" t="s">
         <v>149</v>
       </c>
-      <c r="B34" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" t="s">
-        <v>150</v>
-      </c>
       <c r="E34" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G34" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" t="s">
         <v>151</v>
       </c>
-      <c r="D35" t="s">
-        <v>152</v>
-      </c>
       <c r="E35" t="s">
+        <v>222</v>
+      </c>
+      <c r="F35" t="s">
+        <v>182</v>
+      </c>
+      <c r="G35" t="s">
         <v>227</v>
-      </c>
-      <c r="F35" t="s">
-        <v>184</v>
-      </c>
-      <c r="G35" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" t="s">
+        <v>222</v>
+      </c>
+      <c r="F36" t="s">
         <v>154</v>
       </c>
-      <c r="B36" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" t="s">
-        <v>156</v>
-      </c>
-      <c r="E36" t="s">
-        <v>227</v>
-      </c>
-      <c r="F36" t="s">
-        <v>155</v>
-      </c>
       <c r="G36" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" t="s">
+        <v>222</v>
+      </c>
+      <c r="F37" t="s">
         <v>157</v>
       </c>
-      <c r="B37" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" t="s">
-        <v>159</v>
-      </c>
-      <c r="E37" t="s">
-        <v>227</v>
-      </c>
-      <c r="F37" t="s">
-        <v>158</v>
+      <c r="G37" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" t="s">
         <v>160</v>
       </c>
-      <c r="B38" t="s">
-        <v>116</v>
-      </c>
-      <c r="C38" t="s">
-        <v>162</v>
-      </c>
-      <c r="E38" t="s">
-        <v>227</v>
-      </c>
-      <c r="F38" t="s">
-        <v>185</v>
-      </c>
       <c r="G38" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" t="s">
+        <v>222</v>
+      </c>
+      <c r="F39" t="s">
         <v>163</v>
       </c>
-      <c r="B39" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" t="s">
-        <v>165</v>
-      </c>
-      <c r="D39" t="s">
-        <v>166</v>
-      </c>
-      <c r="E39" t="s">
-        <v>227</v>
-      </c>
-      <c r="F39" t="s">
-        <v>164</v>
-      </c>
       <c r="G39" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" t="s">
+        <v>168</v>
+      </c>
+      <c r="E40" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" t="s">
         <v>167</v>
       </c>
-      <c r="B40" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" t="s">
-        <v>227</v>
-      </c>
-      <c r="F40" t="s">
-        <v>168</v>
-      </c>
       <c r="G40" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
         <v>170</v>
       </c>
-      <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" t="s">
-        <v>171</v>
-      </c>
       <c r="E41" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G41" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E42" t="s">
+        <v>222</v>
+      </c>
+      <c r="F42" t="s">
         <v>172</v>
       </c>
-      <c r="E42" t="s">
-        <v>227</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>173</v>
-      </c>
-      <c r="G42" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" t="s">
+        <v>222</v>
+      </c>
+      <c r="F43" t="s">
         <v>176</v>
       </c>
-      <c r="B43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" t="s">
-        <v>178</v>
-      </c>
-      <c r="D43" t="s">
-        <v>179</v>
-      </c>
-      <c r="E43" t="s">
-        <v>227</v>
-      </c>
-      <c r="F43" t="s">
-        <v>177</v>
-      </c>
       <c r="G43" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" t="s">
         <v>180</v>
       </c>
-      <c r="B44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" t="s">
-        <v>181</v>
-      </c>
       <c r="E44" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F44" t="s">
-        <v>182</v>
+        <v>267</v>
       </c>
       <c r="G44" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C45" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E45" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F45" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G45" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C46" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>192</v>
+        <v>266</v>
       </c>
       <c r="G46" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C47" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G47" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B48" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E48" t="s">
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G48" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="G49" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>198</v>
+      </c>
+      <c r="B50" t="s">
+        <v>199</v>
+      </c>
+      <c r="C50" t="s">
+        <v>199</v>
+      </c>
+      <c r="D50" t="s">
+        <v>200</v>
+      </c>
+      <c r="E50" t="s">
+        <v>222</v>
+      </c>
+      <c r="F50" t="s">
+        <v>201</v>
+      </c>
+      <c r="G50" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>202</v>
+      </c>
+      <c r="B51" t="s">
+        <v>203</v>
+      </c>
+      <c r="C51" t="s">
+        <v>205</v>
+      </c>
+      <c r="D51" t="s">
+        <v>204</v>
+      </c>
+      <c r="E51" t="s">
+        <v>207</v>
+      </c>
+      <c r="F51" t="s">
+        <v>206</v>
+      </c>
+      <c r="G51" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>208</v>
+      </c>
+      <c r="B52" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" t="s">
+        <v>211</v>
+      </c>
+      <c r="E52" t="s">
+        <v>210</v>
+      </c>
+      <c r="F52" t="s">
+        <v>229</v>
+      </c>
+      <c r="G52" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" t="s">
+        <v>214</v>
+      </c>
+      <c r="C53" t="s">
+        <v>212</v>
+      </c>
+      <c r="D53" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" t="s">
+        <v>215</v>
+      </c>
+      <c r="F53" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>203</v>
-      </c>
-      <c r="B50" t="s">
-        <v>204</v>
-      </c>
-      <c r="C50" t="s">
-        <v>204</v>
-      </c>
-      <c r="D50" t="s">
-        <v>205</v>
-      </c>
-      <c r="E50" t="s">
-        <v>227</v>
-      </c>
-      <c r="F50" t="s">
-        <v>206</v>
-      </c>
-      <c r="G50" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>207</v>
-      </c>
-      <c r="B51" t="s">
-        <v>208</v>
-      </c>
-      <c r="C51" t="s">
-        <v>210</v>
-      </c>
-      <c r="D51" t="s">
-        <v>209</v>
-      </c>
-      <c r="E51" t="s">
-        <v>212</v>
-      </c>
-      <c r="F51" t="s">
-        <v>211</v>
-      </c>
-      <c r="G51" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>213</v>
-      </c>
-      <c r="B52" t="s">
-        <v>214</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="G53" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>216</v>
       </c>
-      <c r="E52" t="s">
-        <v>215</v>
-      </c>
-      <c r="F52" t="s">
-        <v>234</v>
-      </c>
-      <c r="G52" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B54" t="s">
         <v>218</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C54" t="s">
+        <v>217</v>
+      </c>
+      <c r="E54" t="s">
         <v>219</v>
       </c>
-      <c r="C53" t="s">
-        <v>217</v>
-      </c>
-      <c r="D53" t="s">
-        <v>264</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="F54" t="s">
         <v>220</v>
       </c>
-      <c r="F53" t="s">
-        <v>233</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>221</v>
-      </c>
-      <c r="B54" t="s">
-        <v>223</v>
-      </c>
-      <c r="C54" t="s">
-        <v>222</v>
-      </c>
-      <c r="E54" t="s">
-        <v>224</v>
-      </c>
-      <c r="F54" t="s">
-        <v>225</v>
-      </c>
-      <c r="G54" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>246</v>
-      </c>
       <c r="B55" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C55" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E55" t="s">
         <v>5</v>
       </c>
       <c r="F55" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+      <c r="G55" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B56" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E56" t="s">
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="G56" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B57" t="s">
-        <v>250</v>
+        <v>271</v>
+      </c>
+      <c r="C57" t="s">
+        <v>271</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G57" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B58" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C58" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D58" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E58" t="s">
         <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="G58" t="s">
-        <v>242</v>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>258</v>
+      </c>
+      <c r="B59" t="s">
+        <v>260</v>
+      </c>
+      <c r="C59" t="s">
+        <v>260</v>
+      </c>
+      <c r="D59" t="s">
+        <v>259</v>
+      </c>
+      <c r="E59" t="s">
+        <v>222</v>
+      </c>
+      <c r="F59" t="s">
+        <v>270</v>
+      </c>
+      <c r="G59" t="s">
+        <v>263</v>
+      </c>
+      <c r="H59" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more projects to xlsx
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B6355-B211-5F4A-BAEA-73B242C09004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C347AF-E6F3-B94F-87F0-A2ED527EA9F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24740" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="369">
   <si>
     <t>name</t>
   </si>
@@ -839,6 +839,294 @@
   </si>
   <si>
     <t>Storing, manipulation and analysis of spectroscopic data sets</t>
+  </si>
+  <si>
+    <t>https://github.com/jobovy/apogee</t>
+  </si>
+  <si>
+    <t>https://github.com/qedsoftware/brukeropusreader</t>
+  </si>
+  <si>
+    <t>https://github.com/BIOS-IMASL/cheshift</t>
+  </si>
+  <si>
+    <t>https://github.com/chianti-atomic/ChiantiPy</t>
+  </si>
+  <si>
+    <t>https://github.com/PINT-NMR/COMPASS</t>
+  </si>
+  <si>
+    <t>https://github.com/CCampJr/CRIkit2</t>
+  </si>
+  <si>
+    <t>https://github.com/mretegan/crispy</t>
+  </si>
+  <si>
+    <t>https://github.com/prajwel/curvit</t>
+  </si>
+  <si>
+    <t>https://github.com/Kongsea/DeepSpectroscopy</t>
+  </si>
+  <si>
+    <t>https://github.com/rcthomas/es</t>
+  </si>
+  <si>
+    <t>https://github.com/Farseer-NMR/FarSeer-NMR</t>
+  </si>
+  <si>
+    <t>https://github.com/nasa-jpl/LiveViewOpenSource</t>
+  </si>
+  <si>
+    <t>https://github.com/CMET-UGent/MicroRaman</t>
+  </si>
+  <si>
+    <t>https://github.com/DeepanshS/mrsimulator</t>
+  </si>
+  <si>
+    <t>https://github.com/pnnl/nmrfit</t>
+  </si>
+  <si>
+    <t>https://github.com/nsherry4/Peakaboo</t>
+  </si>
+  <si>
+    <t>https://github.com/TheAstroFactory/pydis</t>
+  </si>
+  <si>
+    <t>https://github.com/sametz/pydnmr</t>
+  </si>
+  <si>
+    <t>https://github.com/L-Siemons/PyRoShift</t>
+  </si>
+  <si>
+    <t>https://github.com/ibcp/pyspectra</t>
+  </si>
+  <si>
+    <t>https://github.com/pycroscopy/pyUSID</t>
+  </si>
+  <si>
+    <t>https://github.com/radis/radis</t>
+  </si>
+  <si>
+    <t>https://github.com/DerekKaknes/raman</t>
+  </si>
+  <si>
+    <t>https://github.com/raman-noodles/Raman-noodles</t>
+  </si>
+  <si>
+    <t>https://github.com/charlesll/rampy</t>
+  </si>
+  <si>
+    <t>https://github.com/LlucSF/rCRSI</t>
+  </si>
+  <si>
+    <t>https://github.com/paris-saclay-cds/specio</t>
+  </si>
+  <si>
+    <t>https://github.com/astropy/specreduce</t>
+  </si>
+  <si>
+    <t>https://github.com/cheminfo-js/spectra-data</t>
+  </si>
+  <si>
+    <t>https://github.com/clerk67/spectra-formatter</t>
+  </si>
+  <si>
+    <t>https://github.com/charlesll/Spectra.jl</t>
+  </si>
+  <si>
+    <t>https://github.com/PlasmaPy/SpectroscoPyx</t>
+  </si>
+  <si>
+    <t>https://github.com/spacetelescope/specviz</t>
+  </si>
+  <si>
+    <t>https://github.com/workflow4metabolomics/tools-metabolomics</t>
+  </si>
+  <si>
+    <t>https://github.com/VespucciProject/Vespucci</t>
+  </si>
+  <si>
+    <t>https://github.com/archaeological-research-facility/web_geochemistry</t>
+  </si>
+  <si>
+    <t>https://github.com/megbedell/wobble</t>
+  </si>
+  <si>
+    <t>https://github.com/workflow4metabolomics/workflow4metabolomics</t>
+  </si>
+  <si>
+    <t>https://github.com/wcchu/XL-e</t>
+  </si>
+  <si>
+    <t>https://github.com/brianlevay/xrf_filetools</t>
+  </si>
+  <si>
+    <t>https://github.com/dylarm/xrf_parser</t>
+  </si>
+  <si>
+    <t>https://github.com/wojdyr/xylib</t>
+  </si>
+  <si>
+    <t>https://github.com/yokochi47/xyza2pipe</t>
+  </si>
+  <si>
+    <t>Tools for working with APOGEE data</t>
+  </si>
+  <si>
+    <t>bovy at astro dot utoronto dot ca</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1510.06745</t>
+  </si>
+  <si>
+    <t>apogee</t>
+  </si>
+  <si>
+    <t>brukeropusreader</t>
+  </si>
+  <si>
+    <t>Read Bruker OPUS files</t>
+  </si>
+  <si>
+    <t>Data Sharing</t>
+  </si>
+  <si>
+    <t>brukeropusreader-dev@qed.ai</t>
+  </si>
+  <si>
+    <t>CheShift</t>
+  </si>
+  <si>
+    <t>Prediction 13C shifts in proteins</t>
+  </si>
+  <si>
+    <t>https://www.pnas.org/content/110/42/16826</t>
+  </si>
+  <si>
+    <t>Calculate radiative properties of astrophysical plasmas</t>
+  </si>
+  <si>
+    <t>ChiantiPy</t>
+  </si>
+  <si>
+    <t>Protein backbone assignments from triple-resonance peak lists</t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1004022</t>
+  </si>
+  <si>
+    <t>COMPASS</t>
+  </si>
+  <si>
+    <t>charles.camp@nist.gov</t>
+  </si>
+  <si>
+    <t>Hyperspectral imaging toolkit</t>
+  </si>
+  <si>
+    <t>CRIkit2</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/28819335</t>
+  </si>
+  <si>
+    <t>Calculate &amp; plot core-level spectra</t>
+  </si>
+  <si>
+    <t>http://www.esrf.eu/computing/scientific/crispy/</t>
+  </si>
+  <si>
+    <t>crispy</t>
+  </si>
+  <si>
+    <t>Create light curves from UV imaging telescope data</t>
+  </si>
+  <si>
+    <t>UV</t>
+  </si>
+  <si>
+    <t>curvit</t>
+  </si>
+  <si>
+    <t>DeepSpectroscopy</t>
+  </si>
+  <si>
+    <t>Spectroscopy with deep learning</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>Elementary supernova spectrum synthesis</t>
+  </si>
+  <si>
+    <t>https://c3.lbl.gov/es/</t>
+  </si>
+  <si>
+    <t>Analysis &amp; plotting of biological NMR peak lists</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10858-018-0182-5</t>
+  </si>
+  <si>
+    <t>Farseer-NMR</t>
+  </si>
+  <si>
+    <t>https://farseer-nmr.github.io/FarSeer-NMR/</t>
+  </si>
+  <si>
+    <t>Tools for imaging spectrometer development</t>
+  </si>
+  <si>
+    <t>Jacqueline.Ryan@jpl.nasa.gov</t>
+  </si>
+  <si>
+    <t>UV-VIS-IR</t>
+  </si>
+  <si>
+    <t>UV-Vis-IR</t>
+  </si>
+  <si>
+    <t>LiveView</t>
+  </si>
+  <si>
+    <t>MicroRaman</t>
+  </si>
+  <si>
+    <t>Process microbial Raman spectra</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/29909167</t>
+  </si>
+  <si>
+    <t>mrsimulator</t>
+  </si>
+  <si>
+    <t>Toolbox for simulating NMR spectra</t>
+  </si>
+  <si>
+    <t>https://deepanshs.github.io/mrsimulator/</t>
+  </si>
+  <si>
+    <t>frederiekmaarten.kerckhof@ugent.be</t>
+  </si>
+  <si>
+    <t>nmrfit</t>
+  </si>
+  <si>
+    <t>qNMR through least-squares fitting</t>
+  </si>
+  <si>
+    <t>XRF analysis</t>
+  </si>
+  <si>
+    <t>XRF</t>
+  </si>
+  <si>
+    <t>https://peakaboo.org/</t>
+  </si>
+  <si>
+    <t>Peakaboo</t>
   </si>
 </sst>
 </file>
@@ -1699,12 +1987,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1714,7 +2002,7 @@
     <col min="3" max="3" width="62.5" customWidth="1"/>
     <col min="4" max="4" width="71.5" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="93.1640625" customWidth="1"/>
+    <col min="6" max="6" width="78.83203125" customWidth="1"/>
     <col min="7" max="7" width="22.1640625" customWidth="1"/>
     <col min="8" max="8" width="26.1640625" customWidth="1"/>
   </cols>
@@ -2941,6 +3229,488 @@
         <v>262</v>
       </c>
     </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>319</v>
+      </c>
+      <c r="B60" t="s">
+        <v>273</v>
+      </c>
+      <c r="C60" t="s">
+        <v>273</v>
+      </c>
+      <c r="D60" t="s">
+        <v>318</v>
+      </c>
+      <c r="E60" t="s">
+        <v>222</v>
+      </c>
+      <c r="F60" t="s">
+        <v>316</v>
+      </c>
+      <c r="G60" t="s">
+        <v>263</v>
+      </c>
+      <c r="H60" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>320</v>
+      </c>
+      <c r="B61" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" t="s">
+        <v>274</v>
+      </c>
+      <c r="E61" t="s">
+        <v>222</v>
+      </c>
+      <c r="F61" t="s">
+        <v>321</v>
+      </c>
+      <c r="G61" t="s">
+        <v>322</v>
+      </c>
+      <c r="H61" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>324</v>
+      </c>
+      <c r="B62" t="s">
+        <v>275</v>
+      </c>
+      <c r="C62" t="s">
+        <v>275</v>
+      </c>
+      <c r="D62" t="s">
+        <v>326</v>
+      </c>
+      <c r="E62" t="s">
+        <v>222</v>
+      </c>
+      <c r="F62" t="s">
+        <v>325</v>
+      </c>
+      <c r="G62" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>328</v>
+      </c>
+      <c r="B63" t="s">
+        <v>276</v>
+      </c>
+      <c r="C63" t="s">
+        <v>276</v>
+      </c>
+      <c r="E63" t="s">
+        <v>222</v>
+      </c>
+      <c r="F63" t="s">
+        <v>327</v>
+      </c>
+      <c r="G63" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>331</v>
+      </c>
+      <c r="B64" t="s">
+        <v>277</v>
+      </c>
+      <c r="C64" t="s">
+        <v>277</v>
+      </c>
+      <c r="D64" t="s">
+        <v>330</v>
+      </c>
+      <c r="E64" t="s">
+        <v>207</v>
+      </c>
+      <c r="F64" t="s">
+        <v>329</v>
+      </c>
+      <c r="G64" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>334</v>
+      </c>
+      <c r="B65" t="s">
+        <v>278</v>
+      </c>
+      <c r="C65" t="s">
+        <v>278</v>
+      </c>
+      <c r="D65" t="s">
+        <v>335</v>
+      </c>
+      <c r="E65" t="s">
+        <v>222</v>
+      </c>
+      <c r="F65" t="s">
+        <v>333</v>
+      </c>
+      <c r="G65" t="s">
+        <v>233</v>
+      </c>
+      <c r="H65" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>338</v>
+      </c>
+      <c r="B66" t="s">
+        <v>337</v>
+      </c>
+      <c r="C66" t="s">
+        <v>279</v>
+      </c>
+      <c r="E66" t="s">
+        <v>222</v>
+      </c>
+      <c r="F66" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>341</v>
+      </c>
+      <c r="B67" t="s">
+        <v>280</v>
+      </c>
+      <c r="C67" t="s">
+        <v>280</v>
+      </c>
+      <c r="E67" t="s">
+        <v>222</v>
+      </c>
+      <c r="F67" t="s">
+        <v>339</v>
+      </c>
+      <c r="G67" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>342</v>
+      </c>
+      <c r="B68" t="s">
+        <v>281</v>
+      </c>
+      <c r="C68" t="s">
+        <v>281</v>
+      </c>
+      <c r="E68" t="s">
+        <v>222</v>
+      </c>
+      <c r="F68" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>344</v>
+      </c>
+      <c r="B69" t="s">
+        <v>346</v>
+      </c>
+      <c r="C69" t="s">
+        <v>282</v>
+      </c>
+      <c r="E69" t="s">
+        <v>222</v>
+      </c>
+      <c r="F69" t="s">
+        <v>345</v>
+      </c>
+      <c r="G69" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>349</v>
+      </c>
+      <c r="B70" t="s">
+        <v>350</v>
+      </c>
+      <c r="C70" t="s">
+        <v>283</v>
+      </c>
+      <c r="D70" t="s">
+        <v>348</v>
+      </c>
+      <c r="E70" t="s">
+        <v>222</v>
+      </c>
+      <c r="F70" t="s">
+        <v>347</v>
+      </c>
+      <c r="G70" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>355</v>
+      </c>
+      <c r="B71" t="s">
+        <v>284</v>
+      </c>
+      <c r="C71" t="s">
+        <v>284</v>
+      </c>
+      <c r="E71" t="s">
+        <v>215</v>
+      </c>
+      <c r="F71" t="s">
+        <v>351</v>
+      </c>
+      <c r="G71" t="s">
+        <v>353</v>
+      </c>
+      <c r="H71" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>356</v>
+      </c>
+      <c r="B72" t="s">
+        <v>358</v>
+      </c>
+      <c r="C72" t="s">
+        <v>285</v>
+      </c>
+      <c r="D72" t="s">
+        <v>358</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>357</v>
+      </c>
+      <c r="G72" t="s">
+        <v>233</v>
+      </c>
+      <c r="H72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>359</v>
+      </c>
+      <c r="B73" t="s">
+        <v>361</v>
+      </c>
+      <c r="C73" t="s">
+        <v>286</v>
+      </c>
+      <c r="E73" t="s">
+        <v>222</v>
+      </c>
+      <c r="F73" t="s">
+        <v>360</v>
+      </c>
+      <c r="G73" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>363</v>
+      </c>
+      <c r="B74" t="s">
+        <v>287</v>
+      </c>
+      <c r="C74" t="s">
+        <v>287</v>
+      </c>
+      <c r="E74" t="s">
+        <v>222</v>
+      </c>
+      <c r="F74" t="s">
+        <v>364</v>
+      </c>
+      <c r="G74" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>368</v>
+      </c>
+      <c r="B75" t="s">
+        <v>367</v>
+      </c>
+      <c r="C75" t="s">
+        <v>288</v>
+      </c>
+      <c r="E75" t="s">
+        <v>210</v>
+      </c>
+      <c r="F75" t="s">
+        <v>365</v>
+      </c>
+      <c r="G75" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
+        <v>315</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1" display="https://cran.r-project.org/package=pavo" xr:uid="{3E292708-18D0-1C48-B810-34D638D0D26E}"/>

</xml_diff>

<commit_message>
more project entries + Table1.png
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C347AF-E6F3-B94F-87F0-A2ED527EA9F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5367018F-94C7-CB45-8768-D1DA715787E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24740" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="437">
   <si>
     <t>name</t>
   </si>
@@ -130,9 +130,6 @@
     <t>https://github.com/Chathurga/HyperChemoBridge</t>
   </si>
   <si>
-    <t>Interconversion of hyperSpec and ChemoSpec formats</t>
-  </si>
-  <si>
     <t>nmrPipe</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>https://github.com/antoinestevens/prospectr</t>
   </si>
   <si>
-    <t>Vis and NIR</t>
-  </si>
-  <si>
     <t>resemble</t>
   </si>
   <si>
@@ -625,9 +619,6 @@
     <t>https://doi.org/10.1016/j.jmr.2019.02.006</t>
   </si>
   <si>
-    <t>SS NMR processing and fitting</t>
-  </si>
-  <si>
     <t>PINT</t>
   </si>
   <si>
@@ -688,9 +679,6 @@
     <t>focus</t>
   </si>
   <si>
-    <t>Py</t>
-  </si>
-  <si>
     <t>NMR (1D)</t>
   </si>
   <si>
@@ -730,9 +718,6 @@
     <t>NMR (Bruker)</t>
   </si>
   <si>
-    <t>Perceptual analysis, visualization and organization of spectral color data (incl images)</t>
-  </si>
-  <si>
     <t>UV-Vis</t>
   </si>
   <si>
@@ -838,9 +823,6 @@
     <t>https://github.com/PranaGeo/geoSpectral</t>
   </si>
   <si>
-    <t>Storing, manipulation and analysis of spectroscopic data sets</t>
-  </si>
-  <si>
     <t>https://github.com/jobovy/apogee</t>
   </si>
   <si>
@@ -889,9 +871,6 @@
     <t>https://github.com/nsherry4/Peakaboo</t>
   </si>
   <si>
-    <t>https://github.com/TheAstroFactory/pydis</t>
-  </si>
-  <si>
     <t>https://github.com/sametz/pydnmr</t>
   </si>
   <si>
@@ -907,27 +886,15 @@
     <t>https://github.com/radis/radis</t>
   </si>
   <si>
-    <t>https://github.com/DerekKaknes/raman</t>
-  </si>
-  <si>
-    <t>https://github.com/raman-noodles/Raman-noodles</t>
-  </si>
-  <si>
     <t>https://github.com/charlesll/rampy</t>
   </si>
   <si>
     <t>https://github.com/LlucSF/rCRSI</t>
   </si>
   <si>
-    <t>https://github.com/paris-saclay-cds/specio</t>
-  </si>
-  <si>
     <t>https://github.com/astropy/specreduce</t>
   </si>
   <si>
-    <t>https://github.com/cheminfo-js/spectra-data</t>
-  </si>
-  <si>
     <t>https://github.com/clerk67/spectra-formatter</t>
   </si>
   <si>
@@ -940,9 +907,6 @@
     <t>https://github.com/spacetelescope/specviz</t>
   </si>
   <si>
-    <t>https://github.com/workflow4metabolomics/tools-metabolomics</t>
-  </si>
-  <si>
     <t>https://github.com/VespucciProject/Vespucci</t>
   </si>
   <si>
@@ -952,9 +916,6 @@
     <t>https://github.com/megbedell/wobble</t>
   </si>
   <si>
-    <t>https://github.com/workflow4metabolomics/workflow4metabolomics</t>
-  </si>
-  <si>
     <t>https://github.com/wcchu/XL-e</t>
   </si>
   <si>
@@ -964,9 +925,6 @@
     <t>https://github.com/dylarm/xrf_parser</t>
   </si>
   <si>
-    <t>https://github.com/wojdyr/xylib</t>
-  </si>
-  <si>
     <t>https://github.com/yokochi47/xyza2pipe</t>
   </si>
   <si>
@@ -1075,9 +1033,6 @@
     <t>https://farseer-nmr.github.io/FarSeer-NMR/</t>
   </si>
   <si>
-    <t>Tools for imaging spectrometer development</t>
-  </si>
-  <si>
     <t>Jacqueline.Ryan@jpl.nasa.gov</t>
   </si>
   <si>
@@ -1127,6 +1082,255 @@
   </si>
   <si>
     <t>Peakaboo</t>
+  </si>
+  <si>
+    <t>pydnmr</t>
+  </si>
+  <si>
+    <t>Simulation dynamic NMR</t>
+  </si>
+  <si>
+    <t>PyRoShift</t>
+  </si>
+  <si>
+    <t>https://pubs.rsc.org/en/Content/ArticleLanding/2019/CC/C9CC06496F#!divAbstract</t>
+  </si>
+  <si>
+    <t>Compute rotamer populations from 13C NMR shifts</t>
+  </si>
+  <si>
+    <t>lucas.siemons@googlemail.com</t>
+  </si>
+  <si>
+    <t>glvrst@gmail.com</t>
+  </si>
+  <si>
+    <t>General purpose?</t>
+  </si>
+  <si>
+    <t>pyspectra</t>
+  </si>
+  <si>
+    <t>https://pycroscopy.github.io/pyUSID/about.html</t>
+  </si>
+  <si>
+    <t>pyUSID</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1903.09515</t>
+  </si>
+  <si>
+    <t>Universal spectroscopy &amp; imaging data format</t>
+  </si>
+  <si>
+    <t>https://pycroscopy.github.io/pycroscopy/about.html</t>
+  </si>
+  <si>
+    <t>pycroscopy</t>
+  </si>
+  <si>
+    <t>https://github.com/pycroscopy/pycroscopy</t>
+  </si>
+  <si>
+    <t>Imaging microscopy</t>
+  </si>
+  <si>
+    <t>sjesse@ornl.gov</t>
+  </si>
+  <si>
+    <t>RADIS</t>
+  </si>
+  <si>
+    <t>Compute IR spectra</t>
+  </si>
+  <si>
+    <t>https://radis.readthedocs.io/en/latest/</t>
+  </si>
+  <si>
+    <t>RamPy</t>
+  </si>
+  <si>
+    <t>lelosq@ipgp.fr</t>
+  </si>
+  <si>
+    <t>Processing Raman, IR, XAS spectra</t>
+  </si>
+  <si>
+    <t>rCSRI</t>
+  </si>
+  <si>
+    <t>Tools for confocal Raman imaging spectroscopy</t>
+  </si>
+  <si>
+    <t>lluc.semente@urv.cat</t>
+  </si>
+  <si>
+    <t>Reduce &amp; calibrate spectroscopic data</t>
+  </si>
+  <si>
+    <t>specreduce</t>
+  </si>
+  <si>
+    <t>https://github.com/cheminfo-js/spectra</t>
+  </si>
+  <si>
+    <t>spectra</t>
+  </si>
+  <si>
+    <t>https://cheminfo-js.github.io/spectra/packages/spectra-data/docs/</t>
+  </si>
+  <si>
+    <t>Library for UV, IR, 1D &amp; 2D NMR</t>
+  </si>
+  <si>
+    <t>spectra-formatter</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>Tool to write out NMR data for publication summaries</t>
+  </si>
+  <si>
+    <t>https://clerk67.github.io/spectra-formatter/</t>
+  </si>
+  <si>
+    <t>Spectra</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Treatment of spectra (Raman, infrared, XAS, NMR) data</t>
+  </si>
+  <si>
+    <t>charles.lelosq@anu.edu.au</t>
+  </si>
+  <si>
+    <t>SpectroscoPyx</t>
+  </si>
+  <si>
+    <t>https://spectroscopyx.readthedocs.io/en/latest/</t>
+  </si>
+  <si>
+    <t>Atomic/Plasma spectroscopy</t>
+  </si>
+  <si>
+    <t>https://specviz.readthedocs.io/en/stable/</t>
+  </si>
+  <si>
+    <t>SpecViz</t>
+  </si>
+  <si>
+    <t>Interactive analysis of 1D astronomical spectra</t>
+  </si>
+  <si>
+    <t>https://specutils.readthedocs.io/en/stable/</t>
+  </si>
+  <si>
+    <t>specutils</t>
+  </si>
+  <si>
+    <t>Toolbox for astronomical spectroscopic data</t>
+  </si>
+  <si>
+    <t>https://github.com/astropy/specutils</t>
+  </si>
+  <si>
+    <t>contact@nicholasearl.me</t>
+  </si>
+  <si>
+    <t>Tools for spectroscopic data analysis &amp; imaging</t>
+  </si>
+  <si>
+    <t>https://openresearchsoftware.metajnl.com/articles/10.5334/jors.91/</t>
+  </si>
+  <si>
+    <t>Vespucci</t>
+  </si>
+  <si>
+    <t>Shiny app for visualizing XRF &amp; NAA geochemistry concentrations</t>
+  </si>
+  <si>
+    <t>https://arfberkeley.shinyapps.io/web_geochemistry/</t>
+  </si>
+  <si>
+    <t>web_geochemistry</t>
+  </si>
+  <si>
+    <t>wobble</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1901.00503</t>
+  </si>
+  <si>
+    <t>Analysis of stellar spectra time series</t>
+  </si>
+  <si>
+    <t>https://wobble.readthedocs.io/en/latest/</t>
+  </si>
+  <si>
+    <t>Fortran</t>
+  </si>
+  <si>
+    <t>https://journals.aps.org/pra/abstract/10.1103/PhysRevA.89.033427</t>
+  </si>
+  <si>
+    <t>Simulate photoelectron spectra driven by laser pulses</t>
+  </si>
+  <si>
+    <t>PES</t>
+  </si>
+  <si>
+    <t>XL-e</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>XRF file tools</t>
+  </si>
+  <si>
+    <t>xrf_filetools</t>
+  </si>
+  <si>
+    <t>xrf_parsers</t>
+  </si>
+  <si>
+    <t>Parse files from handheld XRF spectrometers</t>
+  </si>
+  <si>
+    <t>File conversion for NMR data formats</t>
+  </si>
+  <si>
+    <t>xyza2pipe</t>
+  </si>
+  <si>
+    <t>Interconversion of hyperSpec &amp; ChemoSpec formats</t>
+  </si>
+  <si>
+    <t>Vis &amp; NIR</t>
+  </si>
+  <si>
+    <t>Perceptual analysis, visualization &amp; organization of spectral color data (incl images)</t>
+  </si>
+  <si>
+    <t>SS NMR processing &amp; fitting</t>
+  </si>
+  <si>
+    <t>Storing, manipulation &amp; analysis of spectroscopic data sets</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Data Sharing (IR)</t>
+  </si>
+  <si>
+    <t>XAS</t>
+  </si>
+  <si>
+    <t>Data sharing (NMR nD)</t>
   </si>
 </sst>
 </file>
@@ -1987,12 +2191,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2015,22 +2219,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2050,7 +2254,7 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2070,7 +2274,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2093,7 +2297,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2113,7 +2317,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2130,13 +2334,13 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2156,7 +2360,7 @@
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2176,7 +2380,7 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2193,167 +2397,167 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>428</v>
       </c>
       <c r="G9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
       </c>
       <c r="F10" t="s">
         <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>45</v>
       </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
       <c r="G11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="G13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>61</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>429</v>
       </c>
       <c r="G15" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
         <v>64</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -2362,1353 +2566,1700 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" t="s">
-        <v>76</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
         <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" t="s">
-        <v>80</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
         <v>82</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>84</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>89</v>
-      </c>
-      <c r="C23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" t="s">
-        <v>91</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G24" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
         <v>96</v>
-      </c>
-      <c r="B25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" t="s">
-        <v>98</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G25" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" t="s">
         <v>122</v>
       </c>
-      <c r="B26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
+        <v>433</v>
+      </c>
+      <c r="F26" t="s">
         <v>123</v>
       </c>
-      <c r="D26" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" t="s">
-        <v>222</v>
-      </c>
-      <c r="F26" t="s">
-        <v>125</v>
-      </c>
       <c r="G26" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" t="s">
+        <v>433</v>
+      </c>
+      <c r="F28" t="s">
         <v>129</v>
       </c>
-      <c r="B28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" t="s">
-        <v>222</v>
-      </c>
-      <c r="F28" t="s">
-        <v>131</v>
-      </c>
       <c r="G28" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F29" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G29" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E30" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F30" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="G30" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E31" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G31" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E32" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G32" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" t="s">
         <v>143</v>
       </c>
-      <c r="B33" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" t="s">
-        <v>145</v>
-      </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E33" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G33" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G34" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E35" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F35" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G35" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" t="s">
         <v>153</v>
       </c>
-      <c r="B36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" t="s">
-        <v>155</v>
-      </c>
       <c r="E36" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G36" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
         <v>156</v>
       </c>
-      <c r="B37" t="s">
-        <v>114</v>
-      </c>
-      <c r="C37" t="s">
-        <v>158</v>
-      </c>
       <c r="E37" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G37" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
         <v>159</v>
       </c>
-      <c r="B38" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" t="s">
-        <v>161</v>
-      </c>
       <c r="E38" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G38" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
         <v>162</v>
       </c>
-      <c r="B39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" t="s">
-        <v>164</v>
-      </c>
       <c r="D39" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E39" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G39" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" t="s">
         <v>166</v>
       </c>
-      <c r="B40" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" t="s">
-        <v>168</v>
-      </c>
       <c r="E40" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G40" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E41" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G41" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" t="s">
+        <v>433</v>
+      </c>
+      <c r="F42" t="s">
+        <v>170</v>
+      </c>
+      <c r="G42" t="s">
         <v>171</v>
-      </c>
-      <c r="E42" t="s">
-        <v>222</v>
-      </c>
-      <c r="F42" t="s">
-        <v>172</v>
-      </c>
-      <c r="G42" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" t="s">
         <v>175</v>
       </c>
-      <c r="B43" t="s">
-        <v>120</v>
-      </c>
-      <c r="C43" t="s">
-        <v>177</v>
-      </c>
       <c r="D43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E43" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G43" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E44" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F44" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G44" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E45" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F45" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G45" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" t="s">
         <v>185</v>
       </c>
-      <c r="B46" t="s">
-        <v>187</v>
-      </c>
       <c r="C46" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G46" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>187</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" t="s">
         <v>189</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C47" t="s">
-        <v>191</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>236</v>
+        <v>430</v>
       </c>
       <c r="G47" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" t="s">
         <v>192</v>
-      </c>
-      <c r="B48" t="s">
-        <v>193</v>
-      </c>
-      <c r="C48" t="s">
-        <v>194</v>
       </c>
       <c r="E48" t="s">
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G48" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B49" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C49" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G49" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>196</v>
+      </c>
+      <c r="B50" t="s">
+        <v>197</v>
+      </c>
+      <c r="C50" t="s">
+        <v>197</v>
+      </c>
+      <c r="D50" t="s">
         <v>198</v>
       </c>
-      <c r="B50" t="s">
-        <v>199</v>
-      </c>
-      <c r="C50" t="s">
-        <v>199</v>
-      </c>
-      <c r="D50" t="s">
-        <v>200</v>
-      </c>
       <c r="E50" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F50" t="s">
-        <v>201</v>
+        <v>431</v>
       </c>
       <c r="G50" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>199</v>
+      </c>
+      <c r="B51" t="s">
+        <v>200</v>
+      </c>
+      <c r="C51" t="s">
         <v>202</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
+        <v>201</v>
+      </c>
+      <c r="E51" t="s">
+        <v>204</v>
+      </c>
+      <c r="F51" t="s">
         <v>203</v>
       </c>
-      <c r="C51" t="s">
-        <v>205</v>
-      </c>
-      <c r="D51" t="s">
-        <v>204</v>
-      </c>
-      <c r="E51" t="s">
-        <v>207</v>
-      </c>
-      <c r="F51" t="s">
-        <v>206</v>
-      </c>
       <c r="G51" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" t="s">
         <v>208</v>
       </c>
-      <c r="B52" t="s">
-        <v>209</v>
-      </c>
-      <c r="C52" t="s">
-        <v>211</v>
-      </c>
       <c r="E52" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F52" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G52" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B53" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C53" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" t="s">
+        <v>252</v>
+      </c>
+      <c r="E53" t="s">
         <v>212</v>
       </c>
-      <c r="D53" t="s">
-        <v>257</v>
-      </c>
-      <c r="E53" t="s">
-        <v>215</v>
-      </c>
       <c r="F53" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G53" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" t="s">
+        <v>215</v>
+      </c>
+      <c r="C54" t="s">
+        <v>214</v>
+      </c>
+      <c r="E54" t="s">
         <v>216</v>
       </c>
-      <c r="B54" t="s">
-        <v>218</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="F54" t="s">
         <v>217</v>
       </c>
-      <c r="E54" t="s">
-        <v>219</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>220</v>
-      </c>
-      <c r="G54" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B55" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C55" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E55" t="s">
         <v>5</v>
       </c>
       <c r="F55" t="s">
-        <v>272</v>
+        <v>432</v>
       </c>
       <c r="G55" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B56" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E56" t="s">
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G56" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B57" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C57" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G57" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B58" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C58" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D58" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E58" t="s">
         <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G58" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>253</v>
+      </c>
+      <c r="B59" t="s">
+        <v>255</v>
+      </c>
+      <c r="C59" t="s">
+        <v>255</v>
+      </c>
+      <c r="D59" t="s">
+        <v>254</v>
+      </c>
+      <c r="E59" t="s">
+        <v>433</v>
+      </c>
+      <c r="F59" t="s">
+        <v>265</v>
+      </c>
+      <c r="G59" t="s">
         <v>258</v>
       </c>
-      <c r="B59" t="s">
-        <v>260</v>
-      </c>
-      <c r="C59" t="s">
-        <v>260</v>
-      </c>
-      <c r="D59" t="s">
-        <v>259</v>
-      </c>
-      <c r="E59" t="s">
-        <v>222</v>
-      </c>
-      <c r="F59" t="s">
-        <v>270</v>
-      </c>
-      <c r="G59" t="s">
-        <v>263</v>
-      </c>
       <c r="H59" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="B60" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C60" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D60" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="E60" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F60" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="G60" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H60" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="B61" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C61" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E61" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F61" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="G61" t="s">
-        <v>322</v>
+        <v>434</v>
       </c>
       <c r="H61" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="B62" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C62" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D62" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="E62" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F62" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="G62" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="B63" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C63" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E63" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F63" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="G63" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="B64" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C64" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D64" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="E64" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F64" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="G64" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B65" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C65" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D65" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E65" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F65" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="G65" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H65" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="B66" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="C66" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E66" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F66" t="s">
-        <v>336</v>
+        <v>322</v>
+      </c>
+      <c r="G66" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="B67" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C67" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E67" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F67" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="G67" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="B68" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C68" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E68" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F68" t="s">
-        <v>343</v>
+        <v>329</v>
+      </c>
+      <c r="G68" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B69" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="C69" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E69" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F69" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="G69" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B70" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="C70" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D70" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="E70" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F70" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="G70" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="B71" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C71" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E71" t="s">
-        <v>215</v>
-      </c>
-      <c r="F71" t="s">
-        <v>351</v>
+        <v>212</v>
       </c>
       <c r="G71" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="H71" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B72" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C72" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D72" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
       </c>
       <c r="F72" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="G72" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H72" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="B73" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="C73" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E73" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F73" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="G73" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="B74" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C74" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E74" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="F74" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="G74" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>353</v>
+      </c>
+      <c r="B75" t="s">
+        <v>352</v>
+      </c>
+      <c r="C75" t="s">
+        <v>282</v>
+      </c>
+      <c r="E75" t="s">
+        <v>207</v>
+      </c>
+      <c r="F75" t="s">
+        <v>350</v>
+      </c>
+      <c r="G75" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>354</v>
+      </c>
+      <c r="B76" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" t="s">
+        <v>283</v>
+      </c>
+      <c r="E76" t="s">
+        <v>433</v>
+      </c>
+      <c r="F76" t="s">
+        <v>355</v>
+      </c>
+      <c r="G76" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>356</v>
+      </c>
+      <c r="B77" t="s">
+        <v>284</v>
+      </c>
+      <c r="C77" t="s">
+        <v>284</v>
+      </c>
+      <c r="D77" t="s">
+        <v>357</v>
+      </c>
+      <c r="E77" t="s">
+        <v>433</v>
+      </c>
+      <c r="F77" t="s">
+        <v>358</v>
+      </c>
+      <c r="G77" t="s">
+        <v>228</v>
+      </c>
+      <c r="H77" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>362</v>
+      </c>
+      <c r="B78" t="s">
+        <v>285</v>
+      </c>
+      <c r="C78" t="s">
+        <v>285</v>
+      </c>
+      <c r="E78" t="s">
+        <v>433</v>
+      </c>
+      <c r="F78" t="s">
+        <v>361</v>
+      </c>
+      <c r="G78" t="s">
+        <v>259</v>
+      </c>
+      <c r="H78" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>364</v>
+      </c>
+      <c r="B79" t="s">
+        <v>363</v>
+      </c>
+      <c r="C79" t="s">
+        <v>286</v>
+      </c>
+      <c r="D79" t="s">
+        <v>365</v>
+      </c>
+      <c r="E79" t="s">
+        <v>433</v>
+      </c>
+      <c r="F79" t="s">
+        <v>366</v>
+      </c>
+      <c r="G79" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>368</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B80" t="s">
         <v>367</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C80" t="s">
+        <v>369</v>
+      </c>
+      <c r="E80" t="s">
+        <v>433</v>
+      </c>
+      <c r="F80" t="s">
+        <v>370</v>
+      </c>
+      <c r="G80" t="s">
+        <v>229</v>
+      </c>
+      <c r="H80" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>372</v>
+      </c>
+      <c r="B81" t="s">
+        <v>374</v>
+      </c>
+      <c r="C81" t="s">
+        <v>287</v>
+      </c>
+      <c r="E81" t="s">
+        <v>433</v>
+      </c>
+      <c r="F81" t="s">
+        <v>373</v>
+      </c>
+      <c r="G81" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>375</v>
+      </c>
+      <c r="B82" t="s">
         <v>288</v>
       </c>
-      <c r="E75" t="s">
-        <v>210</v>
-      </c>
-      <c r="F75" t="s">
-        <v>365</v>
-      </c>
-      <c r="G75" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C76" t="s">
+      <c r="C82" t="s">
+        <v>288</v>
+      </c>
+      <c r="E82" t="s">
+        <v>433</v>
+      </c>
+      <c r="F82" t="s">
+        <v>377</v>
+      </c>
+      <c r="G82" t="s">
+        <v>229</v>
+      </c>
+      <c r="H82" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>378</v>
+      </c>
+      <c r="B83" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C77" t="s">
+      <c r="C83" t="s">
+        <v>289</v>
+      </c>
+      <c r="E83" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" t="s">
+        <v>379</v>
+      </c>
+      <c r="G83" t="s">
+        <v>229</v>
+      </c>
+      <c r="H83" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>382</v>
+      </c>
+      <c r="B84" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C78" t="s">
+      <c r="C84" t="s">
+        <v>290</v>
+      </c>
+      <c r="E84" t="s">
+        <v>433</v>
+      </c>
+      <c r="F84" t="s">
+        <v>381</v>
+      </c>
+      <c r="G84" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>384</v>
+      </c>
+      <c r="B85" t="s">
+        <v>385</v>
+      </c>
+      <c r="C85" t="s">
+        <v>383</v>
+      </c>
+      <c r="E85" t="s">
+        <v>433</v>
+      </c>
+      <c r="F85" t="s">
+        <v>386</v>
+      </c>
+      <c r="G85" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>387</v>
+      </c>
+      <c r="B86" t="s">
+        <v>390</v>
+      </c>
+      <c r="C86" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
+      <c r="E86" t="s">
+        <v>388</v>
+      </c>
+      <c r="F86" t="s">
+        <v>389</v>
+      </c>
+      <c r="G86" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>391</v>
+      </c>
+      <c r="B87" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C80" t="s">
+      <c r="C87" t="s">
+        <v>292</v>
+      </c>
+      <c r="E87" t="s">
+        <v>392</v>
+      </c>
+      <c r="F87" t="s">
+        <v>393</v>
+      </c>
+      <c r="G87" t="s">
+        <v>259</v>
+      </c>
+      <c r="H87" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>395</v>
+      </c>
+      <c r="B88" t="s">
+        <v>396</v>
+      </c>
+      <c r="C88" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" t="s">
+      <c r="E88" t="s">
+        <v>433</v>
+      </c>
+      <c r="F88" t="s">
+        <v>397</v>
+      </c>
+      <c r="G88" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>399</v>
+      </c>
+      <c r="B89" t="s">
+        <v>398</v>
+      </c>
+      <c r="C89" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" t="s">
+      <c r="E89" t="s">
+        <v>433</v>
+      </c>
+      <c r="F89" t="s">
+        <v>400</v>
+      </c>
+      <c r="G89" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>408</v>
+      </c>
+      <c r="B90" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
+      <c r="C90" t="s">
+        <v>295</v>
+      </c>
+      <c r="D90" t="s">
+        <v>407</v>
+      </c>
+      <c r="E90" t="s">
+        <v>212</v>
+      </c>
+      <c r="F90" t="s">
+        <v>406</v>
+      </c>
+      <c r="G90" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>411</v>
+      </c>
+      <c r="B91" t="s">
+        <v>410</v>
+      </c>
+      <c r="C91" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" t="s">
+      <c r="E91" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91" t="s">
+        <v>409</v>
+      </c>
+      <c r="G91" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>412</v>
+      </c>
+      <c r="B92" t="s">
+        <v>415</v>
+      </c>
+      <c r="C92" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" t="s">
+      <c r="D92" t="s">
+        <v>413</v>
+      </c>
+      <c r="E92" t="s">
+        <v>433</v>
+      </c>
+      <c r="F92" t="s">
+        <v>414</v>
+      </c>
+      <c r="G92" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>420</v>
+      </c>
+      <c r="B93" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
+      <c r="C93" t="s">
+        <v>298</v>
+      </c>
+      <c r="D93" t="s">
+        <v>417</v>
+      </c>
+      <c r="E93" t="s">
+        <v>416</v>
+      </c>
+      <c r="F93" t="s">
+        <v>418</v>
+      </c>
+      <c r="G93" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>423</v>
+      </c>
+      <c r="B94" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
+      <c r="C94" t="s">
+        <v>299</v>
+      </c>
+      <c r="E94" t="s">
+        <v>421</v>
+      </c>
+      <c r="F94" t="s">
+        <v>422</v>
+      </c>
+      <c r="G94" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>424</v>
+      </c>
+      <c r="B95" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C88" t="s">
+      <c r="C95" t="s">
+        <v>300</v>
+      </c>
+      <c r="E95" t="s">
+        <v>433</v>
+      </c>
+      <c r="F95" t="s">
+        <v>425</v>
+      </c>
+      <c r="G95" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>427</v>
+      </c>
+      <c r="B96" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C92" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C93" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C94" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C95" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
+        <v>426</v>
+      </c>
+      <c r="G96" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>402</v>
+      </c>
+      <c r="B97" t="s">
+        <v>401</v>
+      </c>
       <c r="C97" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C98" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C100" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C101" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C102" t="s">
-        <v>315</v>
+        <v>404</v>
+      </c>
+      <c r="E97" t="s">
+        <v>433</v>
+      </c>
+      <c r="F97" t="s">
+        <v>403</v>
+      </c>
+      <c r="G97" t="s">
+        <v>232</v>
+      </c>
+      <c r="H97" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a few missing entries fixed
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5367018F-94C7-CB45-8768-D1DA715787E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF07741C-AA43-B145-92B1-2C675C3A875C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24740" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="439">
   <si>
     <t>name</t>
   </si>
@@ -1331,6 +1331,12 @@
   </si>
   <si>
     <t>Data sharing (NMR nD)</t>
+  </si>
+  <si>
+    <t>Real-time visualization tools for imaging spectroscopy</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/bioinformatics/article/28/15/2088/236639</t>
   </si>
 </sst>
 </file>
@@ -2193,10 +2199,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3191,6 +3197,9 @@
       <c r="C48" t="s">
         <v>192</v>
       </c>
+      <c r="D48" t="s">
+        <v>438</v>
+      </c>
       <c r="E48" t="s">
         <v>5</v>
       </c>
@@ -3692,6 +3701,9 @@
       </c>
       <c r="E71" t="s">
         <v>212</v>
+      </c>
+      <c r="F71" t="s">
+        <v>437</v>
       </c>
       <c r="G71" t="s">
         <v>338</v>

</xml_diff>

<commit_message>
troubleshooting a bad link/date
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF07741C-AA43-B145-92B1-2C675C3A875C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48D0291-1FED-7544-812E-1DDC2EB59B58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1336,7 +1336,7 @@
     <t>Real-time visualization tools for imaging spectroscopy</t>
   </si>
   <si>
-    <t>https://academic.oup.com/bioinformatics/article/28/15/2088/236639</t>
+    <t>https://arxiv.org/abs/1105.2204</t>
   </si>
 </sst>
 </file>
@@ -2199,8 +2199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>

</xml_diff>

<commit_message>
Fixed some errors in xlsx
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48D0291-1FED-7544-812E-1DDC2EB59B58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246C20D7-26D7-1B49-BBF9-9226364729F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2680" windowWidth="24740" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="451">
   <si>
     <t>name</t>
   </si>
@@ -181,9 +181,6 @@
     <t>https://github.com/INRA/Rnmr1D</t>
   </si>
   <si>
-    <t>https://link.springer.com/article/10.1007/s11306-017-1178-y</t>
-  </si>
-  <si>
     <t>TIMP</t>
   </si>
   <si>
@@ -1337,6 +1334,45 @@
   </si>
   <si>
     <t>https://arxiv.org/abs/1105.2204</t>
+  </si>
+  <si>
+    <t>Toolbox for coherent multidimensional spectroscopy</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/10.1021/acs.analchem.7b02917</t>
+  </si>
+  <si>
+    <t>https://github.com/wright-group/WrightTools</t>
+  </si>
+  <si>
+    <t>http://wright.tools/en/stable/</t>
+  </si>
+  <si>
+    <t>http://rnmr.nmrfam.wisc.edu/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/19821464</t>
+  </si>
+  <si>
+    <t>NMRProcFlow</t>
+  </si>
+  <si>
+    <t>WrightTools</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007%2Fs11306-017-1178-y</t>
+  </si>
+  <si>
+    <t>Interactive processing of 1D NMR spectra for metabolomics</t>
+  </si>
+  <si>
+    <t>rNMR</t>
+  </si>
+  <si>
+    <t>Visualization of 1D and 2D NMR</t>
+  </si>
+  <si>
+    <t>daniel.jacob@inra.fr</t>
   </si>
 </sst>
 </file>
@@ -2197,12 +2233,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2225,22 +2261,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2260,7 +2296,7 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2280,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2303,7 +2339,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2323,7 +2359,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2340,13 +2376,13 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2366,7 +2402,7 @@
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2386,7 +2422,7 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2403,10 +2439,10 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2426,7 +2462,7 @@
         <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2449,7 +2485,7 @@
         <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2469,290 +2505,287 @@
         <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>264</v>
+        <v>57</v>
       </c>
       <c r="G13" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>428</v>
       </c>
       <c r="G14" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>429</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>230</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>259</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G21" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G22" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>95</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>101</v>
+      </c>
+      <c r="C25" t="s">
+        <v>120</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="G25" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
         <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F26" t="s">
         <v>123</v>
       </c>
       <c r="G26" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2763,33 +2796,33 @@
         <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F27" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>262</v>
       </c>
       <c r="G28" t="s">
         <v>219</v>
@@ -2797,22 +2830,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" t="s">
         <v>132</v>
       </c>
-      <c r="B29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" t="s">
-        <v>130</v>
-      </c>
       <c r="E29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F29" t="s">
-        <v>263</v>
+        <v>136</v>
       </c>
       <c r="G29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -2823,53 +2856,56 @@
         <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
         <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="G31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B32" t="s">
         <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>142</v>
+      </c>
+      <c r="D32" t="s">
+        <v>143</v>
       </c>
       <c r="E32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F32" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="G32" t="s">
         <v>219</v>
@@ -2877,30 +2913,27 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
         <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
+        <v>432</v>
+      </c>
+      <c r="F33" t="s">
         <v>144</v>
       </c>
-      <c r="E33" t="s">
-        <v>433</v>
-      </c>
-      <c r="F33" t="s">
-        <v>142</v>
-      </c>
       <c r="G33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B34" t="s">
         <v>109</v>
@@ -2908,14 +2941,17 @@
       <c r="C34" t="s">
         <v>147</v>
       </c>
+      <c r="D34" t="s">
+        <v>148</v>
+      </c>
       <c r="E34" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F34" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="G34" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2926,99 +2962,96 @@
         <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>148</v>
-      </c>
-      <c r="D35" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F35" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="G35" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B36" t="s">
         <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F36" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G36" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B37" t="s">
         <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F37" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G37" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B38" t="s">
         <v>113</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
+        <v>162</v>
       </c>
       <c r="E38" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F38" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
         <v>114</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
-      </c>
-      <c r="D39" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F39" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G39" t="s">
         <v>220</v>
@@ -3026,27 +3059,27 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
         <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F40" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G40" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B41" t="s">
         <v>116</v>
@@ -3055,13 +3088,13 @@
         <v>168</v>
       </c>
       <c r="E41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F41" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="G41" t="s">
-        <v>219</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -3072,142 +3105,142 @@
         <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
+        <v>174</v>
+      </c>
+      <c r="D42" t="s">
+        <v>175</v>
       </c>
       <c r="E42" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F42" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G42" t="s">
-        <v>171</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B43" t="s">
         <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>175</v>
-      </c>
-      <c r="D43" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E43" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F43" t="s">
-        <v>174</v>
+        <v>261</v>
       </c>
       <c r="G43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
       <c r="C44" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E44" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F44" t="s">
-        <v>262</v>
+        <v>181</v>
       </c>
       <c r="G44" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E45" t="s">
-        <v>433</v>
+        <v>5</v>
       </c>
       <c r="F45" t="s">
-        <v>182</v>
+        <v>260</v>
       </c>
       <c r="G45" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>183</v>
-      </c>
-      <c r="B46" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="C46" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>261</v>
+        <v>429</v>
       </c>
       <c r="G46" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>187</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="B47" t="s">
+        <v>190</v>
       </c>
       <c r="C47" t="s">
-        <v>189</v>
+        <v>191</v>
+      </c>
+      <c r="D47" t="s">
+        <v>437</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>430</v>
+        <v>192</v>
       </c>
       <c r="G47" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C48" t="s">
-        <v>192</v>
-      </c>
-      <c r="D48" t="s">
-        <v>438</v>
+        <v>193</v>
       </c>
       <c r="E48" t="s">
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>193</v>
+        <v>259</v>
       </c>
       <c r="G48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -3215,234 +3248,240 @@
         <v>195</v>
       </c>
       <c r="B49" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s">
-        <v>194</v>
+        <v>196</v>
+      </c>
+      <c r="D49" t="s">
+        <v>197</v>
       </c>
       <c r="E49" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="F49" t="s">
-        <v>260</v>
+        <v>430</v>
       </c>
       <c r="G49" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B50" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C50" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D50" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E50" t="s">
-        <v>433</v>
+        <v>203</v>
       </c>
       <c r="F50" t="s">
-        <v>431</v>
+        <v>202</v>
       </c>
       <c r="G50" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C51" t="s">
-        <v>202</v>
-      </c>
-      <c r="D51" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E51" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F51" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="G51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C52" t="s">
         <v>208</v>
       </c>
+      <c r="D52" t="s">
+        <v>251</v>
+      </c>
       <c r="E52" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F52" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G52" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B53" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C53" t="s">
-        <v>209</v>
-      </c>
-      <c r="D53" t="s">
-        <v>252</v>
+        <v>213</v>
       </c>
       <c r="E53" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F53" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="G53" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="C54" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="E54" t="s">
-        <v>216</v>
+        <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>217</v>
+        <v>431</v>
       </c>
       <c r="G54" t="s">
-        <v>220</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B55" t="s">
         <v>237</v>
       </c>
-      <c r="C55" t="s">
-        <v>236</v>
-      </c>
       <c r="E55" t="s">
         <v>5</v>
       </c>
       <c r="F55" t="s">
-        <v>432</v>
+        <v>239</v>
       </c>
       <c r="G55" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B56" t="s">
-        <v>238</v>
+        <v>265</v>
+      </c>
+      <c r="C56" t="s">
+        <v>265</v>
       </c>
       <c r="E56" t="s">
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G56" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="B57" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C57" t="s">
-        <v>266</v>
+        <v>246</v>
+      </c>
+      <c r="D57" t="s">
+        <v>247</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="G57" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B58" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C58" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="D58" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E58" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="F58" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="G58" t="s">
-        <v>232</v>
+        <v>257</v>
+      </c>
+      <c r="H58" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
       <c r="B59" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="C59" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="D59" t="s">
-        <v>254</v>
+        <v>303</v>
       </c>
       <c r="E59" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F59" t="s">
-        <v>265</v>
+        <v>301</v>
       </c>
       <c r="G59" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H59" t="s">
-        <v>257</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -3455,25 +3494,22 @@
       <c r="C60" t="s">
         <v>267</v>
       </c>
-      <c r="D60" t="s">
-        <v>304</v>
-      </c>
       <c r="E60" t="s">
+        <v>432</v>
+      </c>
+      <c r="F60" t="s">
+        <v>306</v>
+      </c>
+      <c r="G60" t="s">
         <v>433</v>
       </c>
-      <c r="F60" t="s">
-        <v>302</v>
-      </c>
-      <c r="G60" t="s">
-        <v>258</v>
-      </c>
       <c r="H60" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B61" t="s">
         <v>268</v>
@@ -3481,22 +3517,22 @@
       <c r="C61" t="s">
         <v>268</v>
       </c>
+      <c r="D61" t="s">
+        <v>311</v>
+      </c>
       <c r="E61" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F61" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G61" t="s">
-        <v>434</v>
-      </c>
-      <c r="H61" t="s">
-        <v>309</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B62" t="s">
         <v>269</v>
@@ -3504,22 +3540,19 @@
       <c r="C62" t="s">
         <v>269</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
+        <v>432</v>
+      </c>
+      <c r="F62" t="s">
         <v>312</v>
       </c>
-      <c r="E62" t="s">
-        <v>433</v>
-      </c>
-      <c r="F62" t="s">
-        <v>311</v>
-      </c>
       <c r="G62" t="s">
-        <v>228</v>
+        <v>338</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B63" t="s">
         <v>270</v>
@@ -3527,19 +3560,22 @@
       <c r="C63" t="s">
         <v>270</v>
       </c>
+      <c r="D63" t="s">
+        <v>315</v>
+      </c>
       <c r="E63" t="s">
-        <v>433</v>
+        <v>203</v>
       </c>
       <c r="F63" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G63" t="s">
-        <v>339</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B64" t="s">
         <v>271</v>
@@ -3548,62 +3584,59 @@
         <v>271</v>
       </c>
       <c r="D64" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="E64" t="s">
-        <v>204</v>
+        <v>432</v>
       </c>
       <c r="F64" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="G64" t="s">
-        <v>220</v>
+        <v>228</v>
+      </c>
+      <c r="H64" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B65" t="s">
-        <v>272</v>
+        <v>322</v>
       </c>
       <c r="C65" t="s">
         <v>272</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
+        <v>432</v>
+      </c>
+      <c r="F65" t="s">
         <v>321</v>
       </c>
-      <c r="E65" t="s">
-        <v>433</v>
-      </c>
-      <c r="F65" t="s">
-        <v>319</v>
-      </c>
       <c r="G65" t="s">
-        <v>229</v>
-      </c>
-      <c r="H65" t="s">
-        <v>318</v>
+        <v>434</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B66" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="C66" t="s">
         <v>273</v>
       </c>
       <c r="E66" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F66" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G66" t="s">
-        <v>435</v>
+        <v>325</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -3617,76 +3650,79 @@
         <v>274</v>
       </c>
       <c r="E67" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F67" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G67" t="s">
-        <v>326</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B68" t="s">
-        <v>275</v>
+        <v>331</v>
       </c>
       <c r="C68" t="s">
         <v>275</v>
       </c>
       <c r="E68" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F68" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G68" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B69" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C69" t="s">
         <v>276</v>
       </c>
+      <c r="D69" t="s">
+        <v>333</v>
+      </c>
       <c r="E69" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F69" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G69" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B70" t="s">
-        <v>336</v>
+        <v>277</v>
       </c>
       <c r="C70" t="s">
         <v>277</v>
       </c>
-      <c r="D70" t="s">
-        <v>334</v>
-      </c>
       <c r="E70" t="s">
-        <v>433</v>
+        <v>211</v>
       </c>
       <c r="F70" t="s">
-        <v>333</v>
+        <v>436</v>
       </c>
       <c r="G70" t="s">
-        <v>221</v>
+        <v>337</v>
+      </c>
+      <c r="H70" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -3694,88 +3730,85 @@
         <v>340</v>
       </c>
       <c r="B71" t="s">
-        <v>278</v>
+        <v>342</v>
       </c>
       <c r="C71" t="s">
         <v>278</v>
       </c>
+      <c r="D71" t="s">
+        <v>342</v>
+      </c>
       <c r="E71" t="s">
-        <v>212</v>
+        <v>5</v>
       </c>
       <c r="F71" t="s">
-        <v>437</v>
+        <v>341</v>
       </c>
       <c r="G71" t="s">
-        <v>338</v>
+        <v>228</v>
       </c>
       <c r="H71" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B72" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C72" t="s">
         <v>279</v>
       </c>
-      <c r="D72" t="s">
-        <v>343</v>
-      </c>
       <c r="E72" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="F72" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G72" t="s">
-        <v>229</v>
-      </c>
-      <c r="H72" t="s">
-        <v>347</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B73" t="s">
-        <v>346</v>
+        <v>280</v>
       </c>
       <c r="C73" t="s">
         <v>280</v>
       </c>
       <c r="E73" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F73" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="G73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B74" t="s">
-        <v>281</v>
+        <v>351</v>
       </c>
       <c r="C74" t="s">
         <v>281</v>
       </c>
       <c r="E74" t="s">
-        <v>433</v>
+        <v>206</v>
       </c>
       <c r="F74" t="s">
         <v>349</v>
       </c>
       <c r="G74" t="s">
-        <v>220</v>
+        <v>350</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -3783,24 +3816,24 @@
         <v>353</v>
       </c>
       <c r="B75" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
       <c r="C75" t="s">
         <v>282</v>
       </c>
       <c r="E75" t="s">
-        <v>207</v>
+        <v>432</v>
       </c>
       <c r="F75" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="G75" t="s">
-        <v>351</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B76" t="s">
         <v>283</v>
@@ -3808,19 +3841,25 @@
       <c r="C76" t="s">
         <v>283</v>
       </c>
+      <c r="D76" t="s">
+        <v>356</v>
+      </c>
       <c r="E76" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F76" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G76" t="s">
-        <v>219</v>
+        <v>227</v>
+      </c>
+      <c r="H76" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B77" t="s">
         <v>284</v>
@@ -3828,17 +3867,14 @@
       <c r="C77" t="s">
         <v>284</v>
       </c>
-      <c r="D77" t="s">
-        <v>357</v>
-      </c>
       <c r="E77" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F77" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G77" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="H77" t="s">
         <v>359</v>
@@ -3846,96 +3882,96 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>363</v>
+      </c>
+      <c r="B78" t="s">
         <v>362</v>
-      </c>
-      <c r="B78" t="s">
-        <v>285</v>
       </c>
       <c r="C78" t="s">
         <v>285</v>
       </c>
+      <c r="D78" t="s">
+        <v>364</v>
+      </c>
       <c r="E78" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F78" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="G78" t="s">
-        <v>259</v>
-      </c>
-      <c r="H78" t="s">
-        <v>360</v>
+        <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B79" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C79" t="s">
-        <v>286</v>
-      </c>
-      <c r="D79" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="E79" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F79" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="G79" t="s">
-        <v>308</v>
+        <v>228</v>
+      </c>
+      <c r="H79" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B80" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="C80" t="s">
-        <v>369</v>
+        <v>286</v>
       </c>
       <c r="E80" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F80" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="G80" t="s">
-        <v>229</v>
-      </c>
-      <c r="H80" t="s">
-        <v>371</v>
+        <v>257</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B81" t="s">
-        <v>374</v>
+        <v>287</v>
       </c>
       <c r="C81" t="s">
         <v>287</v>
       </c>
       <c r="E81" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F81" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="G81" t="s">
-        <v>258</v>
+        <v>228</v>
+      </c>
+      <c r="H81" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B82" t="s">
         <v>288</v>
@@ -3944,21 +3980,21 @@
         <v>288</v>
       </c>
       <c r="E82" t="s">
-        <v>433</v>
+        <v>5</v>
       </c>
       <c r="F82" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G82" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H82" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B83" t="s">
         <v>289</v>
@@ -3967,162 +4003,159 @@
         <v>289</v>
       </c>
       <c r="E83" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="F83" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G83" t="s">
-        <v>229</v>
-      </c>
-      <c r="H83" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>383</v>
+      </c>
+      <c r="B84" t="s">
+        <v>384</v>
+      </c>
+      <c r="C84" t="s">
         <v>382</v>
       </c>
-      <c r="B84" t="s">
-        <v>290</v>
-      </c>
-      <c r="C84" t="s">
-        <v>290</v>
-      </c>
       <c r="E84" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F84" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="G84" t="s">
-        <v>339</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B85" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="C85" t="s">
-        <v>383</v>
+        <v>290</v>
       </c>
       <c r="E85" t="s">
-        <v>433</v>
+        <v>387</v>
       </c>
       <c r="F85" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="G85" t="s">
-        <v>259</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B86" t="s">
-        <v>390</v>
+        <v>291</v>
       </c>
       <c r="C86" t="s">
         <v>291</v>
       </c>
       <c r="E86" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="F86" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="G86" t="s">
-        <v>219</v>
+        <v>258</v>
+      </c>
+      <c r="H86" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B87" t="s">
-        <v>292</v>
+        <v>395</v>
       </c>
       <c r="C87" t="s">
         <v>292</v>
       </c>
       <c r="E87" t="s">
-        <v>392</v>
+        <v>432</v>
       </c>
       <c r="F87" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="G87" t="s">
-        <v>259</v>
-      </c>
-      <c r="H87" t="s">
-        <v>394</v>
+        <v>231</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B88" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C88" t="s">
         <v>293</v>
       </c>
       <c r="E88" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F88" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G88" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="B89" t="s">
-        <v>398</v>
+        <v>294</v>
       </c>
       <c r="C89" t="s">
         <v>294</v>
       </c>
+      <c r="D89" t="s">
+        <v>406</v>
+      </c>
       <c r="E89" t="s">
-        <v>433</v>
+        <v>211</v>
       </c>
       <c r="F89" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="G89" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B90" t="s">
-        <v>295</v>
+        <v>409</v>
       </c>
       <c r="C90" t="s">
         <v>295</v>
       </c>
-      <c r="D90" t="s">
-        <v>407</v>
-      </c>
       <c r="E90" t="s">
-        <v>212</v>
+        <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G90" t="s">
-        <v>229</v>
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -4130,47 +4163,50 @@
         <v>411</v>
       </c>
       <c r="B91" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C91" t="s">
         <v>296</v>
       </c>
+      <c r="D91" t="s">
+        <v>412</v>
+      </c>
       <c r="E91" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="F91" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="G91" t="s">
-        <v>351</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="B92" t="s">
-        <v>415</v>
+        <v>297</v>
       </c>
       <c r="C92" t="s">
         <v>297</v>
       </c>
       <c r="D92" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E92" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="F92" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="G92" t="s">
-        <v>233</v>
+        <v>418</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B93" t="s">
         <v>298</v>
@@ -4178,17 +4214,14 @@
       <c r="C93" t="s">
         <v>298</v>
       </c>
-      <c r="D93" t="s">
-        <v>417</v>
-      </c>
       <c r="E93" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="F93" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="G93" t="s">
-        <v>419</v>
+        <v>350</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -4202,18 +4235,18 @@
         <v>299</v>
       </c>
       <c r="E94" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="F94" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="G94" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B95" t="s">
         <v>300</v>
@@ -4222,61 +4255,130 @@
         <v>300</v>
       </c>
       <c r="E95" t="s">
-        <v>433</v>
+        <v>19</v>
       </c>
       <c r="F95" t="s">
         <v>425</v>
       </c>
       <c r="G95" t="s">
-        <v>351</v>
+        <v>435</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
       <c r="B96" t="s">
-        <v>301</v>
+        <v>400</v>
       </c>
       <c r="C96" t="s">
-        <v>301</v>
+        <v>403</v>
       </c>
       <c r="E96" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="F96" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="G96" t="s">
-        <v>436</v>
+        <v>231</v>
+      </c>
+      <c r="H96" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>402</v>
+        <v>445</v>
       </c>
       <c r="B97" t="s">
-        <v>401</v>
+        <v>441</v>
       </c>
       <c r="C97" t="s">
-        <v>404</v>
+        <v>440</v>
+      </c>
+      <c r="D97" t="s">
+        <v>439</v>
       </c>
       <c r="E97" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F97" t="s">
-        <v>403</v>
+        <v>438</v>
       </c>
       <c r="G97" t="s">
-        <v>232</v>
-      </c>
-      <c r="H97" t="s">
-        <v>405</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>444</v>
+      </c>
+      <c r="B98" t="s">
+        <v>51</v>
+      </c>
+      <c r="D98" t="s">
+        <v>446</v>
+      </c>
+      <c r="E98" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" t="s">
+        <v>447</v>
+      </c>
+      <c r="G98" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99" t="s">
+        <v>51</v>
+      </c>
+      <c r="C99" t="s">
+        <v>52</v>
+      </c>
+      <c r="D99" t="s">
+        <v>446</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+      <c r="F99" t="s">
+        <v>263</v>
+      </c>
+      <c r="G99" t="s">
+        <v>218</v>
+      </c>
+      <c r="H99" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>448</v>
+      </c>
+      <c r="B100" t="s">
+        <v>442</v>
+      </c>
+      <c r="D100" t="s">
+        <v>443</v>
+      </c>
+      <c r="E100" t="s">
+        <v>5</v>
+      </c>
+      <c r="F100" t="s">
+        <v>449</v>
+      </c>
+      <c r="G100" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B47" r:id="rId1" display="https://cran.r-project.org/package=pavo" xr:uid="{3E292708-18D0-1C48-B810-34D638D0D26E}"/>
+    <hyperlink ref="B46" r:id="rId1" display="https://cran.r-project.org/package=pavo" xr:uid="{3E292708-18D0-1C48-B810-34D638D0D26E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed a few more errors in xlsx
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246C20D7-26D7-1B49-BBF9-9226364729F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4059ED5F-8EAE-7F4D-8102-F628483FDBD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2680" windowWidth="24740" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="461">
   <si>
     <t>name</t>
   </si>
@@ -1291,9 +1291,6 @@
     <t>xrf_filetools</t>
   </si>
   <si>
-    <t>xrf_parsers</t>
-  </si>
-  <si>
     <t>Parse files from handheld XRF spectrometers</t>
   </si>
   <si>
@@ -1373,13 +1370,46 @@
   </si>
   <si>
     <t>daniel.jacob@inra.fr</t>
+  </si>
+  <si>
+    <t>PRFFECT</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0169743917305257</t>
+  </si>
+  <si>
+    <t>https://github.com/zhangfy1993/PRFFECT</t>
+  </si>
+  <si>
+    <t>benjamin.r.smith@strath.ac.uk</t>
+  </si>
+  <si>
+    <t>Pre-processing &amp; random forest feature extraction</t>
+  </si>
+  <si>
+    <t>https://bmcchem.biomedcentral.com/articles/10.1186/1752-153X-1-31</t>
+  </si>
+  <si>
+    <t>JSpecView</t>
+  </si>
+  <si>
+    <t>http://jspecview.sourceforge.net/</t>
+  </si>
+  <si>
+    <t>Read &amp; view spectra in JCAMP-DX format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">robert.lancashire@uwimona.edu.jm </t>
+  </si>
+  <si>
+    <t>xrf_parser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1527,6 +1557,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="HgqjsrGiovanni"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1871,12 +1912,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2233,15 +2276,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="61.33203125" customWidth="1"/>
@@ -2253,7 +2296,7 @@
     <col min="8" max="8" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2279,7 +2322,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2299,7 +2342,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2319,7 +2362,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2342,7 +2385,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2362,7 +2405,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2376,7 +2419,7 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
@@ -2385,7 +2428,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2405,7 +2448,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2425,7 +2468,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -2439,13 +2482,13 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G9" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2465,7 +2508,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2488,7 +2531,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2508,7 +2551,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2531,7 +2574,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2545,13 +2588,13 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2571,7 +2614,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -2588,7 +2631,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -2605,7 +2648,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2628,7 +2671,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -2648,7 +2691,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -2668,7 +2711,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2685,7 +2728,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -2708,7 +2751,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -2725,7 +2768,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2745,7 +2788,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -2759,7 +2802,7 @@
         <v>121</v>
       </c>
       <c r="E25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F25" t="s">
         <v>122</v>
@@ -2768,7 +2811,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>125</v>
       </c>
@@ -2779,7 +2822,7 @@
         <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F26" t="s">
         <v>123</v>
@@ -2788,7 +2831,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -2799,7 +2842,7 @@
         <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F27" t="s">
         <v>128</v>
@@ -2808,7 +2851,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>131</v>
       </c>
@@ -2819,7 +2862,7 @@
         <v>129</v>
       </c>
       <c r="E28" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F28" t="s">
         <v>262</v>
@@ -2828,7 +2871,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -2839,7 +2882,7 @@
         <v>132</v>
       </c>
       <c r="E29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F29" t="s">
         <v>136</v>
@@ -2848,7 +2891,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -2859,7 +2902,7 @@
         <v>139</v>
       </c>
       <c r="E30" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F30" t="s">
         <v>135</v>
@@ -2868,7 +2911,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -2879,7 +2922,7 @@
         <v>137</v>
       </c>
       <c r="E31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F31" t="s">
         <v>178</v>
@@ -2888,7 +2931,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>140</v>
       </c>
@@ -2902,7 +2945,7 @@
         <v>143</v>
       </c>
       <c r="E32" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -2911,7 +2954,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -2922,7 +2965,7 @@
         <v>146</v>
       </c>
       <c r="E33" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F33" t="s">
         <v>144</v>
@@ -2931,7 +2974,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -2945,7 +2988,7 @@
         <v>148</v>
       </c>
       <c r="E34" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F34" t="s">
         <v>179</v>
@@ -2954,7 +2997,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>150</v>
       </c>
@@ -2965,7 +3008,7 @@
         <v>152</v>
       </c>
       <c r="E35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F35" t="s">
         <v>151</v>
@@ -2974,7 +3017,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>153</v>
       </c>
@@ -2985,7 +3028,7 @@
         <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -2994,7 +3037,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>156</v>
       </c>
@@ -3005,7 +3048,7 @@
         <v>158</v>
       </c>
       <c r="E37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F37" t="s">
         <v>157</v>
@@ -3014,7 +3057,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -3028,7 +3071,7 @@
         <v>162</v>
       </c>
       <c r="E38" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F38" t="s">
         <v>160</v>
@@ -3037,7 +3080,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -3048,7 +3091,7 @@
         <v>165</v>
       </c>
       <c r="E39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -3057,7 +3100,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -3068,7 +3111,7 @@
         <v>167</v>
       </c>
       <c r="E40" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F40" t="s">
         <v>157</v>
@@ -3077,7 +3120,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>171</v>
       </c>
@@ -3088,7 +3131,7 @@
         <v>168</v>
       </c>
       <c r="E41" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F41" t="s">
         <v>169</v>
@@ -3097,7 +3140,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>172</v>
       </c>
@@ -3111,7 +3154,7 @@
         <v>175</v>
       </c>
       <c r="E42" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F42" t="s">
         <v>173</v>
@@ -3120,7 +3163,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>176</v>
       </c>
@@ -3131,7 +3174,7 @@
         <v>177</v>
       </c>
       <c r="E43" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F43" t="s">
         <v>261</v>
@@ -3140,7 +3183,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>180</v>
       </c>
@@ -3151,7 +3194,7 @@
         <v>185</v>
       </c>
       <c r="E44" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F44" t="s">
         <v>181</v>
@@ -3160,7 +3203,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -3180,7 +3223,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -3194,13 +3237,13 @@
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G46" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>189</v>
       </c>
@@ -3211,7 +3254,7 @@
         <v>191</v>
       </c>
       <c r="D47" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
@@ -3223,7 +3266,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>194</v>
       </c>
@@ -3243,7 +3286,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>195</v>
       </c>
@@ -3257,16 +3300,16 @@
         <v>197</v>
       </c>
       <c r="E49" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G49" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>198</v>
       </c>
@@ -3289,7 +3332,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>204</v>
       </c>
@@ -3309,7 +3352,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -3332,7 +3375,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>212</v>
       </c>
@@ -3352,7 +3395,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>234</v>
       </c>
@@ -3366,13 +3409,13 @@
         <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G54" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>238</v>
       </c>
@@ -3389,7 +3432,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>240</v>
       </c>
@@ -3409,7 +3452,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>250</v>
       </c>
@@ -3432,7 +3475,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>252</v>
       </c>
@@ -3446,7 +3489,7 @@
         <v>253</v>
       </c>
       <c r="E58" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F58" t="s">
         <v>264</v>
@@ -3458,7 +3501,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>304</v>
       </c>
@@ -3472,7 +3515,7 @@
         <v>303</v>
       </c>
       <c r="E59" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F59" t="s">
         <v>301</v>
@@ -3484,7 +3527,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>305</v>
       </c>
@@ -3495,19 +3538,19 @@
         <v>267</v>
       </c>
       <c r="E60" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F60" t="s">
         <v>306</v>
       </c>
       <c r="G60" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H60" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>309</v>
       </c>
@@ -3521,7 +3564,7 @@
         <v>311</v>
       </c>
       <c r="E61" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F61" t="s">
         <v>310</v>
@@ -3530,7 +3573,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>313</v>
       </c>
@@ -3541,7 +3584,7 @@
         <v>269</v>
       </c>
       <c r="E62" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F62" t="s">
         <v>312</v>
@@ -3550,7 +3593,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>316</v>
       </c>
@@ -3573,7 +3616,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>319</v>
       </c>
@@ -3587,7 +3630,7 @@
         <v>320</v>
       </c>
       <c r="E64" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F64" t="s">
         <v>318</v>
@@ -3599,7 +3642,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>323</v>
       </c>
@@ -3610,16 +3653,16 @@
         <v>272</v>
       </c>
       <c r="E65" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F65" t="s">
         <v>321</v>
       </c>
       <c r="G65" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>326</v>
       </c>
@@ -3630,7 +3673,7 @@
         <v>273</v>
       </c>
       <c r="E66" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F66" t="s">
         <v>324</v>
@@ -3639,7 +3682,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>327</v>
       </c>
@@ -3650,7 +3693,7 @@
         <v>274</v>
       </c>
       <c r="E67" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F67" t="s">
         <v>328</v>
@@ -3659,7 +3702,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>329</v>
       </c>
@@ -3670,7 +3713,7 @@
         <v>275</v>
       </c>
       <c r="E68" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F68" t="s">
         <v>330</v>
@@ -3679,7 +3722,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>334</v>
       </c>
@@ -3693,7 +3736,7 @@
         <v>333</v>
       </c>
       <c r="E69" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F69" t="s">
         <v>332</v>
@@ -3702,7 +3745,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>339</v>
       </c>
@@ -3716,7 +3759,7 @@
         <v>211</v>
       </c>
       <c r="F70" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G70" t="s">
         <v>337</v>
@@ -3725,12 +3768,12 @@
         <v>336</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>340</v>
       </c>
       <c r="B71" t="s">
-        <v>342</v>
+        <v>278</v>
       </c>
       <c r="C71" t="s">
         <v>278</v>
@@ -3751,7 +3794,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>343</v>
       </c>
@@ -3762,7 +3805,7 @@
         <v>279</v>
       </c>
       <c r="E72" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F72" t="s">
         <v>344</v>
@@ -3771,7 +3814,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>347</v>
       </c>
@@ -3782,7 +3825,7 @@
         <v>280</v>
       </c>
       <c r="E73" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F73" t="s">
         <v>348</v>
@@ -3791,7 +3834,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>352</v>
       </c>
@@ -3811,7 +3854,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>353</v>
       </c>
@@ -3822,7 +3865,7 @@
         <v>282</v>
       </c>
       <c r="E75" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F75" t="s">
         <v>354</v>
@@ -3831,7 +3874,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>355</v>
       </c>
@@ -3845,7 +3888,7 @@
         <v>356</v>
       </c>
       <c r="E76" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F76" t="s">
         <v>357</v>
@@ -3857,7 +3900,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>361</v>
       </c>
@@ -3868,7 +3911,7 @@
         <v>284</v>
       </c>
       <c r="E77" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F77" t="s">
         <v>360</v>
@@ -3880,7 +3923,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>363</v>
       </c>
@@ -3894,7 +3937,7 @@
         <v>364</v>
       </c>
       <c r="E78" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F78" t="s">
         <v>365</v>
@@ -3903,7 +3946,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>367</v>
       </c>
@@ -3914,7 +3957,7 @@
         <v>368</v>
       </c>
       <c r="E79" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F79" t="s">
         <v>369</v>
@@ -3926,7 +3969,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>371</v>
       </c>
@@ -3937,7 +3980,7 @@
         <v>286</v>
       </c>
       <c r="E80" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F80" t="s">
         <v>372</v>
@@ -3946,7 +3989,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>374</v>
       </c>
@@ -3957,7 +4000,7 @@
         <v>287</v>
       </c>
       <c r="E81" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F81" t="s">
         <v>376</v>
@@ -3969,7 +4012,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>377</v>
       </c>
@@ -3992,7 +4035,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>381</v>
       </c>
@@ -4003,7 +4046,7 @@
         <v>289</v>
       </c>
       <c r="E83" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F83" t="s">
         <v>380</v>
@@ -4012,7 +4055,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>383</v>
       </c>
@@ -4023,7 +4066,7 @@
         <v>382</v>
       </c>
       <c r="E84" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F84" t="s">
         <v>385</v>
@@ -4032,7 +4075,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>386</v>
       </c>
@@ -4052,7 +4095,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>390</v>
       </c>
@@ -4075,7 +4118,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>394</v>
       </c>
@@ -4086,7 +4129,7 @@
         <v>292</v>
       </c>
       <c r="E87" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F87" t="s">
         <v>396</v>
@@ -4095,7 +4138,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>398</v>
       </c>
@@ -4106,7 +4149,7 @@
         <v>293</v>
       </c>
       <c r="E88" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F88" t="s">
         <v>399</v>
@@ -4115,7 +4158,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>407</v>
       </c>
@@ -4138,7 +4181,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>410</v>
       </c>
@@ -4158,7 +4201,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>411</v>
       </c>
@@ -4172,7 +4215,7 @@
         <v>412</v>
       </c>
       <c r="E91" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F91" t="s">
         <v>413</v>
@@ -4181,7 +4224,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>419</v>
       </c>
@@ -4204,7 +4247,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>422</v>
       </c>
@@ -4224,9 +4267,9 @@
         <v>350</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>423</v>
+        <v>460</v>
       </c>
       <c r="B94" t="s">
         <v>299</v>
@@ -4235,18 +4278,18 @@
         <v>299</v>
       </c>
       <c r="E94" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F94" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G94" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B95" t="s">
         <v>300</v>
@@ -4258,13 +4301,13 @@
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G95" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>401</v>
       </c>
@@ -4275,7 +4318,7 @@
         <v>403</v>
       </c>
       <c r="E96" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F96" t="s">
         <v>402</v>
@@ -4287,50 +4330,50 @@
         <v>404</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B97" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C97" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D97" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E97" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F97" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G97" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B98" t="s">
         <v>51</v>
       </c>
       <c r="D98" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E98" t="s">
         <v>5</v>
       </c>
       <c r="F98" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G98" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>50</v>
       </c>
@@ -4341,7 +4384,7 @@
         <v>52</v>
       </c>
       <c r="D99" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E99" t="s">
         <v>5</v>
@@ -4353,27 +4396,76 @@
         <v>218</v>
       </c>
       <c r="H99" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B100" t="s">
+        <v>441</v>
+      </c>
+      <c r="D100" t="s">
         <v>442</v>
-      </c>
-      <c r="D100" t="s">
-        <v>443</v>
       </c>
       <c r="E100" t="s">
         <v>5</v>
       </c>
       <c r="F100" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G100" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="17">
+      <c r="A101" t="s">
+        <v>450</v>
+      </c>
+      <c r="B101" t="s">
+        <v>452</v>
+      </c>
+      <c r="C101" t="s">
+        <v>452</v>
+      </c>
+      <c r="D101" t="s">
+        <v>451</v>
+      </c>
+      <c r="E101" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" t="s">
+        <v>454</v>
+      </c>
+      <c r="G101" t="s">
+        <v>257</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>456</v>
+      </c>
+      <c r="B102" t="s">
+        <v>457</v>
+      </c>
+      <c r="D102" t="s">
+        <v>455</v>
+      </c>
+      <c r="E102" t="s">
+        <v>206</v>
+      </c>
+      <c r="F102" t="s">
+        <v>458</v>
+      </c>
+      <c r="G102" t="s">
+        <v>307</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cannot reach host peakaboo.org
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3A362B-2BB8-6148-90C2-063CEA90808A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087AAAD6-DB19-7F41-8F30-ACCC83089C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="1940" windowWidth="24740" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="473">
   <si>
     <t>name</t>
   </si>
@@ -1073,9 +1073,6 @@
   </si>
   <si>
     <t>XRF</t>
-  </si>
-  <si>
-    <t>https://peakaboo.org/</t>
   </si>
   <si>
     <t>Peakaboo</t>
@@ -2318,10 +2315,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2459,7 +2456,7 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
@@ -2522,7 +2519,7 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G9" t="s">
         <v>225</v>
@@ -2628,7 +2625,7 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G14" t="s">
         <v>243</v>
@@ -2842,7 +2839,7 @@
         <v>121</v>
       </c>
       <c r="E25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F25" t="s">
         <v>122</v>
@@ -2862,7 +2859,7 @@
         <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F26" t="s">
         <v>123</v>
@@ -2882,7 +2879,7 @@
         <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F27" t="s">
         <v>128</v>
@@ -2902,7 +2899,7 @@
         <v>129</v>
       </c>
       <c r="E28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F28" t="s">
         <v>262</v>
@@ -2922,7 +2919,7 @@
         <v>132</v>
       </c>
       <c r="E29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F29" t="s">
         <v>136</v>
@@ -2942,7 +2939,7 @@
         <v>139</v>
       </c>
       <c r="E30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F30" t="s">
         <v>135</v>
@@ -2962,7 +2959,7 @@
         <v>137</v>
       </c>
       <c r="E31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F31" t="s">
         <v>178</v>
@@ -2985,7 +2982,7 @@
         <v>143</v>
       </c>
       <c r="E32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -3005,7 +3002,7 @@
         <v>146</v>
       </c>
       <c r="E33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F33" t="s">
         <v>144</v>
@@ -3028,7 +3025,7 @@
         <v>148</v>
       </c>
       <c r="E34" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F34" t="s">
         <v>179</v>
@@ -3048,7 +3045,7 @@
         <v>152</v>
       </c>
       <c r="E35" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F35" t="s">
         <v>151</v>
@@ -3068,7 +3065,7 @@
         <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -3088,7 +3085,7 @@
         <v>158</v>
       </c>
       <c r="E37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F37" t="s">
         <v>157</v>
@@ -3111,7 +3108,7 @@
         <v>162</v>
       </c>
       <c r="E38" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F38" t="s">
         <v>160</v>
@@ -3131,7 +3128,7 @@
         <v>165</v>
       </c>
       <c r="E39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -3151,7 +3148,7 @@
         <v>167</v>
       </c>
       <c r="E40" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F40" t="s">
         <v>157</v>
@@ -3171,7 +3168,7 @@
         <v>168</v>
       </c>
       <c r="E41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F41" t="s">
         <v>169</v>
@@ -3194,7 +3191,7 @@
         <v>175</v>
       </c>
       <c r="E42" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F42" t="s">
         <v>173</v>
@@ -3214,7 +3211,7 @@
         <v>177</v>
       </c>
       <c r="E43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F43" t="s">
         <v>261</v>
@@ -3234,7 +3231,7 @@
         <v>185</v>
       </c>
       <c r="E44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F44" t="s">
         <v>181</v>
@@ -3277,7 +3274,7 @@
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G46" t="s">
         <v>231</v>
@@ -3294,7 +3291,7 @@
         <v>191</v>
       </c>
       <c r="D47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
@@ -3340,10 +3337,10 @@
         <v>197</v>
       </c>
       <c r="E49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F49" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G49" t="s">
         <v>222</v>
@@ -3449,7 +3446,7 @@
         <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G54" t="s">
         <v>258</v>
@@ -3529,7 +3526,7 @@
         <v>253</v>
       </c>
       <c r="E58" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F58" t="s">
         <v>264</v>
@@ -3555,7 +3552,7 @@
         <v>303</v>
       </c>
       <c r="E59" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F59" t="s">
         <v>301</v>
@@ -3578,13 +3575,13 @@
         <v>267</v>
       </c>
       <c r="E60" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F60" t="s">
         <v>306</v>
       </c>
       <c r="G60" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H60" t="s">
         <v>308</v>
@@ -3604,7 +3601,7 @@
         <v>311</v>
       </c>
       <c r="E61" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F61" t="s">
         <v>310</v>
@@ -3624,7 +3621,7 @@
         <v>269</v>
       </c>
       <c r="E62" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F62" t="s">
         <v>312</v>
@@ -3670,7 +3667,7 @@
         <v>320</v>
       </c>
       <c r="E64" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F64" t="s">
         <v>318</v>
@@ -3693,13 +3690,13 @@
         <v>272</v>
       </c>
       <c r="E65" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F65" t="s">
         <v>321</v>
       </c>
       <c r="G65" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3713,7 +3710,7 @@
         <v>273</v>
       </c>
       <c r="E66" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F66" t="s">
         <v>324</v>
@@ -3733,7 +3730,7 @@
         <v>274</v>
       </c>
       <c r="E67" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F67" t="s">
         <v>328</v>
@@ -3753,7 +3750,7 @@
         <v>275</v>
       </c>
       <c r="E68" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F68" t="s">
         <v>330</v>
@@ -3776,7 +3773,7 @@
         <v>333</v>
       </c>
       <c r="E69" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F69" t="s">
         <v>332</v>
@@ -3799,7 +3796,7 @@
         <v>211</v>
       </c>
       <c r="F70" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G70" t="s">
         <v>337</v>
@@ -3845,7 +3842,7 @@
         <v>279</v>
       </c>
       <c r="E72" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F72" t="s">
         <v>344</v>
@@ -3865,7 +3862,7 @@
         <v>280</v>
       </c>
       <c r="E73" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F73" t="s">
         <v>348</v>
@@ -3876,10 +3873,10 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B74" t="s">
-        <v>351</v>
+        <v>281</v>
       </c>
       <c r="C74" t="s">
         <v>281</v>
@@ -3896,7 +3893,7 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B75" t="s">
         <v>282</v>
@@ -3905,10 +3902,10 @@
         <v>282</v>
       </c>
       <c r="E75" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F75" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G75" t="s">
         <v>218</v>
@@ -3916,7 +3913,7 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B76" t="s">
         <v>283</v>
@@ -3925,24 +3922,24 @@
         <v>283</v>
       </c>
       <c r="D76" t="s">
+        <v>355</v>
+      </c>
+      <c r="E76" t="s">
+        <v>430</v>
+      </c>
+      <c r="F76" t="s">
         <v>356</v>
-      </c>
-      <c r="E76" t="s">
-        <v>431</v>
-      </c>
-      <c r="F76" t="s">
-        <v>357</v>
       </c>
       <c r="G76" t="s">
         <v>227</v>
       </c>
       <c r="H76" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B77" t="s">
         <v>284</v>
@@ -3951,36 +3948,36 @@
         <v>284</v>
       </c>
       <c r="E77" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F77" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G77" t="s">
         <v>258</v>
       </c>
       <c r="H77" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B78" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C78" t="s">
         <v>285</v>
       </c>
       <c r="D78" t="s">
+        <v>363</v>
+      </c>
+      <c r="E78" t="s">
+        <v>430</v>
+      </c>
+      <c r="F78" t="s">
         <v>364</v>
-      </c>
-      <c r="E78" t="s">
-        <v>431</v>
-      </c>
-      <c r="F78" t="s">
-        <v>365</v>
       </c>
       <c r="G78" t="s">
         <v>307</v>
@@ -3988,42 +3985,42 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
+        <v>366</v>
+      </c>
+      <c r="B79" t="s">
+        <v>365</v>
+      </c>
+      <c r="C79" t="s">
         <v>367</v>
       </c>
-      <c r="B79" t="s">
-        <v>366</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
+        <v>430</v>
+      </c>
+      <c r="F79" t="s">
         <v>368</v>
-      </c>
-      <c r="E79" t="s">
-        <v>431</v>
-      </c>
-      <c r="F79" t="s">
-        <v>369</v>
       </c>
       <c r="G79" t="s">
         <v>228</v>
       </c>
       <c r="H79" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C80" t="s">
         <v>286</v>
       </c>
       <c r="E80" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F80" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G80" t="s">
         <v>257</v>
@@ -4031,7 +4028,7 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B81" t="s">
         <v>287</v>
@@ -4040,21 +4037,21 @@
         <v>287</v>
       </c>
       <c r="E81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F81" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G81" t="s">
         <v>228</v>
       </c>
       <c r="H81" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B82" t="s">
         <v>288</v>
@@ -4066,18 +4063,18 @@
         <v>5</v>
       </c>
       <c r="F82" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G82" t="s">
         <v>228</v>
       </c>
       <c r="H82" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B83" t="s">
         <v>289</v>
@@ -4086,10 +4083,10 @@
         <v>289</v>
       </c>
       <c r="E83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F83" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G83" t="s">
         <v>338</v>
@@ -4097,19 +4094,19 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
+        <v>382</v>
+      </c>
+      <c r="B84" t="s">
         <v>383</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>381</v>
+      </c>
+      <c r="E84" t="s">
+        <v>430</v>
+      </c>
+      <c r="F84" t="s">
         <v>384</v>
-      </c>
-      <c r="C84" t="s">
-        <v>382</v>
-      </c>
-      <c r="E84" t="s">
-        <v>431</v>
-      </c>
-      <c r="F84" t="s">
-        <v>385</v>
       </c>
       <c r="G84" t="s">
         <v>258</v>
@@ -4117,19 +4114,19 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B85" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C85" t="s">
         <v>290</v>
       </c>
       <c r="E85" t="s">
+        <v>386</v>
+      </c>
+      <c r="F85" t="s">
         <v>387</v>
-      </c>
-      <c r="F85" t="s">
-        <v>388</v>
       </c>
       <c r="G85" t="s">
         <v>218</v>
@@ -4137,7 +4134,7 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B86" t="s">
         <v>291</v>
@@ -4146,33 +4143,33 @@
         <v>291</v>
       </c>
       <c r="E86" t="s">
+        <v>390</v>
+      </c>
+      <c r="F86" t="s">
         <v>391</v>
-      </c>
-      <c r="F86" t="s">
-        <v>392</v>
       </c>
       <c r="G86" t="s">
         <v>258</v>
       </c>
       <c r="H86" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
+        <v>393</v>
+      </c>
+      <c r="B87" t="s">
         <v>394</v>
-      </c>
-      <c r="B87" t="s">
-        <v>395</v>
       </c>
       <c r="C87" t="s">
         <v>292</v>
       </c>
       <c r="E87" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F87" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G87" t="s">
         <v>231</v>
@@ -4180,19 +4177,19 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B88" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C88" t="s">
         <v>293</v>
       </c>
       <c r="E88" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F88" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G88" t="s">
         <v>231</v>
@@ -4200,7 +4197,7 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B89" t="s">
         <v>294</v>
@@ -4209,13 +4206,13 @@
         <v>294</v>
       </c>
       <c r="D89" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E89" t="s">
         <v>211</v>
       </c>
       <c r="F89" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G89" t="s">
         <v>228</v>
@@ -4223,10 +4220,10 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B90" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C90" t="s">
         <v>295</v>
@@ -4235,7 +4232,7 @@
         <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G90" t="s">
         <v>350</v>
@@ -4243,22 +4240,22 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B91" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C91" t="s">
         <v>296</v>
       </c>
       <c r="D91" t="s">
+        <v>411</v>
+      </c>
+      <c r="E91" t="s">
+        <v>430</v>
+      </c>
+      <c r="F91" t="s">
         <v>412</v>
-      </c>
-      <c r="E91" t="s">
-        <v>431</v>
-      </c>
-      <c r="F91" t="s">
-        <v>413</v>
       </c>
       <c r="G91" t="s">
         <v>232</v>
@@ -4266,7 +4263,7 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B92" t="s">
         <v>297</v>
@@ -4275,21 +4272,21 @@
         <v>297</v>
       </c>
       <c r="D92" t="s">
+        <v>415</v>
+      </c>
+      <c r="E92" t="s">
+        <v>414</v>
+      </c>
+      <c r="F92" t="s">
         <v>416</v>
       </c>
-      <c r="E92" t="s">
-        <v>415</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>417</v>
-      </c>
-      <c r="G92" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B93" t="s">
         <v>298</v>
@@ -4298,10 +4295,10 @@
         <v>298</v>
       </c>
       <c r="E93" t="s">
+        <v>419</v>
+      </c>
+      <c r="F93" t="s">
         <v>420</v>
-      </c>
-      <c r="F93" t="s">
-        <v>421</v>
       </c>
       <c r="G93" t="s">
         <v>350</v>
@@ -4309,7 +4306,7 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B94" t="s">
         <v>299</v>
@@ -4318,10 +4315,10 @@
         <v>299</v>
       </c>
       <c r="E94" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F94" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G94" t="s">
         <v>350</v>
@@ -4329,7 +4326,7 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B95" t="s">
         <v>300</v>
@@ -4341,53 +4338,53 @@
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G95" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
+        <v>400</v>
+      </c>
+      <c r="B96" t="s">
+        <v>399</v>
+      </c>
+      <c r="C96" t="s">
+        <v>402</v>
+      </c>
+      <c r="E96" t="s">
+        <v>430</v>
+      </c>
+      <c r="F96" t="s">
         <v>401</v>
-      </c>
-      <c r="B96" t="s">
-        <v>400</v>
-      </c>
-      <c r="C96" t="s">
-        <v>403</v>
-      </c>
-      <c r="E96" t="s">
-        <v>431</v>
-      </c>
-      <c r="F96" t="s">
-        <v>402</v>
       </c>
       <c r="G96" t="s">
         <v>231</v>
       </c>
       <c r="H96" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B97" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C97" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D97" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E97" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F97" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G97" t="s">
         <v>228</v>
@@ -4395,19 +4392,19 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B98" t="s">
         <v>51</v>
       </c>
       <c r="D98" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E98" t="s">
         <v>5</v>
       </c>
       <c r="F98" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G98" t="s">
         <v>218</v>
@@ -4424,7 +4421,7 @@
         <v>52</v>
       </c>
       <c r="D99" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E99" t="s">
         <v>5</v>
@@ -4436,24 +4433,24 @@
         <v>218</v>
       </c>
       <c r="H99" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B100" t="s">
+        <v>440</v>
+      </c>
+      <c r="D100" t="s">
         <v>441</v>
-      </c>
-      <c r="D100" t="s">
-        <v>442</v>
       </c>
       <c r="E100" t="s">
         <v>5</v>
       </c>
       <c r="F100" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G100" t="s">
         <v>221</v>
@@ -4461,103 +4458,103 @@
     </row>
     <row r="101" spans="1:8" ht="17">
       <c r="A101" t="s">
+        <v>449</v>
+      </c>
+      <c r="B101" t="s">
+        <v>451</v>
+      </c>
+      <c r="C101" t="s">
+        <v>451</v>
+      </c>
+      <c r="D101" t="s">
         <v>450</v>
-      </c>
-      <c r="B101" t="s">
-        <v>452</v>
-      </c>
-      <c r="C101" t="s">
-        <v>452</v>
-      </c>
-      <c r="D101" t="s">
-        <v>451</v>
       </c>
       <c r="E101" t="s">
         <v>5</v>
       </c>
       <c r="F101" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G101" t="s">
         <v>257</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
+        <v>455</v>
+      </c>
+      <c r="B102" t="s">
         <v>456</v>
       </c>
-      <c r="B102" t="s">
-        <v>457</v>
-      </c>
       <c r="D102" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E102" t="s">
         <v>206</v>
       </c>
       <c r="F102" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G102" t="s">
         <v>307</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
+        <v>460</v>
+      </c>
+      <c r="B103" t="s">
+        <v>462</v>
+      </c>
+      <c r="C103" t="s">
         <v>461</v>
       </c>
-      <c r="B103" t="s">
+      <c r="D103" t="s">
         <v>463</v>
-      </c>
-      <c r="C103" t="s">
-        <v>462</v>
-      </c>
-      <c r="D103" t="s">
-        <v>464</v>
       </c>
       <c r="E103" t="s">
         <v>5</v>
       </c>
       <c r="F103" t="s">
+        <v>464</v>
+      </c>
+      <c r="G103" t="s">
         <v>465</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H103" t="s">
         <v>466</v>
-      </c>
-      <c r="H103" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
+        <v>467</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="C104" t="s">
+        <v>470</v>
+      </c>
+      <c r="D104" t="s">
         <v>468</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="C104" t="s">
-        <v>471</v>
-      </c>
-      <c r="D104" t="s">
-        <v>469</v>
       </c>
       <c r="E104" t="s">
         <v>5</v>
       </c>
       <c r="F104" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G104" t="s">
         <v>257</v>
       </c>
       <c r="H104" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restored peakaboo.org link (fixed by owner)
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087AAAD6-DB19-7F41-8F30-ACCC83089C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8400DF65-2F3F-BE4A-BBC7-359736ED0AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="1940" windowWidth="24740" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="474">
   <si>
     <t>name</t>
   </si>
@@ -1439,6 +1439,9 @@
   </si>
   <si>
     <t>Robert Geitner &lt;r.geitner at uu.nl&gt;</t>
+  </si>
+  <si>
+    <t>https://peakaboo.org</t>
   </si>
 </sst>
 </file>
@@ -2315,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
@@ -3876,7 +3879,7 @@
         <v>351</v>
       </c>
       <c r="B74" t="s">
-        <v>281</v>
+        <v>473</v>
       </c>
       <c r="C74" t="s">
         <v>281</v>

</xml_diff>

<commit_message>
add OpenVibSpec & octavvs
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8400DF65-2F3F-BE4A-BBC7-359736ED0AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1414FF83-2777-534C-B21E-BAA60B96A90C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="1940" windowWidth="24740" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26240" yWindow="1200" windowWidth="22640" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="480">
   <si>
     <t>name</t>
   </si>
@@ -1442,6 +1442,24 @@
   </si>
   <si>
     <t>https://peakaboo.org</t>
+  </si>
+  <si>
+    <t>OpenVibSpec</t>
+  </si>
+  <si>
+    <t>https://github.com/arnrau/OpenVibSpec</t>
+  </si>
+  <si>
+    <t>Vibrational spectroscopy</t>
+  </si>
+  <si>
+    <t>IR, Raman</t>
+  </si>
+  <si>
+    <t>octavvs</t>
+  </si>
+  <si>
+    <t>https://github.com/ctroein/octavvs</t>
   </si>
 </sst>
 </file>
@@ -2316,12 +2334,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4560,6 +4578,46 @@
         <v>472</v>
       </c>
     </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>474</v>
+      </c>
+      <c r="B105" t="s">
+        <v>475</v>
+      </c>
+      <c r="C105" t="s">
+        <v>475</v>
+      </c>
+      <c r="E105" t="s">
+        <v>430</v>
+      </c>
+      <c r="F105" t="s">
+        <v>476</v>
+      </c>
+      <c r="G105" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>478</v>
+      </c>
+      <c r="B106" t="s">
+        <v>479</v>
+      </c>
+      <c r="C106" t="s">
+        <v>479</v>
+      </c>
+      <c r="E106" t="s">
+        <v>430</v>
+      </c>
+      <c r="F106" t="s">
+        <v>476</v>
+      </c>
+      <c r="G106" t="s">
+        <v>477</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B46" r:id="rId1" display="https://cran.r-project.org/package=pavo" xr:uid="{3E292708-18D0-1C48-B810-34D638D0D26E}"/>

</xml_diff>

<commit_message>
add library(xlm2) trying to fix missing as_list
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AE0ED4-070E-FC45-B0E9-985468EF2184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9ABBCF-EABD-8E4F-8372-A1CCE0C8E6B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26240" yWindow="1200" windowWidth="22640" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOSS4Spec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="486">
   <si>
     <t>name</t>
   </si>
@@ -1469,6 +1469,15 @@
   </si>
   <si>
     <t>General purpose running on Orange</t>
+  </si>
+  <si>
+    <t>https://github.com/chatcannon/pytnt</t>
+  </si>
+  <si>
+    <t>pytnt</t>
+  </si>
+  <si>
+    <t>Read files from TecMag NMR instruments</t>
   </si>
 </sst>
 </file>
@@ -2343,12 +2352,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G107" sqref="G107"/>
+      <selection pane="bottomLeft" activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4647,6 +4656,26 @@
         <v>258</v>
       </c>
     </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>484</v>
+      </c>
+      <c r="B108" t="s">
+        <v>483</v>
+      </c>
+      <c r="C108" t="s">
+        <v>483</v>
+      </c>
+      <c r="E108" t="s">
+        <v>430</v>
+      </c>
+      <c r="F108" t="s">
+        <v>485</v>
+      </c>
+      <c r="G108" t="s">
+        <v>219</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B46" r:id="rId1" display="https://cran.r-project.org/package=pavo" xr:uid="{3E292708-18D0-1C48-B810-34D638D0D26E}"/>

</xml_diff>

<commit_message>
make focus tags consistent
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D495344-A7EA-D74E-971D-8F2BF6F019BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EB9C9A-E1AE-284A-B635-90B6E073DA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="22660" windowHeight="9340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="582">
   <si>
     <t>name</t>
   </si>
@@ -1718,9 +1718,6 @@
   </si>
   <si>
     <t>Dereplication of natural product 2D NMR spectra</t>
-  </si>
-  <si>
-    <t>2DNMR</t>
   </si>
   <si>
     <t>https://pubs.acs.org/doi/10.1021/acs.jnatprod.0c01076</t>
@@ -2168,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5323,13 +5320,13 @@
         <v>564</v>
       </c>
       <c r="B122" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C122" t="s">
         <v>563</v>
       </c>
       <c r="D122" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E122" t="s">
         <v>38</v>
@@ -5338,27 +5335,27 @@
         <v>565</v>
       </c>
       <c r="G122" t="s">
-        <v>566</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>568</v>
+      </c>
+      <c r="B123" t="s">
+        <v>11</v>
+      </c>
+      <c r="C123" t="s">
         <v>569</v>
       </c>
-      <c r="B123" t="s">
-        <v>11</v>
-      </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
+        <v>571</v>
+      </c>
+      <c r="E123" t="s">
+        <v>38</v>
+      </c>
+      <c r="F123" t="s">
         <v>570</v>
-      </c>
-      <c r="D123" t="s">
-        <v>572</v>
-      </c>
-      <c r="E123" t="s">
-        <v>38</v>
-      </c>
-      <c r="F123" t="s">
-        <v>571</v>
       </c>
       <c r="G123" t="s">
         <v>147</v>
@@ -5366,45 +5363,45 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>574</v>
+      </c>
+      <c r="B124" t="s">
+        <v>576</v>
+      </c>
+      <c r="C124" t="s">
+        <v>572</v>
+      </c>
+      <c r="D124" t="s">
         <v>575</v>
-      </c>
-      <c r="B124" t="s">
-        <v>577</v>
-      </c>
-      <c r="C124" t="s">
-        <v>573</v>
-      </c>
-      <c r="D124" t="s">
-        <v>576</v>
       </c>
       <c r="E124" t="s">
         <v>12</v>
       </c>
       <c r="F124" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G124" t="s">
-        <v>566</v>
+        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B125" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C125" t="s">
+        <v>579</v>
+      </c>
+      <c r="D125" t="s">
         <v>580</v>
-      </c>
-      <c r="D125" t="s">
-        <v>581</v>
       </c>
       <c r="E125" t="s">
         <v>12</v>
       </c>
       <c r="F125" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G125" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
add to database; fix links
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9966A5B6-B8CF-3F4E-9C93-1B21114654E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D702AF0C-65FC-8545-8402-2E2847B46D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="22660" windowHeight="9340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="617">
   <si>
     <t>name</t>
   </si>
@@ -1781,6 +1781,96 @@
   </si>
   <si>
     <t>Taha Ahmed &lt;taha@chepec.se&gt;</t>
+  </si>
+  <si>
+    <t>ANSURR</t>
+  </si>
+  <si>
+    <t>https://github.com/nickjf/ANSURR2</t>
+  </si>
+  <si>
+    <t>Validate accuracy of protein NMR structures</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41467-020-20177-1</t>
+  </si>
+  <si>
+    <t>nmr-parser</t>
+  </si>
+  <si>
+    <t>https://github.com/cheminfo/nmr-parser</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Parse 1D &amp; 2D NMR files to JSON</t>
+  </si>
+  <si>
+    <t>nmrgnn</t>
+  </si>
+  <si>
+    <t>https://github.com/ur-whitelab/nmrgnn</t>
+  </si>
+  <si>
+    <t>Graph neural network prediction of NMR shifts</t>
+  </si>
+  <si>
+    <t>https://pubs.rsc.org/en/content/articlehtml/2021/sc/d1sc01895g</t>
+  </si>
+  <si>
+    <t>cwepr</t>
+  </si>
+  <si>
+    <t>https://docs.cwepr.de/v0.2/</t>
+  </si>
+  <si>
+    <t>https://github.com/tillbiskup/cwepr</t>
+  </si>
+  <si>
+    <t>Processing continuous wave EPR data</t>
+  </si>
+  <si>
+    <t>EPR</t>
+  </si>
+  <si>
+    <t>ASpecD</t>
+  </si>
+  <si>
+    <t>https://www.aspecd.de/public/index</t>
+  </si>
+  <si>
+    <t>https://github.com/tillbiskup/aspecd</t>
+  </si>
+  <si>
+    <t>General handling of spectroscopic data</t>
+  </si>
+  <si>
+    <t>trEPR</t>
+  </si>
+  <si>
+    <t>Time-resolved EPR spectroscopy</t>
+  </si>
+  <si>
+    <t>https://github.com/tillbiskup/trepr</t>
+  </si>
+  <si>
+    <t>https://docs.trepr.de/v0.2/index.html</t>
+  </si>
+  <si>
+    <t>NMR-EsPy</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1090780722000313</t>
+  </si>
+  <si>
+    <t>https://github.com/foroozandehgroup/NMR-EsPy</t>
+  </si>
+  <si>
+    <t>https://foroozandehgroup.github.io/NMR-EsPy/</t>
+  </si>
+  <si>
+    <t>Estimation of NMR parameters</t>
   </si>
 </sst>
 </file>
@@ -2178,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D116" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H126" sqref="H126"/>
+    <sheetView tabSelected="1" topLeftCell="B127" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5443,6 +5533,155 @@
       </c>
       <c r="H126" t="s">
         <v>586</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>587</v>
+      </c>
+      <c r="B127" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127" t="s">
+        <v>588</v>
+      </c>
+      <c r="D127" t="s">
+        <v>590</v>
+      </c>
+      <c r="E127" t="s">
+        <v>38</v>
+      </c>
+      <c r="F127" t="s">
+        <v>589</v>
+      </c>
+      <c r="G127" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>591</v>
+      </c>
+      <c r="B128" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" t="s">
+        <v>592</v>
+      </c>
+      <c r="E128" t="s">
+        <v>593</v>
+      </c>
+      <c r="F128" t="s">
+        <v>594</v>
+      </c>
+      <c r="G128" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>595</v>
+      </c>
+      <c r="B129" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" t="s">
+        <v>596</v>
+      </c>
+      <c r="D129" t="s">
+        <v>598</v>
+      </c>
+      <c r="E129" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" t="s">
+        <v>597</v>
+      </c>
+      <c r="G129" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>599</v>
+      </c>
+      <c r="B130" t="s">
+        <v>600</v>
+      </c>
+      <c r="C130" t="s">
+        <v>601</v>
+      </c>
+      <c r="E130" t="s">
+        <v>38</v>
+      </c>
+      <c r="F130" t="s">
+        <v>602</v>
+      </c>
+      <c r="G130" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>604</v>
+      </c>
+      <c r="B131" t="s">
+        <v>605</v>
+      </c>
+      <c r="C131" t="s">
+        <v>606</v>
+      </c>
+      <c r="E131" t="s">
+        <v>38</v>
+      </c>
+      <c r="F131" t="s">
+        <v>607</v>
+      </c>
+      <c r="G131" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>608</v>
+      </c>
+      <c r="B132" t="s">
+        <v>611</v>
+      </c>
+      <c r="C132" t="s">
+        <v>610</v>
+      </c>
+      <c r="E132" t="s">
+        <v>38</v>
+      </c>
+      <c r="F132" t="s">
+        <v>609</v>
+      </c>
+      <c r="G132" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>612</v>
+      </c>
+      <c r="B133" t="s">
+        <v>615</v>
+      </c>
+      <c r="C133" t="s">
+        <v>614</v>
+      </c>
+      <c r="D133" t="s">
+        <v>613</v>
+      </c>
+      <c r="E133" t="s">
+        <v>38</v>
+      </c>
+      <c r="F133" t="s">
+        <v>616</v>
+      </c>
+      <c r="G133" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
many new entries; only name, repo, desc so far
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_teic01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FDAC3B-3271-4830-91FD-E97389CBF17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17106717-E54E-1F41-8D75-1C5035889185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DF" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="706">
   <si>
     <t>name</t>
   </si>
@@ -1883,6 +1883,261 @@
   </si>
   <si>
     <t>ir</t>
+  </si>
+  <si>
+    <t>PALMA</t>
+  </si>
+  <si>
+    <t>rampy</t>
+  </si>
+  <si>
+    <t>raman</t>
+  </si>
+  <si>
+    <t>Spectra.jl</t>
+  </si>
+  <si>
+    <t>BaselineRemoval</t>
+  </si>
+  <si>
+    <t>py-wdf-reader</t>
+  </si>
+  <si>
+    <t>specio</t>
+  </si>
+  <si>
+    <t>Raman-and-SERS-Processing</t>
+  </si>
+  <si>
+    <t>raman-fitting</t>
+  </si>
+  <si>
+    <t>raman-cnn</t>
+  </si>
+  <si>
+    <t>rCRSI</t>
+  </si>
+  <si>
+    <t>ramkit</t>
+  </si>
+  <si>
+    <t>spectroscopy</t>
+  </si>
+  <si>
+    <t>ASPIRED</t>
+  </si>
+  <si>
+    <t>spectrophotometry</t>
+  </si>
+  <si>
+    <t>AutomatedLIBS</t>
+  </si>
+  <si>
+    <t>LIBS</t>
+  </si>
+  <si>
+    <t>pyDichroX</t>
+  </si>
+  <si>
+    <t>https://github.com/delsuc/PALMA</t>
+  </si>
+  <si>
+    <t>https://github.com/DerekKaknes/raman</t>
+  </si>
+  <si>
+    <t>https://github.com/StatguyUser/BaselineRemoval</t>
+  </si>
+  <si>
+    <t>https://github.com/alchem0x2A/py-wdf-reader</t>
+  </si>
+  <si>
+    <t>https://github.com/paris-saclay-cds/specio</t>
+  </si>
+  <si>
+    <t>https://github.com/MarjorieRWillner/Raman-and-SERS-Processing</t>
+  </si>
+  <si>
+    <t>https://github.com/MyPyDavid/raman-fitting</t>
+  </si>
+  <si>
+    <t>https://github.com/rjkilpatrick/raman-cnn</t>
+  </si>
+  <si>
+    <t>https://github.com/niemingzhao/ramkit</t>
+  </si>
+  <si>
+    <t>https://github.com/Cambridge-PAM/spectroscopy</t>
+  </si>
+  <si>
+    <t>https://github.com/cylammarco/ASPIRED</t>
+  </si>
+  <si>
+    <t>https://github.com/lhosszu/spectrophotometry</t>
+  </si>
+  <si>
+    <t>https://github.com/mrDIMAS/AutomatedLIBS</t>
+  </si>
+  <si>
+    <t>https://github.com/jason-r-becker/LIBS</t>
+  </si>
+  <si>
+    <t>https://github.com/BeppeC/pyDichroX</t>
+  </si>
+  <si>
+    <t>DNPLab</t>
+  </si>
+  <si>
+    <t>jcamp-dx</t>
+  </si>
+  <si>
+    <t>spectrochempy</t>
+  </si>
+  <si>
+    <t>DeerLab</t>
+  </si>
+  <si>
+    <t>customxepr</t>
+  </si>
+  <si>
+    <t>hanlab</t>
+  </si>
+  <si>
+    <t>spa-on-python</t>
+  </si>
+  <si>
+    <t>nira</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>nmrium</t>
+  </si>
+  <si>
+    <t>FarSeer-NMR</t>
+  </si>
+  <si>
+    <t>spike</t>
+  </si>
+  <si>
+    <t>https://github.com/DNPLab/DNPLab</t>
+  </si>
+  <si>
+    <t>https://github.com/fracpete/jcamp-dx</t>
+  </si>
+  <si>
+    <t>https://github.com/JeschkeLab/DeerLab</t>
+  </si>
+  <si>
+    <t>https://github.com/OE-FET/customxepr</t>
+  </si>
+  <si>
+    <t>https://github.com/thcasey3/hanlab</t>
+  </si>
+  <si>
+    <t>https://github.com/lerkoah/spa-on-python</t>
+  </si>
+  <si>
+    <t>https://github.com/admedeiros/nira</t>
+  </si>
+  <si>
+    <t>https://github.com/jwist/coffee</t>
+  </si>
+  <si>
+    <t>https://github.com/cheminfo/nmrium</t>
+  </si>
+  <si>
+    <t>https://github.com/spike-project/spike</t>
+  </si>
+  <si>
+    <t>DNPLab - Bringing the power of Python to DNP-NMR Spectroscopy</t>
+  </si>
+  <si>
+    <t>Reference implemention of the IUPAC JCAMP-DX spectroscopy data standard. Fork of https://sourceforge.net/projects/jcamp-dx/</t>
+  </si>
+  <si>
+    <t>SpectroChemPy is a framework for processing, analyzing and modeling spectroscopic data for chemistry with Python</t>
+  </si>
+  <si>
+    <t>Python package for data analysis for dipolar EPR spectroscopy</t>
+  </si>
+  <si>
+    <t>Instrument control suite for Bruker E500, MercuryiTC and Keithley 2600.</t>
+  </si>
+  <si>
+    <t>code used to process, fit, and analyze various types of DNP, NMR, and EPR data generated in the lab of Songi Han at UCSB</t>
+  </si>
+  <si>
+    <t>Read Nicolet/Thermo Omnic files on python (.spa).</t>
+  </si>
+  <si>
+    <t>Near-Infrared Analysis</t>
+  </si>
+  <si>
+    <t>Datasets of metabolic profiles of coffees from different species and origin</t>
+  </si>
+  <si>
+    <t>React component to display and process nuclear magnetic resonance (NMR) spectra.</t>
+  </si>
+  <si>
+    <t>A software suite for automatic treatment, analysis and plotting of large and multivariable datasets of bioNMR peaklists.</t>
+  </si>
+  <si>
+    <t>SPIKE a collaborative development for a FT-spectroscopy processing program.</t>
+  </si>
+  <si>
+    <t>repository associated with manuscript "PALMA, an improved algorithm for DOSY signal processing"</t>
+  </si>
+  <si>
+    <t>Python software for spectral data processing (IR, Raman, XAS...)</t>
+  </si>
+  <si>
+    <t>Deep CNN for Raman Applications</t>
+  </si>
+  <si>
+    <t>Spectra.jl aims at helping treatment of spectral (Raman, Infrared, XAS, NMR) data under the Julia language</t>
+  </si>
+  <si>
+    <t>Perform baseline removal, baseline correction and baseline substraction for raman spectra using Modpoly, ImodPoly and Zhang fit. Returns baseline-subtracted spectrum</t>
+  </si>
+  <si>
+    <t>Python package for read-only accessing the wdf Raman spectroscopy from Ranishaw WiRE software</t>
+  </si>
+  <si>
+    <t>specio: Python input/output for spectroscopic files</t>
+  </si>
+  <si>
+    <t>Code for processing either Raman or SERS maps. Includes baseline correction, peak comparison, and post processing anaylsis.</t>
+  </si>
+  <si>
+    <t>A Python framework for the batch processing and deconvolution of Raman spectra of carbonaceous materials.</t>
+  </si>
+  <si>
+    <t>Neural network classifier for Raman spectral data using TensorFlow</t>
+  </si>
+  <si>
+    <t>Visualitzation and processing toolbox for Confocal Raman Spectroscopy Imaging</t>
+  </si>
+  <si>
+    <t>An analysis kernel for raman spectrum.</t>
+  </si>
+  <si>
+    <t>Jupyter Notebooks for spectroscopic data processing</t>
+  </si>
+  <si>
+    <t>Automated SpectroPhotometric Image REDuction (ASPIRED)</t>
+  </si>
+  <si>
+    <t>An Android application for controlling a Bluetooth spectrophotometer (ESP32 &amp; C12880MA)</t>
+  </si>
+  <si>
+    <t>Laser-Induced Break Down Spectroscopy spectra analysis software</t>
+  </si>
+  <si>
+    <t>Analysis codes for Laser-Induced Breakdown Spectroscopy data</t>
+  </si>
+  <si>
+    <t>Program to analyse XAS data</t>
   </si>
 </sst>
 </file>
@@ -1943,8 +2198,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1960,7 +2215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2280,27 +2535,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
-    <col min="6" max="6" width="100.77734375" customWidth="1"/>
-    <col min="7" max="7" width="23.77734375" customWidth="1"/>
-    <col min="8" max="8" width="60.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="100.83203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="60.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2326,7 +2581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2352,7 +2607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2378,7 +2633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2404,7 +2659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2430,7 +2685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -2456,7 +2711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -2482,7 +2737,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2508,7 +2763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2534,7 +2789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2560,7 +2815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -2586,7 +2841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -2612,7 +2867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2638,7 +2893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -2664,7 +2919,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -2690,7 +2945,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -2716,7 +2971,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -2742,7 +2997,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -2768,7 +3023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2794,7 +3049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -2820,7 +3075,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -2846,7 +3101,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -2872,7 +3127,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>119</v>
       </c>
@@ -2898,7 +3153,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -2924,7 +3179,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>129</v>
       </c>
@@ -2950,7 +3205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -2976,7 +3231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3002,7 +3257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>143</v>
       </c>
@@ -3028,7 +3283,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -3054,7 +3309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -3080,7 +3335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>156</v>
       </c>
@@ -3106,7 +3361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -3132,7 +3387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -3158,7 +3413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>169</v>
       </c>
@@ -3184,7 +3439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -3210,7 +3465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>179</v>
       </c>
@@ -3236,7 +3491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -3262,7 +3517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>187</v>
       </c>
@@ -3288,7 +3543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>192</v>
       </c>
@@ -3314,7 +3569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>196</v>
       </c>
@@ -3340,7 +3595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>199</v>
       </c>
@@ -3366,7 +3621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>204</v>
       </c>
@@ -3392,7 +3647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>209</v>
       </c>
@@ -3418,7 +3673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>213</v>
       </c>
@@ -3444,7 +3699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>216</v>
       </c>
@@ -3470,7 +3725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>221</v>
       </c>
@@ -3496,7 +3751,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>227</v>
       </c>
@@ -3522,7 +3777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>232</v>
       </c>
@@ -3548,7 +3803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>235</v>
       </c>
@@ -3574,7 +3829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>239</v>
       </c>
@@ -3600,7 +3855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>245</v>
       </c>
@@ -3626,7 +3881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>250</v>
       </c>
@@ -3652,7 +3907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>257</v>
       </c>
@@ -3678,7 +3933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>262</v>
       </c>
@@ -3704,7 +3959,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>267</v>
       </c>
@@ -3730,7 +3985,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>271</v>
       </c>
@@ -3756,7 +4011,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>276</v>
       </c>
@@ -3782,7 +4037,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>282</v>
       </c>
@@ -3808,7 +4063,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>288</v>
       </c>
@@ -3834,7 +4089,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>293</v>
       </c>
@@ -3860,7 +4115,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>298</v>
       </c>
@@ -3886,7 +4141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>302</v>
       </c>
@@ -3912,7 +4167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>306</v>
       </c>
@@ -3938,7 +4193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>310</v>
       </c>
@@ -3964,7 +4219,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>315</v>
       </c>
@@ -3990,7 +4245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>320</v>
       </c>
@@ -4016,7 +4271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>324</v>
       </c>
@@ -4042,7 +4297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>327</v>
       </c>
@@ -4068,7 +4323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>331</v>
       </c>
@@ -4094,7 +4349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>336</v>
       </c>
@@ -4120,7 +4375,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>341</v>
       </c>
@@ -4146,7 +4401,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>346</v>
       </c>
@@ -4172,7 +4427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>350</v>
       </c>
@@ -4198,7 +4453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>353</v>
       </c>
@@ -4224,7 +4479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>358</v>
       </c>
@@ -4250,7 +4505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>361</v>
       </c>
@@ -4276,7 +4531,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>366</v>
       </c>
@@ -4302,7 +4557,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>370</v>
       </c>
@@ -4328,7 +4583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>376</v>
       </c>
@@ -4354,7 +4609,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>381</v>
       </c>
@@ -4380,7 +4635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>385</v>
       </c>
@@ -4406,7 +4661,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>389</v>
       </c>
@@ -4432,7 +4687,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>393</v>
       </c>
@@ -4458,7 +4713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>396</v>
       </c>
@@ -4484,7 +4739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>400</v>
       </c>
@@ -4510,7 +4765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>405</v>
       </c>
@@ -4536,7 +4791,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>410</v>
       </c>
@@ -4562,7 +4817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>414</v>
       </c>
@@ -4588,7 +4843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>418</v>
       </c>
@@ -4614,7 +4869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>422</v>
       </c>
@@ -4640,7 +4895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>426</v>
       </c>
@@ -4666,7 +4921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>431</v>
       </c>
@@ -4692,7 +4947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>437</v>
       </c>
@@ -4718,7 +4973,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>441</v>
       </c>
@@ -4744,7 +4999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>444</v>
       </c>
@@ -4770,7 +5025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>448</v>
       </c>
@@ -4796,7 +5051,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>453</v>
       </c>
@@ -4822,7 +5077,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>458</v>
       </c>
@@ -4848,7 +5103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>462</v>
       </c>
@@ -4874,7 +5129,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>466</v>
       </c>
@@ -4900,7 +5155,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>470</v>
       </c>
@@ -4926,7 +5181,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>475</v>
       </c>
@@ -4952,7 +5207,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>480</v>
       </c>
@@ -4978,7 +5233,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>487</v>
       </c>
@@ -5004,7 +5259,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>493</v>
       </c>
@@ -5030,7 +5285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>497</v>
       </c>
@@ -5056,7 +5311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>499</v>
       </c>
@@ -5082,7 +5337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>502</v>
       </c>
@@ -5108,7 +5363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>505</v>
       </c>
@@ -5134,7 +5389,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>509</v>
       </c>
@@ -5160,7 +5415,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>512</v>
       </c>
@@ -5186,7 +5441,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>518</v>
       </c>
@@ -5212,7 +5467,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>523</v>
       </c>
@@ -5238,7 +5493,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>521</v>
       </c>
@@ -5264,7 +5519,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>532</v>
       </c>
@@ -5290,7 +5545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>536</v>
       </c>
@@ -5316,7 +5571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>540</v>
       </c>
@@ -5342,7 +5597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>545</v>
       </c>
@@ -5368,7 +5623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>551</v>
       </c>
@@ -5388,7 +5643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>552</v>
       </c>
@@ -5411,7 +5666,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>558</v>
       </c>
@@ -5434,7 +5689,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>564</v>
       </c>
@@ -5457,7 +5712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>568</v>
       </c>
@@ -5480,7 +5735,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>574</v>
       </c>
@@ -5503,7 +5758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>577</v>
       </c>
@@ -5526,7 +5781,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>584</v>
       </c>
@@ -5549,7 +5804,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>587</v>
       </c>
@@ -5572,7 +5827,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>591</v>
       </c>
@@ -5592,7 +5847,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>595</v>
       </c>
@@ -5615,7 +5870,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>599</v>
       </c>
@@ -5635,7 +5890,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>604</v>
       </c>
@@ -5655,7 +5910,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>608</v>
       </c>
@@ -5675,7 +5930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>612</v>
       </c>
@@ -5698,7 +5953,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>620</v>
       </c>
@@ -5722,6 +5977,336 @@
       </c>
       <c r="H134" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>654</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="F135" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>655</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="F136" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>656</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F137" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>657</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="F138" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>658</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="F139" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>659</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="F140" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>660</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="F141" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>661</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="F142" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>662</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="F143" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>663</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="F144" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>664</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F145" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>665</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="F146" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>621</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="F147" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>622</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F148" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>623</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="F149" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>624</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F150" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>625</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F151" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>626</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="F152" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>627</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="F153" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>628</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="F154" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>629</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="F155" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>630</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="F156" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>631</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="F157" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>632</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="F158" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>633</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="F159" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>634</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="F160" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>635</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="F161" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>636</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="F162" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>637</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="F163" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>638</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="F164" t="s">
+        <v>705</v>
       </c>
     </row>
   </sheetData>
@@ -5988,6 +6573,36 @@
     <hyperlink ref="D117" r:id="rId260" location="!divAbstract" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
     <hyperlink ref="B118" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
     <hyperlink ref="C118" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="C135" r:id="rId263" xr:uid="{185FB0CC-1BFF-5145-BEB3-72BDF47C8947}"/>
+    <hyperlink ref="C136" r:id="rId264" xr:uid="{97A80B27-831C-6549-8311-FA687785EA30}"/>
+    <hyperlink ref="C137" r:id="rId265" xr:uid="{C6C180D4-D87A-4D48-8817-ABD91B6243AD}"/>
+    <hyperlink ref="C138" r:id="rId266" xr:uid="{F4F61C2C-C1F7-7147-8DAC-F04A10994944}"/>
+    <hyperlink ref="C139" r:id="rId267" xr:uid="{1E329ECB-8E96-9C44-BFA1-914822245AD5}"/>
+    <hyperlink ref="C141" r:id="rId268" xr:uid="{6D6FADB7-CFCB-EF42-B4C8-5A772019679B}"/>
+    <hyperlink ref="C142" r:id="rId269" xr:uid="{2A87F5BC-C340-6149-B12F-3F9425A0527B}"/>
+    <hyperlink ref="C143" r:id="rId270" xr:uid="{D0E7A090-9133-1442-A80D-229E6F82D51F}"/>
+    <hyperlink ref="C144" r:id="rId271" xr:uid="{2407433B-D83D-2742-B1C3-CF65FF93283D}"/>
+    <hyperlink ref="C145" r:id="rId272" xr:uid="{D918A6CC-4DE8-5749-B396-C5BE2178FEAC}"/>
+    <hyperlink ref="C146" r:id="rId273" xr:uid="{993B79A8-C154-C64D-AAA1-BA2D47F20826}"/>
+    <hyperlink ref="C147" r:id="rId274" xr:uid="{42BB3483-8CC1-E142-BE62-922281DD72B0}"/>
+    <hyperlink ref="C148" r:id="rId275" xr:uid="{CADE7398-4579-394B-8CCD-E2C7CC0E02E7}"/>
+    <hyperlink ref="C149" r:id="rId276" xr:uid="{17D20192-38F2-2344-AC9A-F1DF646DA898}"/>
+    <hyperlink ref="C150" r:id="rId277" xr:uid="{F748A52A-20AD-7D4D-ADFF-FF4E6B3B904F}"/>
+    <hyperlink ref="C151" r:id="rId278" xr:uid="{BDA7CC67-1472-8248-946E-93B6F618685B}"/>
+    <hyperlink ref="C152" r:id="rId279" xr:uid="{EA63AAC0-2987-5B4D-8CA8-F8E8B820ED36}"/>
+    <hyperlink ref="C153" r:id="rId280" xr:uid="{A66AC424-A7F4-B84A-9280-820A43B4AEBA}"/>
+    <hyperlink ref="C154" r:id="rId281" xr:uid="{64547E34-44D9-1848-AAA7-1C3BBB7DB2D9}"/>
+    <hyperlink ref="C155" r:id="rId282" xr:uid="{E7A6808E-50F2-0948-9C94-628B4F9ACF7D}"/>
+    <hyperlink ref="C156" r:id="rId283" xr:uid="{0B5221E8-DE05-0E4E-9EE3-DCADE66F2696}"/>
+    <hyperlink ref="C157" r:id="rId284" xr:uid="{EA1D837B-5F6A-B54C-9B61-2034B0CE85B3}"/>
+    <hyperlink ref="C158" r:id="rId285" xr:uid="{A3994F4F-3387-1942-A3D6-B8B67EB06BC1}"/>
+    <hyperlink ref="C159" r:id="rId286" xr:uid="{B8D152B1-8B72-E74D-88F6-C43A49A5AB2F}"/>
+    <hyperlink ref="C160" r:id="rId287" xr:uid="{6964114A-F58F-724D-A2B4-173388BA5302}"/>
+    <hyperlink ref="C161" r:id="rId288" xr:uid="{0BC4DD0E-7FEB-0D4D-A81D-6609730F3270}"/>
+    <hyperlink ref="C162" r:id="rId289" xr:uid="{3BD56E0B-D3CE-AD4D-91FA-51D4543B137E}"/>
+    <hyperlink ref="C163" r:id="rId290" xr:uid="{23A75913-BCC4-4E47-9B47-B952CD9112B4}"/>
+    <hyperlink ref="C164" r:id="rId291" xr:uid="{60B2A7C5-DB9E-5F41-B146-74A96ECCE834}"/>
+    <hyperlink ref="C140" r:id="rId292" xr:uid="{F7F12410-9273-7F45-805B-07CE4BFEB9E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
clean up forgotten changes
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2900E926-D0B5-6C49-8D79-DB9D2033FE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABAACE2-6E1B-C54C-8B25-2BAE3210B52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1020" windowWidth="23700" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5240" yWindow="700" windowWidth="23700" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DF" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1112">
   <si>
     <t>name</t>
   </si>
@@ -3344,6 +3344,18 @@
   </si>
   <si>
     <t>https://www.openanalysis.org/openspecy</t>
+  </si>
+  <si>
+    <t>NMRTools</t>
+  </si>
+  <si>
+    <t>https://juliapackages.com/p/nmrtools</t>
+  </si>
+  <si>
+    <t>https://github.com/chriswaudby/NMRTools.jl</t>
+  </si>
+  <si>
+    <t>Import and plot NMR spectra</t>
   </si>
 </sst>
 </file>
@@ -3750,12 +3762,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H245"/>
+  <dimension ref="A1:H246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
+      <selection pane="bottomLeft" activeCell="E246" sqref="E246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10015,6 +10027,29 @@
       </c>
       <c r="H245" t="s">
         <v>1085</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B246" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C246" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D246" t="s">
+        <v>11</v>
+      </c>
+      <c r="E246" t="s">
+        <v>370</v>
+      </c>
+      <c r="F246" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G246" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add rchemo & Jchemo
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABAACE2-6E1B-C54C-8B25-2BAE3210B52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F42ADA4-E094-AA44-A8A6-5A4834AD2407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="700" windowWidth="23700" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="700" windowWidth="23700" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DF" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="1119">
   <si>
     <t>name</t>
   </si>
@@ -3356,6 +3356,27 @@
   </si>
   <si>
     <t>Import and plot NMR spectra</t>
+  </si>
+  <si>
+    <t>https://github.com/mlesnoff/rchemo</t>
+  </si>
+  <si>
+    <t>matthieu.lesnoff@cirad.fr</t>
+  </si>
+  <si>
+    <t>Dimension reduction, regression and discrimination for chemometrics</t>
+  </si>
+  <si>
+    <t>rchemo</t>
+  </si>
+  <si>
+    <t>https://github.com/mlesnoff/Jchemo.jl</t>
+  </si>
+  <si>
+    <t>Jchemo</t>
+  </si>
+  <si>
+    <t>https://analyticalsciencejournals.onlinelibrary.wiley.com/doi/10.1002/cem.3209</t>
   </si>
 </sst>
 </file>
@@ -3762,12 +3783,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H246"/>
+  <dimension ref="A1:H248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E246" sqref="E246"/>
+      <selection pane="bottomLeft" activeCell="B248" sqref="B248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10050,6 +10071,58 @@
       </c>
       <c r="G246" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B247" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C247" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D247" t="s">
+        <v>11</v>
+      </c>
+      <c r="E247" t="s">
+        <v>12</v>
+      </c>
+      <c r="F247" t="s">
+        <v>1114</v>
+      </c>
+      <c r="G247" t="s">
+        <v>13</v>
+      </c>
+      <c r="H247" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B248" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C248" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D248" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E248" t="s">
+        <v>370</v>
+      </c>
+      <c r="F248" t="s">
+        <v>1114</v>
+      </c>
+      <c r="G248" t="s">
+        <v>13</v>
+      </c>
+      <c r="H248" t="s">
+        <v>1113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed duplicate entry Spectra.jl
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanhanson/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F42ADA4-E094-AA44-A8A6-5A4834AD2407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B44FFA-7F01-F748-9546-1AC73F29385B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="700" windowWidth="23700" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="1117">
   <si>
     <t>name</t>
   </si>
@@ -1729,9 +1729,6 @@
     <t>PALMA</t>
   </si>
   <si>
-    <t>Spectra.jl</t>
-  </si>
-  <si>
     <t>BaselineRemoval</t>
   </si>
   <si>
@@ -1910,9 +1907,6 @@
   </si>
   <si>
     <t>DOSY signal processing</t>
-  </si>
-  <si>
-    <t>Treatment of spectral (Raman, Infrared, XAS, NMR) data</t>
   </si>
   <si>
     <t>https://specio.readthedocs.io/en/stable/</t>
@@ -3783,12 +3777,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H248"/>
+  <dimension ref="A1:H247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B248" sqref="B248"/>
+      <selection pane="bottomLeft" activeCell="A135" sqref="A135:XFD135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3846,7 +3840,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -3872,7 +3866,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
@@ -4002,7 +3996,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="G8" t="s">
         <v>338</v>
@@ -4135,7 +4129,7 @@
         <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="H13" t="s">
         <v>68</v>
@@ -4161,7 +4155,7 @@
         <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="H14" t="s">
         <v>73</v>
@@ -4187,7 +4181,7 @@
         <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="H15" t="s">
         <v>73</v>
@@ -4210,7 +4204,7 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
@@ -4340,7 +4334,7 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="G21" t="s">
         <v>31</v>
@@ -4366,7 +4360,7 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="G22" t="s">
         <v>107</v>
@@ -4421,7 +4415,7 @@
         <v>116</v>
       </c>
       <c r="G24" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="H24" t="s">
         <v>117</v>
@@ -4444,7 +4438,7 @@
         <v>36</v>
       </c>
       <c r="F25" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="G25" t="s">
         <v>122</v>
@@ -4785,7 +4779,7 @@
         <v>194</v>
       </c>
       <c r="G38" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="H38" t="s">
         <v>11</v>
@@ -4808,7 +4802,7 @@
         <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="G39" t="s">
         <v>198</v>
@@ -5071,7 +5065,7 @@
         <v>245</v>
       </c>
       <c r="G49" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="H49" t="s">
         <v>246</v>
@@ -5198,7 +5192,7 @@
         <v>36</v>
       </c>
       <c r="F54" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="G54" t="s">
         <v>90</v>
@@ -5227,7 +5221,7 @@
         <v>274</v>
       </c>
       <c r="G55" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="H55" t="s">
         <v>11</v>
@@ -5435,7 +5429,7 @@
         <v>307</v>
       </c>
       <c r="G63" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="H63" t="s">
         <v>308</v>
@@ -5536,7 +5530,7 @@
         <v>36</v>
       </c>
       <c r="F67" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="G67" t="s">
         <v>31</v>
@@ -5588,7 +5582,7 @@
         <v>36</v>
       </c>
       <c r="F69" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="G69" t="s">
         <v>13</v>
@@ -5747,7 +5741,7 @@
         <v>358</v>
       </c>
       <c r="G75" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="H75" t="s">
         <v>11</v>
@@ -5929,7 +5923,7 @@
         <v>389</v>
       </c>
       <c r="G82" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="H82" t="s">
         <v>11</v>
@@ -5981,7 +5975,7 @@
         <v>399</v>
       </c>
       <c r="G84" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="H84" t="s">
         <v>11</v>
@@ -6007,7 +6001,7 @@
         <v>402</v>
       </c>
       <c r="G85" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="H85" t="s">
         <v>11</v>
@@ -6033,7 +6027,7 @@
         <v>405</v>
       </c>
       <c r="G86" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="H86" t="s">
         <v>11</v>
@@ -6160,7 +6154,7 @@
         <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="G91" t="s">
         <v>24</v>
@@ -6342,7 +6336,7 @@
         <v>36</v>
       </c>
       <c r="F98" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="G98" t="s">
         <v>13</v>
@@ -6371,7 +6365,7 @@
         <v>460</v>
       </c>
       <c r="G99" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="H99" t="s">
         <v>11</v>
@@ -6394,7 +6388,7 @@
         <v>12</v>
       </c>
       <c r="F100" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="G100" t="s">
         <v>13</v>
@@ -6420,7 +6414,7 @@
         <v>12</v>
       </c>
       <c r="F101" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="G101" t="s">
         <v>13</v>
@@ -6446,7 +6440,7 @@
         <v>12</v>
       </c>
       <c r="F102" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="G102" t="s">
         <v>135</v>
@@ -6602,7 +6596,7 @@
         <v>36</v>
       </c>
       <c r="F108" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="G108" t="s">
         <v>135</v>
@@ -6628,7 +6622,7 @@
         <v>12</v>
       </c>
       <c r="F109" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="G109" t="s">
         <v>13</v>
@@ -6654,7 +6648,7 @@
         <v>36</v>
       </c>
       <c r="F110" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="G110" t="s">
         <v>13</v>
@@ -6665,7 +6659,7 @@
         <v>503</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C111" t="s">
         <v>504</v>
@@ -6780,7 +6774,7 @@
         <v>526</v>
       </c>
       <c r="B116" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C116" t="s">
         <v>528</v>
@@ -6867,7 +6861,7 @@
         <v>542</v>
       </c>
       <c r="G119" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -6927,13 +6921,13 @@
         <v>554</v>
       </c>
       <c r="D122" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E122" t="s">
         <v>36</v>
       </c>
       <c r="F122" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="G122" t="s">
         <v>13</v>
@@ -7013,22 +7007,22 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B126" t="s">
+        <v>615</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="D126" t="s">
+        <v>11</v>
+      </c>
+      <c r="E126" t="s">
+        <v>36</v>
+      </c>
+      <c r="F126" t="s">
         <v>616</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="D126" t="s">
-        <v>11</v>
-      </c>
-      <c r="E126" t="s">
-        <v>36</v>
-      </c>
-      <c r="F126" t="s">
-        <v>617</v>
       </c>
       <c r="G126" t="s">
         <v>135</v>
@@ -7036,13 +7030,13 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D127" t="s">
         <v>11</v>
@@ -7051,7 +7045,7 @@
         <v>221</v>
       </c>
       <c r="F127" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G127" t="s">
         <v>338</v>
@@ -7059,13 +7053,13 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B128" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D128" t="s">
         <v>11</v>
@@ -7074,7 +7068,7 @@
         <v>36</v>
       </c>
       <c r="F128" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G128" t="s">
         <v>551</v>
@@ -7082,36 +7076,36 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B129" t="s">
+        <v>620</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D129" t="s">
+        <v>11</v>
+      </c>
+      <c r="E129" t="s">
+        <v>36</v>
+      </c>
+      <c r="F129" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G129" t="s">
         <v>621</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="D129" t="s">
-        <v>11</v>
-      </c>
-      <c r="E129" t="s">
-        <v>36</v>
-      </c>
-      <c r="F129" t="s">
-        <v>1043</v>
-      </c>
-      <c r="G129" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D130" t="s">
         <v>11</v>
@@ -7120,7 +7114,7 @@
         <v>12</v>
       </c>
       <c r="F130" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G130" t="s">
         <v>442</v>
@@ -7128,22 +7122,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B131" t="s">
+        <v>622</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="D131" t="s">
+        <v>11</v>
+      </c>
+      <c r="E131" t="s">
         <v>623</v>
       </c>
-      <c r="C131" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="D131" t="s">
-        <v>11</v>
-      </c>
-      <c r="E131" t="s">
-        <v>624</v>
-      </c>
       <c r="F131" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="G131" t="s">
         <v>135</v>
@@ -7151,10 +7145,10 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B132" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>302</v>
@@ -7166,7 +7160,7 @@
         <v>36</v>
       </c>
       <c r="F132" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G132" t="s">
         <v>135</v>
@@ -7174,22 +7168,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B133" t="s">
+        <v>625</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="D133" t="s">
+        <v>11</v>
+      </c>
+      <c r="E133" t="s">
+        <v>36</v>
+      </c>
+      <c r="F133" t="s">
         <v>626</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="D133" t="s">
-        <v>11</v>
-      </c>
-      <c r="E133" t="s">
-        <v>36</v>
-      </c>
-      <c r="F133" t="s">
-        <v>627</v>
       </c>
       <c r="G133" t="s">
         <v>135</v>
@@ -7200,19 +7194,19 @@
         <v>568</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D134" t="s">
+        <v>627</v>
+      </c>
+      <c r="E134" t="s">
+        <v>36</v>
+      </c>
+      <c r="F134" t="s">
         <v>628</v>
-      </c>
-      <c r="E134" t="s">
-        <v>36</v>
-      </c>
-      <c r="F134" t="s">
-        <v>629</v>
       </c>
       <c r="G134" t="s">
         <v>135</v>
@@ -7223,19 +7217,19 @@
         <v>569</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>369</v>
+        <v>582</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>369</v>
+        <v>582</v>
       </c>
       <c r="D135" t="s">
         <v>11</v>
       </c>
       <c r="E135" t="s">
-        <v>370</v>
+        <v>36</v>
       </c>
       <c r="F135" t="s">
-        <v>630</v>
+        <v>1043</v>
       </c>
       <c r="G135" t="s">
         <v>13</v>
@@ -7258,18 +7252,18 @@
         <v>36</v>
       </c>
       <c r="F136" t="s">
-        <v>1045</v>
+        <v>1028</v>
       </c>
       <c r="G136" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>571</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>584</v>
+      <c r="B137" t="s">
+        <v>629</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>584</v>
@@ -7281,18 +7275,18 @@
         <v>36</v>
       </c>
       <c r="F137" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="G137" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>572</v>
       </c>
-      <c r="B138" t="s">
-        <v>631</v>
+      <c r="B138" s="2" t="s">
+        <v>585</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>585</v>
@@ -7304,10 +7298,10 @@
         <v>36</v>
       </c>
       <c r="F138" t="s">
-        <v>1031</v>
+        <v>1044</v>
       </c>
       <c r="G138" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
@@ -7327,7 +7321,7 @@
         <v>36</v>
       </c>
       <c r="F139" t="s">
-        <v>1046</v>
+        <v>610</v>
       </c>
       <c r="G139" t="s">
         <v>107</v>
@@ -7338,19 +7332,19 @@
         <v>574</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>587</v>
+        <v>353</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>587</v>
+        <v>353</v>
       </c>
       <c r="D140" t="s">
         <v>11</v>
       </c>
       <c r="E140" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F140" t="s">
-        <v>611</v>
+        <v>630</v>
       </c>
       <c r="G140" t="s">
         <v>107</v>
@@ -7361,19 +7355,19 @@
         <v>575</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>353</v>
+        <v>587</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>353</v>
+        <v>587</v>
       </c>
       <c r="D141" t="s">
         <v>11</v>
       </c>
       <c r="E141" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F141" t="s">
-        <v>632</v>
+        <v>611</v>
       </c>
       <c r="G141" t="s">
         <v>107</v>
@@ -7396,10 +7390,10 @@
         <v>36</v>
       </c>
       <c r="F142" t="s">
-        <v>612</v>
+        <v>631</v>
       </c>
       <c r="G142" t="s">
-        <v>107</v>
+        <v>453</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
@@ -7413,16 +7407,16 @@
         <v>589</v>
       </c>
       <c r="D143" t="s">
-        <v>11</v>
+        <v>632</v>
       </c>
       <c r="E143" t="s">
         <v>36</v>
       </c>
       <c r="F143" t="s">
-        <v>633</v>
+        <v>612</v>
       </c>
       <c r="G143" t="s">
-        <v>453</v>
+        <v>198</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
@@ -7436,16 +7430,16 @@
         <v>590</v>
       </c>
       <c r="D144" t="s">
+        <v>11</v>
+      </c>
+      <c r="E144" t="s">
         <v>634</v>
-      </c>
-      <c r="E144" t="s">
-        <v>36</v>
       </c>
       <c r="F144" t="s">
         <v>613</v>
       </c>
       <c r="G144" t="s">
-        <v>198</v>
+        <v>579</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -7462,13 +7456,13 @@
         <v>11</v>
       </c>
       <c r="E145" t="s">
-        <v>636</v>
+        <v>36</v>
       </c>
       <c r="F145" t="s">
         <v>614</v>
       </c>
       <c r="G145" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -7488,21 +7482,21 @@
         <v>36</v>
       </c>
       <c r="F146" t="s">
-        <v>615</v>
+        <v>633</v>
       </c>
       <c r="G146" t="s">
-        <v>580</v>
+        <v>288</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>581</v>
+        <v>635</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>593</v>
+        <v>770</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>593</v>
+        <v>770</v>
       </c>
       <c r="D147" t="s">
         <v>11</v>
@@ -7511,21 +7505,24 @@
         <v>36</v>
       </c>
       <c r="F147" t="s">
-        <v>635</v>
+        <v>716</v>
       </c>
       <c r="G147" t="s">
-        <v>288</v>
+        <v>135</v>
+      </c>
+      <c r="H147" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D148" t="s">
         <v>11</v>
@@ -7534,24 +7531,24 @@
         <v>36</v>
       </c>
       <c r="F148" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="G148" t="s">
         <v>135</v>
       </c>
       <c r="H148" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>773</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
+      </c>
+      <c r="C149" t="s">
+        <v>918</v>
       </c>
       <c r="D149" t="s">
         <v>11</v>
@@ -7560,73 +7557,73 @@
         <v>36</v>
       </c>
       <c r="F149" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G149" t="s">
         <v>135</v>
       </c>
       <c r="H149" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C150" t="s">
-        <v>920</v>
+        <v>561</v>
       </c>
       <c r="D150" t="s">
-        <v>11</v>
+        <v>560</v>
       </c>
       <c r="E150" t="s">
         <v>36</v>
       </c>
       <c r="F150" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G150" t="s">
         <v>135</v>
       </c>
       <c r="H150" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C151" t="s">
-        <v>561</v>
+        <v>919</v>
       </c>
       <c r="D151" t="s">
-        <v>560</v>
+        <v>11</v>
       </c>
       <c r="E151" t="s">
         <v>36</v>
       </c>
       <c r="F151" t="s">
-        <v>721</v>
+        <v>1045</v>
       </c>
       <c r="G151" t="s">
         <v>135</v>
       </c>
       <c r="H151" t="s">
-        <v>852</v>
+        <v>920</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>776</v>
+        <v>128</v>
       </c>
       <c r="C152" t="s">
         <v>921</v>
@@ -7638,24 +7635,24 @@
         <v>36</v>
       </c>
       <c r="F152" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G152" t="s">
         <v>135</v>
       </c>
       <c r="H152" t="s">
-        <v>922</v>
+        <v>851</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="C153" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D153" t="s">
         <v>11</v>
@@ -7664,10 +7661,10 @@
         <v>36</v>
       </c>
       <c r="F153" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G153" t="s">
-        <v>135</v>
+        <v>1006</v>
       </c>
       <c r="H153" t="s">
         <v>853</v>
@@ -7675,10 +7672,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>161</v>
+        <v>775</v>
       </c>
       <c r="C154" t="s">
         <v>924</v>
@@ -7690,24 +7687,24 @@
         <v>36</v>
       </c>
       <c r="F154" t="s">
-        <v>1049</v>
+        <v>923</v>
       </c>
       <c r="G154" t="s">
-        <v>1008</v>
+        <v>229</v>
       </c>
       <c r="H154" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C155" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D155" t="s">
         <v>11</v>
@@ -7716,24 +7713,24 @@
         <v>36</v>
       </c>
       <c r="F155" t="s">
-        <v>925</v>
+        <v>720</v>
       </c>
       <c r="G155" t="s">
-        <v>229</v>
+        <v>135</v>
       </c>
       <c r="H155" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C156" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D156" t="s">
         <v>11</v>
@@ -7742,47 +7739,47 @@
         <v>36</v>
       </c>
       <c r="F156" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G156" t="s">
         <v>135</v>
       </c>
       <c r="H156" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C157" t="s">
         <v>928</v>
       </c>
       <c r="D157" t="s">
-        <v>11</v>
+        <v>927</v>
       </c>
       <c r="E157" t="s">
         <v>36</v>
       </c>
       <c r="F157" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="G157" t="s">
         <v>135</v>
       </c>
       <c r="H157" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C158" t="s">
         <v>930</v>
@@ -7794,50 +7791,50 @@
         <v>36</v>
       </c>
       <c r="F158" t="s">
-        <v>724</v>
+        <v>1030</v>
       </c>
       <c r="G158" t="s">
-        <v>135</v>
+        <v>18</v>
       </c>
       <c r="H158" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C159" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D159" t="s">
-        <v>931</v>
+        <v>11</v>
       </c>
       <c r="E159" t="s">
         <v>36</v>
       </c>
       <c r="F159" t="s">
-        <v>1032</v>
+        <v>1048</v>
       </c>
       <c r="G159" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="H159" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C160" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D160" t="s">
         <v>11</v>
@@ -7846,24 +7843,24 @@
         <v>36</v>
       </c>
       <c r="F160" t="s">
-        <v>1050</v>
+        <v>1033</v>
       </c>
       <c r="G160" t="s">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="H160" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C161" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D161" t="s">
         <v>11</v>
@@ -7872,102 +7869,102 @@
         <v>36</v>
       </c>
       <c r="F161" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="G161" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="H161" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>651</v>
+        <v>176</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>784</v>
+        <v>177</v>
       </c>
       <c r="C162" t="s">
-        <v>935</v>
+        <v>178</v>
       </c>
       <c r="D162" t="s">
-        <v>11</v>
+        <v>927</v>
       </c>
       <c r="E162" t="s">
         <v>36</v>
       </c>
       <c r="F162" t="s">
-        <v>1033</v>
+        <v>1049</v>
       </c>
       <c r="G162" t="s">
         <v>135</v>
       </c>
       <c r="H162" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>176</v>
+        <v>650</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>177</v>
+        <v>783</v>
       </c>
       <c r="C163" t="s">
-        <v>178</v>
+        <v>934</v>
       </c>
       <c r="D163" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E163" t="s">
         <v>36</v>
       </c>
       <c r="F163" t="s">
-        <v>1051</v>
+        <v>1032</v>
       </c>
       <c r="G163" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="H163" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>652</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>785</v>
+        <v>651</v>
+      </c>
+      <c r="B164" t="s">
+        <v>784</v>
       </c>
       <c r="C164" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D164" t="s">
-        <v>929</v>
+        <v>11</v>
       </c>
       <c r="E164" t="s">
         <v>36</v>
       </c>
       <c r="F164" t="s">
-        <v>1034</v>
+        <v>723</v>
       </c>
       <c r="G164" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="H164" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>653</v>
-      </c>
-      <c r="B165" t="s">
-        <v>786</v>
+        <v>652</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="C165" t="s">
-        <v>937</v>
+        <v>607</v>
       </c>
       <c r="D165" t="s">
         <v>11</v>
@@ -7976,24 +7973,24 @@
         <v>36</v>
       </c>
       <c r="F165" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="G165" t="s">
-        <v>135</v>
+        <v>936</v>
       </c>
       <c r="H165" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>654</v>
+        <v>140</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="C166" t="s">
-        <v>608</v>
+        <v>142</v>
       </c>
       <c r="D166" t="s">
         <v>11</v>
@@ -8002,24 +7999,24 @@
         <v>36</v>
       </c>
       <c r="F166" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G166" t="s">
-        <v>938</v>
+        <v>135</v>
       </c>
       <c r="H166" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>140</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C167" t="s">
-        <v>142</v>
+        <v>653</v>
+      </c>
+      <c r="B167" t="s">
+        <v>937</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>785</v>
       </c>
       <c r="D167" t="s">
         <v>11</v>
@@ -8028,24 +8025,24 @@
         <v>36</v>
       </c>
       <c r="F167" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G167" t="s">
         <v>135</v>
       </c>
       <c r="H167" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>655</v>
-      </c>
-      <c r="B168" t="s">
-        <v>939</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>787</v>
+        <v>314</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="C168" t="s">
+        <v>938</v>
       </c>
       <c r="D168" t="s">
         <v>11</v>
@@ -8054,24 +8051,24 @@
         <v>36</v>
       </c>
       <c r="F168" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G168" t="s">
         <v>135</v>
       </c>
       <c r="H168" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>314</v>
+        <v>654</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C169" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D169" t="s">
         <v>11</v>
@@ -8080,10 +8077,10 @@
         <v>36</v>
       </c>
       <c r="F169" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G169" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="H169" t="s">
         <v>867</v>
@@ -8091,13 +8088,13 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>656</v>
+        <v>165</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>789</v>
+        <v>166</v>
       </c>
       <c r="C170" t="s">
-        <v>941</v>
+        <v>166</v>
       </c>
       <c r="D170" t="s">
         <v>11</v>
@@ -8106,24 +8103,24 @@
         <v>36</v>
       </c>
       <c r="F170" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G170" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="H170" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>165</v>
+        <v>655</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>166</v>
+        <v>788</v>
       </c>
       <c r="C171" t="s">
-        <v>166</v>
+        <v>940</v>
       </c>
       <c r="D171" t="s">
         <v>11</v>
@@ -8132,47 +8129,47 @@
         <v>36</v>
       </c>
       <c r="F171" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G171" t="s">
         <v>135</v>
       </c>
       <c r="H171" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>790</v>
+        <v>168</v>
       </c>
       <c r="C172" t="s">
+        <v>941</v>
+      </c>
+      <c r="D172" t="s">
+        <v>11</v>
+      </c>
+      <c r="E172" t="s">
+        <v>36</v>
+      </c>
+      <c r="F172" t="s">
         <v>942</v>
-      </c>
-      <c r="D172" t="s">
-        <v>11</v>
-      </c>
-      <c r="E172" t="s">
-        <v>36</v>
-      </c>
-      <c r="F172" t="s">
-        <v>732</v>
       </c>
       <c r="G172" t="s">
         <v>135</v>
       </c>
       <c r="H172" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>168</v>
+        <v>789</v>
       </c>
       <c r="C173" t="s">
         <v>943</v>
@@ -8184,24 +8181,24 @@
         <v>36</v>
       </c>
       <c r="F173" t="s">
-        <v>944</v>
+        <v>1050</v>
       </c>
       <c r="G173" t="s">
         <v>135</v>
       </c>
       <c r="H173" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C174" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
@@ -8210,76 +8207,76 @@
         <v>36</v>
       </c>
       <c r="F174" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="G174" t="s">
         <v>135</v>
       </c>
       <c r="H174" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C175" t="s">
         <v>946</v>
       </c>
       <c r="D175" t="s">
-        <v>11</v>
+        <v>945</v>
       </c>
       <c r="E175" t="s">
         <v>36</v>
       </c>
       <c r="F175" t="s">
-        <v>1053</v>
+        <v>731</v>
       </c>
       <c r="G175" t="s">
         <v>135</v>
       </c>
       <c r="H175" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C176" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D176" t="s">
-        <v>947</v>
+        <v>11</v>
       </c>
       <c r="E176" t="s">
         <v>36</v>
       </c>
       <c r="F176" t="s">
-        <v>733</v>
+        <v>1052</v>
       </c>
       <c r="G176" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="H176" t="s">
-        <v>875</v>
+        <v>860</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C177" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D177" t="s">
         <v>11</v>
@@ -8288,154 +8285,154 @@
         <v>36</v>
       </c>
       <c r="F177" t="s">
-        <v>1054</v>
+        <v>732</v>
       </c>
       <c r="G177" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="H177" t="s">
-        <v>862</v>
+        <v>874</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>663</v>
+        <v>147</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>795</v>
+        <v>148</v>
       </c>
       <c r="C178" t="s">
-        <v>950</v>
+        <v>149</v>
       </c>
       <c r="D178" t="s">
-        <v>11</v>
+        <v>949</v>
       </c>
       <c r="E178" t="s">
         <v>36</v>
       </c>
       <c r="F178" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G178" t="s">
         <v>135</v>
       </c>
       <c r="H178" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>147</v>
+        <v>662</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>148</v>
+        <v>794</v>
       </c>
       <c r="C179" t="s">
-        <v>149</v>
+        <v>950</v>
       </c>
       <c r="D179" t="s">
-        <v>951</v>
+        <v>11</v>
       </c>
       <c r="E179" t="s">
         <v>36</v>
       </c>
       <c r="F179" t="s">
-        <v>735</v>
+        <v>1053</v>
       </c>
       <c r="G179" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="H179" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C180" t="s">
+        <v>951</v>
+      </c>
+      <c r="D180" t="s">
         <v>952</v>
       </c>
-      <c r="D180" t="s">
-        <v>11</v>
-      </c>
       <c r="E180" t="s">
         <v>36</v>
       </c>
       <c r="F180" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="G180" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="H180" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C181" t="s">
         <v>953</v>
       </c>
       <c r="D181" t="s">
-        <v>954</v>
+        <v>11</v>
       </c>
       <c r="E181" t="s">
         <v>36</v>
       </c>
       <c r="F181" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G181" t="s">
         <v>135</v>
       </c>
       <c r="H181" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C182" t="s">
+        <v>954</v>
+      </c>
+      <c r="D182" t="s">
+        <v>11</v>
+      </c>
+      <c r="E182" t="s">
+        <v>36</v>
+      </c>
+      <c r="F182" t="s">
+        <v>734</v>
+      </c>
+      <c r="G182" t="s">
         <v>955</v>
       </c>
-      <c r="D182" t="s">
-        <v>11</v>
-      </c>
-      <c r="E182" t="s">
-        <v>36</v>
-      </c>
-      <c r="F182" t="s">
-        <v>1057</v>
-      </c>
-      <c r="G182" t="s">
-        <v>135</v>
-      </c>
       <c r="H182" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>667</v>
+        <v>179</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>799</v>
+        <v>180</v>
       </c>
       <c r="C183" t="s">
-        <v>956</v>
+        <v>181</v>
       </c>
       <c r="D183" t="s">
         <v>11</v>
@@ -8444,24 +8441,24 @@
         <v>36</v>
       </c>
       <c r="F183" t="s">
-        <v>736</v>
+        <v>1056</v>
       </c>
       <c r="G183" t="s">
-        <v>957</v>
+        <v>1018</v>
       </c>
       <c r="H183" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>179</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C184" t="s">
-        <v>181</v>
+        <v>666</v>
+      </c>
+      <c r="B184" t="s">
+        <v>956</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>798</v>
       </c>
       <c r="D184" t="s">
         <v>11</v>
@@ -8470,24 +8467,24 @@
         <v>36</v>
       </c>
       <c r="F184" t="s">
-        <v>1058</v>
+        <v>735</v>
       </c>
       <c r="G184" t="s">
-        <v>1020</v>
+        <v>135</v>
       </c>
       <c r="H184" t="s">
-        <v>882</v>
+        <v>866</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>668</v>
-      </c>
-      <c r="B185" t="s">
-        <v>958</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>800</v>
+        <v>667</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="C185" t="s">
+        <v>957</v>
       </c>
       <c r="D185" t="s">
         <v>11</v>
@@ -8496,24 +8493,24 @@
         <v>36</v>
       </c>
       <c r="F185" t="s">
-        <v>737</v>
+        <v>1057</v>
       </c>
       <c r="G185" t="s">
         <v>135</v>
       </c>
       <c r="H185" t="s">
-        <v>868</v>
+        <v>881</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C186" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D186" t="s">
         <v>11</v>
@@ -8522,24 +8519,24 @@
         <v>36</v>
       </c>
       <c r="F186" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G186" t="s">
         <v>135</v>
       </c>
       <c r="H186" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>802</v>
+        <v>182</v>
       </c>
       <c r="C187" t="s">
-        <v>960</v>
+        <v>183</v>
       </c>
       <c r="D187" t="s">
         <v>11</v>
@@ -8548,24 +8545,24 @@
         <v>36</v>
       </c>
       <c r="F187" t="s">
-        <v>1060</v>
+        <v>736</v>
       </c>
       <c r="G187" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="H187" t="s">
-        <v>884</v>
+        <v>852</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>182</v>
+        <v>801</v>
       </c>
       <c r="C188" t="s">
-        <v>183</v>
+        <v>959</v>
       </c>
       <c r="D188" t="s">
         <v>11</v>
@@ -8574,24 +8571,24 @@
         <v>36</v>
       </c>
       <c r="F188" t="s">
-        <v>738</v>
+        <v>1059</v>
       </c>
       <c r="G188" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="H188" t="s">
-        <v>854</v>
+        <v>883</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C189" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D189" t="s">
         <v>11</v>
@@ -8600,7 +8597,7 @@
         <v>36</v>
       </c>
       <c r="F189" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G189" t="s">
         <v>13</v>
@@ -8611,65 +8608,65 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>673</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>804</v>
-      </c>
-      <c r="C190" t="s">
+        <v>672</v>
+      </c>
+      <c r="B190" t="s">
+        <v>961</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="D190" t="s">
         <v>962</v>
       </c>
-      <c r="D190" t="s">
-        <v>11</v>
-      </c>
       <c r="E190" t="s">
         <v>36</v>
       </c>
       <c r="F190" t="s">
-        <v>1062</v>
+        <v>737</v>
       </c>
       <c r="G190" t="s">
-        <v>13</v>
+        <v>551</v>
       </c>
       <c r="H190" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>674</v>
-      </c>
-      <c r="B191" t="s">
+        <v>673</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="C191" t="s">
         <v>963</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>805</v>
-      </c>
       <c r="D191" t="s">
-        <v>964</v>
+        <v>11</v>
       </c>
       <c r="E191" t="s">
         <v>36</v>
       </c>
       <c r="F191" t="s">
-        <v>739</v>
+        <v>1061</v>
       </c>
       <c r="G191" t="s">
-        <v>551</v>
+        <v>198</v>
       </c>
       <c r="H191" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C192" t="s">
-        <v>965</v>
+        <v>554</v>
       </c>
       <c r="D192" t="s">
         <v>11</v>
@@ -8678,24 +8675,24 @@
         <v>36</v>
       </c>
       <c r="F192" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G192" t="s">
-        <v>198</v>
+        <v>13</v>
       </c>
       <c r="H192" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C193" t="s">
-        <v>554</v>
+        <v>964</v>
       </c>
       <c r="D193" t="s">
         <v>11</v>
@@ -8704,24 +8701,24 @@
         <v>36</v>
       </c>
       <c r="F193" t="s">
-        <v>1064</v>
+        <v>738</v>
       </c>
       <c r="G193" t="s">
         <v>13</v>
       </c>
       <c r="H193" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C194" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D194" t="s">
         <v>11</v>
@@ -8730,99 +8727,99 @@
         <v>36</v>
       </c>
       <c r="F194" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G194" t="s">
-        <v>13</v>
+        <v>338</v>
       </c>
       <c r="H194" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C195" t="s">
+        <v>966</v>
+      </c>
+      <c r="D195" t="s">
         <v>967</v>
       </c>
-      <c r="D195" t="s">
-        <v>11</v>
-      </c>
       <c r="E195" t="s">
         <v>36</v>
       </c>
       <c r="F195" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="G195" t="s">
-        <v>338</v>
+        <v>1019</v>
       </c>
       <c r="H195" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C196" t="s">
         <v>968</v>
       </c>
       <c r="D196" t="s">
-        <v>969</v>
+        <v>11</v>
       </c>
       <c r="E196" t="s">
         <v>36</v>
       </c>
       <c r="F196" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G196" t="s">
-        <v>1021</v>
+        <v>198</v>
       </c>
       <c r="H196" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C197" t="s">
+        <v>969</v>
+      </c>
+      <c r="D197" t="s">
+        <v>11</v>
+      </c>
+      <c r="E197" t="s">
+        <v>36</v>
+      </c>
+      <c r="F197" t="s">
+        <v>742</v>
+      </c>
+      <c r="G197" t="s">
         <v>970</v>
       </c>
-      <c r="D197" t="s">
-        <v>11</v>
-      </c>
-      <c r="E197" t="s">
-        <v>36</v>
-      </c>
-      <c r="F197" t="s">
-        <v>743</v>
-      </c>
-      <c r="G197" t="s">
-        <v>198</v>
-      </c>
       <c r="H197" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C198" t="s">
         <v>971</v>
@@ -8834,24 +8831,24 @@
         <v>36</v>
       </c>
       <c r="F198" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="G198" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="H198" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C199" t="s">
-        <v>973</v>
+        <v>1013</v>
       </c>
       <c r="D199" t="s">
         <v>11</v>
@@ -8860,24 +8857,24 @@
         <v>36</v>
       </c>
       <c r="F199" t="s">
-        <v>745</v>
+        <v>1012</v>
       </c>
       <c r="G199" t="s">
-        <v>972</v>
+        <v>198</v>
       </c>
       <c r="H199" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="C200" t="s">
-        <v>1015</v>
+        <v>813</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>813</v>
       </c>
       <c r="D200" t="s">
         <v>11</v>
@@ -8886,24 +8883,24 @@
         <v>36</v>
       </c>
       <c r="F200" t="s">
-        <v>1014</v>
+        <v>744</v>
       </c>
       <c r="G200" t="s">
-        <v>198</v>
+        <v>442</v>
       </c>
       <c r="H200" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>815</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
+      </c>
+      <c r="C201" t="s">
+        <v>972</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
@@ -8912,24 +8909,21 @@
         <v>36</v>
       </c>
       <c r="F201" t="s">
-        <v>746</v>
+        <v>1063</v>
       </c>
       <c r="G201" t="s">
         <v>442</v>
       </c>
-      <c r="H201" t="s">
-        <v>895</v>
-      </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C202" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D202" t="s">
         <v>11</v>
@@ -8938,21 +8932,24 @@
         <v>36</v>
       </c>
       <c r="F202" t="s">
-        <v>1065</v>
+        <v>745</v>
       </c>
       <c r="G202" t="s">
         <v>442</v>
       </c>
+      <c r="H202" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C203" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
@@ -8961,24 +8958,24 @@
         <v>36</v>
       </c>
       <c r="F203" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G203" t="s">
         <v>442</v>
       </c>
       <c r="H203" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>818</v>
-      </c>
-      <c r="C204" t="s">
-        <v>976</v>
+        <v>817</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D204" t="s">
         <v>11</v>
@@ -8987,24 +8984,24 @@
         <v>36</v>
       </c>
       <c r="F204" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="G204" t="s">
         <v>442</v>
       </c>
       <c r="H204" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D205" t="s">
         <v>11</v>
@@ -9013,24 +9010,24 @@
         <v>36</v>
       </c>
       <c r="F205" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G205" t="s">
         <v>442</v>
       </c>
       <c r="H205" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D206" t="s">
         <v>11</v>
@@ -9039,24 +9036,24 @@
         <v>36</v>
       </c>
       <c r="F206" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G206" t="s">
         <v>442</v>
       </c>
       <c r="H206" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D207" t="s">
         <v>11</v>
@@ -9065,24 +9062,24 @@
         <v>36</v>
       </c>
       <c r="F207" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G207" t="s">
         <v>442</v>
       </c>
       <c r="H207" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D208" t="s">
         <v>11</v>
@@ -9091,24 +9088,24 @@
         <v>36</v>
       </c>
       <c r="F208" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G208" t="s">
         <v>442</v>
       </c>
       <c r="H208" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D209" t="s">
         <v>11</v>
@@ -9117,24 +9114,24 @@
         <v>36</v>
       </c>
       <c r="F209" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G209" t="s">
         <v>442</v>
       </c>
       <c r="H209" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>824</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
+      </c>
+      <c r="C210" t="s">
+        <v>975</v>
       </c>
       <c r="D210" t="s">
         <v>11</v>
@@ -9143,24 +9140,24 @@
         <v>36</v>
       </c>
       <c r="F210" t="s">
-        <v>754</v>
+        <v>1064</v>
       </c>
       <c r="G210" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="H210" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C211" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D211" t="s">
         <v>11</v>
@@ -9169,24 +9166,24 @@
         <v>36</v>
       </c>
       <c r="F211" t="s">
-        <v>1066</v>
+        <v>753</v>
       </c>
       <c r="G211" t="s">
-        <v>453</v>
+        <v>257</v>
       </c>
       <c r="H211" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C212" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="D212" t="s">
         <v>11</v>
@@ -9195,24 +9192,24 @@
         <v>36</v>
       </c>
       <c r="F212" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G212" t="s">
         <v>257</v>
       </c>
       <c r="H212" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C213" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D213" t="s">
         <v>11</v>
@@ -9221,24 +9218,24 @@
         <v>36</v>
       </c>
       <c r="F213" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G213" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="H213" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C214" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D214" t="s">
         <v>11</v>
@@ -9247,24 +9244,24 @@
         <v>36</v>
       </c>
       <c r="F214" t="s">
-        <v>757</v>
+        <v>1065</v>
       </c>
       <c r="G214" t="s">
-        <v>267</v>
+        <v>453</v>
       </c>
       <c r="H214" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C215" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D215" t="s">
         <v>11</v>
@@ -9273,24 +9270,24 @@
         <v>36</v>
       </c>
       <c r="F215" t="s">
-        <v>1067</v>
+        <v>756</v>
       </c>
       <c r="G215" t="s">
-        <v>453</v>
+        <v>107</v>
       </c>
       <c r="H215" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>830</v>
-      </c>
-      <c r="C216" t="s">
-        <v>982</v>
+        <v>829</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>829</v>
       </c>
       <c r="D216" t="s">
         <v>11</v>
@@ -9299,102 +9296,102 @@
         <v>36</v>
       </c>
       <c r="F216" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G216" t="s">
         <v>107</v>
       </c>
       <c r="H216" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>831</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
+      </c>
+      <c r="C217" t="s">
+        <v>981</v>
       </c>
       <c r="D217" t="s">
-        <v>11</v>
+        <v>982</v>
       </c>
       <c r="E217" t="s">
         <v>36</v>
       </c>
       <c r="F217" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G217" t="s">
         <v>107</v>
       </c>
       <c r="H217" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>832</v>
-      </c>
-      <c r="C218" t="s">
+        <v>831</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="D218" t="s">
         <v>983</v>
       </c>
-      <c r="D218" t="s">
-        <v>984</v>
-      </c>
       <c r="E218" t="s">
         <v>36</v>
       </c>
       <c r="F218" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G218" t="s">
         <v>107</v>
       </c>
       <c r="H218" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>833</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
+      </c>
+      <c r="C219" t="s">
+        <v>984</v>
       </c>
       <c r="D219" t="s">
-        <v>985</v>
+        <v>11</v>
       </c>
       <c r="E219" t="s">
         <v>36</v>
       </c>
       <c r="F219" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="G219" t="s">
         <v>107</v>
       </c>
       <c r="H219" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C220" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D220" t="s">
         <v>11</v>
@@ -9403,24 +9400,24 @@
         <v>36</v>
       </c>
       <c r="F220" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G220" t="s">
         <v>107</v>
       </c>
       <c r="H220" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C221" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D221" t="s">
         <v>11</v>
@@ -9429,24 +9426,24 @@
         <v>36</v>
       </c>
       <c r="F221" t="s">
-        <v>763</v>
+        <v>1066</v>
       </c>
       <c r="G221" t="s">
         <v>107</v>
       </c>
       <c r="H221" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C222" t="s">
-        <v>988</v>
+        <v>583</v>
       </c>
       <c r="D222" t="s">
         <v>11</v>
@@ -9455,24 +9452,24 @@
         <v>36</v>
       </c>
       <c r="F222" t="s">
-        <v>1068</v>
+        <v>762</v>
       </c>
       <c r="G222" t="s">
-        <v>107</v>
+        <v>1007</v>
       </c>
       <c r="H222" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>706</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>837</v>
-      </c>
-      <c r="C223" t="s">
-        <v>584</v>
+        <v>705</v>
+      </c>
+      <c r="B223" t="s">
+        <v>991</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>836</v>
       </c>
       <c r="D223" t="s">
         <v>11</v>
@@ -9481,24 +9478,21 @@
         <v>36</v>
       </c>
       <c r="F223" t="s">
-        <v>764</v>
+        <v>1067</v>
       </c>
       <c r="G223" t="s">
-        <v>1009</v>
-      </c>
-      <c r="H223" t="s">
-        <v>911</v>
+        <v>107</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>707</v>
-      </c>
-      <c r="B224" t="s">
-        <v>993</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>838</v>
+        <v>706</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="C224" t="s">
+        <v>992</v>
       </c>
       <c r="D224" t="s">
         <v>11</v>
@@ -9507,21 +9501,24 @@
         <v>36</v>
       </c>
       <c r="F224" t="s">
-        <v>1069</v>
+        <v>763</v>
       </c>
       <c r="G224" t="s">
-        <v>107</v>
+        <v>13</v>
+      </c>
+      <c r="H224" t="s">
+        <v>910</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C225" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D225" t="s">
         <v>11</v>
@@ -9530,24 +9527,24 @@
         <v>36</v>
       </c>
       <c r="F225" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G225" t="s">
-        <v>13</v>
+        <v>1007</v>
       </c>
       <c r="H225" t="s">
-        <v>912</v>
+        <v>903</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C226" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D226" t="s">
         <v>11</v>
@@ -9556,24 +9553,24 @@
         <v>36</v>
       </c>
       <c r="F226" t="s">
-        <v>766</v>
+        <v>1068</v>
       </c>
       <c r="G226" t="s">
-        <v>1009</v>
+        <v>13</v>
       </c>
       <c r="H226" t="s">
-        <v>905</v>
+        <v>911</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C227" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D227" t="s">
         <v>11</v>
@@ -9582,24 +9579,24 @@
         <v>36</v>
       </c>
       <c r="F227" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="G227" t="s">
-        <v>13</v>
+        <v>322</v>
       </c>
       <c r="H227" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C228" t="s">
-        <v>997</v>
+        <v>841</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>841</v>
       </c>
       <c r="D228" t="s">
         <v>11</v>
@@ -9608,24 +9605,21 @@
         <v>36</v>
       </c>
       <c r="F228" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G228" t="s">
         <v>322</v>
       </c>
-      <c r="H228" t="s">
-        <v>914</v>
-      </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
+      </c>
+      <c r="C229" t="s">
+        <v>996</v>
       </c>
       <c r="D229" t="s">
         <v>11</v>
@@ -9634,21 +9628,24 @@
         <v>36</v>
       </c>
       <c r="F229" t="s">
-        <v>1072</v>
+        <v>765</v>
       </c>
       <c r="G229" t="s">
-        <v>322</v>
+        <v>579</v>
+      </c>
+      <c r="H229" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C230" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D230" t="s">
         <v>11</v>
@@ -9657,24 +9654,24 @@
         <v>36</v>
       </c>
       <c r="F230" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G230" t="s">
-        <v>580</v>
+        <v>288</v>
       </c>
       <c r="H230" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C231" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D231" t="s">
         <v>11</v>
@@ -9683,76 +9680,76 @@
         <v>36</v>
       </c>
       <c r="F231" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G231" t="s">
         <v>288</v>
       </c>
       <c r="H231" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C232" t="s">
-        <v>1000</v>
+        <v>845</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>845</v>
       </c>
       <c r="D232" t="s">
-        <v>11</v>
+        <v>999</v>
       </c>
       <c r="E232" t="s">
         <v>36</v>
       </c>
       <c r="F232" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G232" t="s">
         <v>288</v>
       </c>
       <c r="H232" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
+      </c>
+      <c r="C233" t="s">
+        <v>1000</v>
       </c>
       <c r="D233" t="s">
-        <v>1001</v>
+        <v>11</v>
       </c>
       <c r="E233" t="s">
         <v>36</v>
       </c>
       <c r="F233" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G233" t="s">
         <v>288</v>
       </c>
       <c r="H233" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>717</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>848</v>
+        <v>987</v>
+      </c>
+      <c r="B234" t="s">
+        <v>988</v>
       </c>
       <c r="C234" t="s">
-        <v>1002</v>
+        <v>989</v>
       </c>
       <c r="D234" t="s">
         <v>11</v>
@@ -9761,70 +9758,70 @@
         <v>36</v>
       </c>
       <c r="F234" t="s">
-        <v>771</v>
+        <v>990</v>
       </c>
       <c r="G234" t="s">
-        <v>288</v>
-      </c>
-      <c r="H234" t="s">
-        <v>919</v>
+        <v>13</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>989</v>
+        <v>1002</v>
       </c>
       <c r="B235" t="s">
-        <v>990</v>
+        <v>1003</v>
       </c>
       <c r="C235" t="s">
-        <v>991</v>
+        <v>1004</v>
       </c>
       <c r="D235" t="s">
         <v>11</v>
       </c>
       <c r="E235" t="s">
-        <v>36</v>
+        <v>370</v>
       </c>
       <c r="F235" t="s">
-        <v>992</v>
+        <v>1005</v>
       </c>
       <c r="G235" t="s">
-        <v>13</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>1004</v>
+        <v>1073</v>
       </c>
       <c r="B236" t="s">
-        <v>1005</v>
+        <v>1088</v>
       </c>
       <c r="C236" t="s">
-        <v>1006</v>
+        <v>1079</v>
       </c>
       <c r="D236" t="s">
         <v>11</v>
       </c>
       <c r="E236" t="s">
-        <v>370</v>
+        <v>12</v>
       </c>
       <c r="F236" t="s">
-        <v>1007</v>
+        <v>1092</v>
       </c>
       <c r="G236" t="s">
-        <v>1010</v>
+        <v>13</v>
+      </c>
+      <c r="H236" t="s">
+        <v>1090</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B237" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C237" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="D237" t="s">
         <v>11</v>
@@ -9833,24 +9830,24 @@
         <v>12</v>
       </c>
       <c r="F237" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="G237" t="s">
-        <v>13</v>
+        <v>338</v>
       </c>
       <c r="H237" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B238" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C238" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="D238" t="s">
         <v>11</v>
@@ -9859,24 +9856,24 @@
         <v>12</v>
       </c>
       <c r="F238" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="G238" t="s">
         <v>338</v>
       </c>
       <c r="H238" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B239" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C239" t="s">
-        <v>1079</v>
+        <v>1100</v>
       </c>
       <c r="D239" t="s">
         <v>11</v>
@@ -9885,24 +9882,24 @@
         <v>12</v>
       </c>
       <c r="F239" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="G239" t="s">
-        <v>338</v>
+        <v>13</v>
       </c>
       <c r="H239" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>1078</v>
+        <v>1084</v>
       </c>
       <c r="B240" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C240" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="D240" t="s">
         <v>11</v>
@@ -9911,24 +9908,24 @@
         <v>12</v>
       </c>
       <c r="F240" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="G240" t="s">
-        <v>13</v>
+        <v>338</v>
       </c>
       <c r="H240" t="s">
-        <v>1092</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B241" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C241" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="D241" t="s">
         <v>11</v>
@@ -9937,24 +9934,24 @@
         <v>12</v>
       </c>
       <c r="F241" t="s">
-        <v>1099</v>
+        <v>1103</v>
       </c>
       <c r="G241" t="s">
         <v>338</v>
       </c>
       <c r="H241" t="s">
-        <v>1101</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B242" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C242" t="s">
-        <v>1104</v>
+        <v>1089</v>
       </c>
       <c r="D242" t="s">
         <v>11</v>
@@ -9963,21 +9960,21 @@
         <v>12</v>
       </c>
       <c r="F242" t="s">
-        <v>1105</v>
+        <v>1093</v>
       </c>
       <c r="G242" t="s">
         <v>338</v>
       </c>
       <c r="H242" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B243" t="s">
         <v>1088</v>
-      </c>
-      <c r="B243" t="s">
-        <v>1090</v>
       </c>
       <c r="C243" t="s">
         <v>1091</v>
@@ -9989,24 +9986,24 @@
         <v>12</v>
       </c>
       <c r="F243" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="G243" t="s">
         <v>338</v>
       </c>
       <c r="H243" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>1089</v>
+        <v>1080</v>
       </c>
       <c r="B244" t="s">
-        <v>1090</v>
+        <v>1081</v>
       </c>
       <c r="C244" t="s">
-        <v>1093</v>
+        <v>1081</v>
       </c>
       <c r="D244" t="s">
         <v>11</v>
@@ -10015,47 +10012,44 @@
         <v>12</v>
       </c>
       <c r="F244" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="G244" t="s">
-        <v>338</v>
+        <v>13</v>
       </c>
       <c r="H244" t="s">
-        <v>1092</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>1082</v>
+        <v>1106</v>
       </c>
       <c r="B245" t="s">
-        <v>1083</v>
+        <v>1107</v>
       </c>
       <c r="C245" t="s">
-        <v>1083</v>
+        <v>1108</v>
       </c>
       <c r="D245" t="s">
         <v>11</v>
       </c>
       <c r="E245" t="s">
-        <v>12</v>
+        <v>370</v>
       </c>
       <c r="F245" t="s">
-        <v>1084</v>
+        <v>1109</v>
       </c>
       <c r="G245" t="s">
-        <v>13</v>
-      </c>
-      <c r="H245" t="s">
-        <v>1085</v>
+        <v>135</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>1108</v>
+        <v>1113</v>
       </c>
       <c r="B246" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C246" t="s">
         <v>1110</v>
@@ -10064,13 +10058,16 @@
         <v>11</v>
       </c>
       <c r="E246" t="s">
-        <v>370</v>
+        <v>12</v>
       </c>
       <c r="F246" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G246" t="s">
+        <v>13</v>
+      </c>
+      <c r="H246" t="s">
         <v>1111</v>
-      </c>
-      <c r="G246" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.2">
@@ -10078,51 +10075,25 @@
         <v>1115</v>
       </c>
       <c r="B247" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C247" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D247" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E247" t="s">
+        <v>370</v>
+      </c>
+      <c r="F247" t="s">
         <v>1112</v>
-      </c>
-      <c r="C247" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D247" t="s">
-        <v>11</v>
-      </c>
-      <c r="E247" t="s">
-        <v>12</v>
-      </c>
-      <c r="F247" t="s">
-        <v>1114</v>
       </c>
       <c r="G247" t="s">
         <v>13</v>
       </c>
       <c r="H247" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A248" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B248" t="s">
-        <v>1116</v>
-      </c>
-      <c r="C248" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D248" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E248" t="s">
-        <v>370</v>
-      </c>
-      <c r="F248" t="s">
-        <v>1114</v>
-      </c>
-      <c r="G248" t="s">
-        <v>13</v>
-      </c>
-      <c r="H248" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
   </sheetData>
@@ -10377,137 +10348,135 @@
     <hyperlink ref="C132" r:id="rId248" xr:uid="{D918A6CC-4DE8-5749-B396-C5BE2178FEAC}"/>
     <hyperlink ref="C133" r:id="rId249" xr:uid="{993B79A8-C154-C64D-AAA1-BA2D47F20826}"/>
     <hyperlink ref="C134" r:id="rId250" xr:uid="{42BB3483-8CC1-E142-BE62-922281DD72B0}"/>
-    <hyperlink ref="C135" r:id="rId251" xr:uid="{F748A52A-20AD-7D4D-ADFF-FF4E6B3B904F}"/>
-    <hyperlink ref="C136" r:id="rId252" xr:uid="{BDA7CC67-1472-8248-946E-93B6F618685B}"/>
-    <hyperlink ref="C137" r:id="rId253" xr:uid="{EA63AAC0-2987-5B4D-8CA8-F8E8B820ED36}"/>
-    <hyperlink ref="C138" r:id="rId254" xr:uid="{A66AC424-A7F4-B84A-9280-820A43B4AEBA}"/>
-    <hyperlink ref="C139" r:id="rId255" xr:uid="{E7A6808E-50F2-0948-9C94-628B4F9ACF7D}"/>
-    <hyperlink ref="C140" r:id="rId256" xr:uid="{0B5221E8-DE05-0E4E-9EE3-DCADE66F2696}"/>
-    <hyperlink ref="C141" r:id="rId257" xr:uid="{EA1D837B-5F6A-B54C-9B61-2034B0CE85B3}"/>
-    <hyperlink ref="C142" r:id="rId258" xr:uid="{A3994F4F-3387-1942-A3D6-B8B67EB06BC1}"/>
-    <hyperlink ref="C143" r:id="rId259" xr:uid="{B8D152B1-8B72-E74D-88F6-C43A49A5AB2F}"/>
-    <hyperlink ref="B144" r:id="rId260" xr:uid="{6964114A-F58F-724D-A2B4-173388BA5302}"/>
-    <hyperlink ref="B145" r:id="rId261" xr:uid="{3BD56E0B-D3CE-AD4D-91FA-51D4543B137E}"/>
-    <hyperlink ref="B146" r:id="rId262" xr:uid="{23A75913-BCC4-4E47-9B47-B952CD9112B4}"/>
-    <hyperlink ref="B147" r:id="rId263" xr:uid="{60B2A7C5-DB9E-5F41-B146-74A96ECCE834}"/>
-    <hyperlink ref="C129" r:id="rId264" xr:uid="{F7F12410-9273-7F45-805B-07CE4BFEB9E8}"/>
-    <hyperlink ref="B148" r:id="rId265" xr:uid="{F234784D-26C2-A545-B685-EF602C8D974F}"/>
-    <hyperlink ref="B149" r:id="rId266" xr:uid="{0CF53428-4492-AE40-9C02-9FABA2BA0D3B}"/>
-    <hyperlink ref="B151" r:id="rId267" xr:uid="{6E42F66B-4B80-564E-8A39-545051468745}"/>
-    <hyperlink ref="B152" r:id="rId268" xr:uid="{D200C44B-A95E-434E-B96F-F097A5CB9796}"/>
-    <hyperlink ref="B153" r:id="rId269" xr:uid="{6C870BBD-0FCA-4E4D-8C04-64F66A4CDDBD}"/>
-    <hyperlink ref="B154" r:id="rId270" xr:uid="{13618F8B-EF5F-744B-92F0-4F8047208B03}"/>
-    <hyperlink ref="B155" r:id="rId271" xr:uid="{369A99E5-8534-484F-9378-38EA1F763D49}"/>
-    <hyperlink ref="B156" r:id="rId272" xr:uid="{F755E08D-37B2-7740-8B78-61FD6A0062F8}"/>
-    <hyperlink ref="B157" r:id="rId273" xr:uid="{DE03D456-C44C-C442-8758-FF0ADB5910C9}"/>
-    <hyperlink ref="B158" r:id="rId274" xr:uid="{DD51AED9-A8BF-E340-A7B8-574926029C7A}"/>
-    <hyperlink ref="B159" r:id="rId275" xr:uid="{4106DA73-80ED-0C48-9333-CF22AD9B453B}"/>
-    <hyperlink ref="B160" r:id="rId276" xr:uid="{24AA6FBD-DA03-1641-9CCE-C4125E436587}"/>
-    <hyperlink ref="B161" r:id="rId277" xr:uid="{671C41C7-BBE6-6244-AC5F-C2D5050A9976}"/>
-    <hyperlink ref="B162" r:id="rId278" xr:uid="{0A61AD93-54F4-B64C-A125-A39B41D20037}"/>
-    <hyperlink ref="B163" r:id="rId279" xr:uid="{B21EB3D6-55DF-A648-99FE-B9174BEB51CF}"/>
-    <hyperlink ref="B164" r:id="rId280" xr:uid="{EDD64D5C-42F2-1944-868E-02CE17E0C28C}"/>
-    <hyperlink ref="B166" r:id="rId281" xr:uid="{76E6FFD7-9F09-F545-9058-D27B73251ABF}"/>
-    <hyperlink ref="B167" r:id="rId282" xr:uid="{9ADE58D5-16AC-DC4F-A820-2981CD2C5EE1}"/>
-    <hyperlink ref="C168" r:id="rId283" xr:uid="{8D033399-8CBD-724D-80CD-C7397C3C2A0F}"/>
-    <hyperlink ref="B169" r:id="rId284" xr:uid="{01B1B80B-C304-4D4F-A53E-AB4D0EE61624}"/>
-    <hyperlink ref="B170" r:id="rId285" xr:uid="{F690EC01-0A49-E548-9E56-0EACEA75EA38}"/>
-    <hyperlink ref="B171" r:id="rId286" xr:uid="{7F51F9C1-398D-9749-A281-E22D1309A30E}"/>
-    <hyperlink ref="B172" r:id="rId287" xr:uid="{64214232-7C7F-8444-9AAC-0A4BBD3AF2D1}"/>
-    <hyperlink ref="B173" r:id="rId288" xr:uid="{7AF546D0-B342-424F-A68E-944E05062E8A}"/>
-    <hyperlink ref="B174" r:id="rId289" xr:uid="{0050ED55-AE7F-E64C-87FF-712ACBB46C7D}"/>
-    <hyperlink ref="B175" r:id="rId290" xr:uid="{83754876-42D8-E74F-91FA-9CECBBAC6924}"/>
-    <hyperlink ref="B176" r:id="rId291" xr:uid="{337A6E39-03DD-064F-BF1E-FA6674858C0B}"/>
-    <hyperlink ref="B177" r:id="rId292" xr:uid="{8D3B4445-BD15-E441-B13B-E90EAF62DA8E}"/>
-    <hyperlink ref="B178" r:id="rId293" xr:uid="{F8DCC388-ABD3-2544-8E1A-8EAF5A2DAA9C}"/>
-    <hyperlink ref="B179" r:id="rId294" xr:uid="{BC6EE541-680A-884F-958C-C07EA84B94D8}"/>
-    <hyperlink ref="B180" r:id="rId295" xr:uid="{DD1C41B7-F12D-0B4A-807D-2D572F6BC0DA}"/>
-    <hyperlink ref="B181" r:id="rId296" xr:uid="{456B4E6A-BAF0-1C4B-A5A2-33029913A11F}"/>
-    <hyperlink ref="B182" r:id="rId297" xr:uid="{AB596C81-A2E4-D84E-97FF-F4EDC38B3AB7}"/>
-    <hyperlink ref="B183" r:id="rId298" xr:uid="{6925BDA1-8306-C94C-B344-AC929606B70C}"/>
-    <hyperlink ref="B184" r:id="rId299" xr:uid="{F1F6DFAC-7F73-E242-80A6-0A54A6B92CBA}"/>
-    <hyperlink ref="C185" r:id="rId300" xr:uid="{2B979D45-F5FD-A54F-886F-C8E41EB241BE}"/>
-    <hyperlink ref="B186" r:id="rId301" xr:uid="{A4B83D25-A914-374B-AC70-67BC2B213C2A}"/>
-    <hyperlink ref="B187" r:id="rId302" xr:uid="{F533F9B9-2BCF-A847-AC92-C786DBA1CF4B}"/>
-    <hyperlink ref="B188" r:id="rId303" xr:uid="{6C8BEC30-39CE-A548-BBDD-73A01B452059}"/>
-    <hyperlink ref="B189" r:id="rId304" xr:uid="{85FCE497-9E96-6648-867F-752AA283D510}"/>
-    <hyperlink ref="B190" r:id="rId305" xr:uid="{43C3B803-5A07-A642-8293-EBD66D59834D}"/>
-    <hyperlink ref="C191" r:id="rId306" xr:uid="{31EDEE6A-D8E5-8C48-87E9-064EB36F385C}"/>
-    <hyperlink ref="B192" r:id="rId307" xr:uid="{F9240DAF-1152-804D-82D6-CD96D548238C}"/>
-    <hyperlink ref="B193" r:id="rId308" xr:uid="{DD79C80C-1BE5-F149-88DD-8DA5369DFCAD}"/>
-    <hyperlink ref="B194" r:id="rId309" xr:uid="{B0E436A7-E831-8E4C-9EAC-5207B2FC9DA3}"/>
-    <hyperlink ref="B195" r:id="rId310" xr:uid="{945AD53A-A851-EB4A-B3AC-9B72897828BE}"/>
-    <hyperlink ref="B196" r:id="rId311" xr:uid="{FAEF4F3C-0C71-C542-B31C-BDECF30F1ABE}"/>
-    <hyperlink ref="B197" r:id="rId312" xr:uid="{16789C92-8D31-CA42-A3C5-F457DE323071}"/>
-    <hyperlink ref="B198" r:id="rId313" xr:uid="{C9BB414A-D34A-A743-8C91-1506BC729AF1}"/>
-    <hyperlink ref="B199" r:id="rId314" xr:uid="{7E709984-032A-6D43-B8C0-35BB36F33A8B}"/>
-    <hyperlink ref="B200" r:id="rId315" xr:uid="{AF735B37-2761-6B44-8457-C70F018D475D}"/>
-    <hyperlink ref="C201" r:id="rId316" xr:uid="{F3E9CC02-E232-F247-910C-0F8F818F15FD}"/>
-    <hyperlink ref="B202" r:id="rId317" xr:uid="{CF20CF77-6D17-A640-BC1C-06D8AC56128F}"/>
-    <hyperlink ref="B203" r:id="rId318" xr:uid="{05A67C14-E63C-6643-A98B-DE5374A332F7}"/>
-    <hyperlink ref="B204" r:id="rId319" xr:uid="{2E28DB30-178A-5F43-BABB-5699190A802A}"/>
-    <hyperlink ref="C205" r:id="rId320" xr:uid="{D1AA51DE-D608-3D45-AD22-E8B64F1419E7}"/>
-    <hyperlink ref="C206" r:id="rId321" xr:uid="{9BABC60F-FE82-5248-9E79-B718EC0F659A}"/>
-    <hyperlink ref="C207" r:id="rId322" xr:uid="{03289203-0011-5743-AC70-D84C9B97DC6E}"/>
-    <hyperlink ref="C208" r:id="rId323" xr:uid="{1B79D66B-2C73-624F-A90B-DE414F9850D6}"/>
-    <hyperlink ref="C209" r:id="rId324" xr:uid="{43F13A60-CCD1-0C40-AB37-E9F9EE97732E}"/>
-    <hyperlink ref="C210" r:id="rId325" xr:uid="{1C156BC9-5818-4049-8EF2-B540C3E68E81}"/>
-    <hyperlink ref="B211" r:id="rId326" xr:uid="{53D53A00-1672-664D-91C8-7C5331F6CCA5}"/>
-    <hyperlink ref="B212" r:id="rId327" xr:uid="{515855E3-E3E4-F845-9DC8-E34325F7F3DA}"/>
-    <hyperlink ref="B213" r:id="rId328" xr:uid="{BA928391-E722-7746-BED2-1C83F80C0DBC}"/>
-    <hyperlink ref="B214" r:id="rId329" xr:uid="{102F6A53-9ABC-3E45-BD5C-B9BF66066C2A}"/>
-    <hyperlink ref="B215" r:id="rId330" xr:uid="{1285018C-691B-2E4B-A2D4-583D0B414C1F}"/>
-    <hyperlink ref="B216" r:id="rId331" xr:uid="{76AAE9CF-2707-B143-B652-46D8CE36A647}"/>
-    <hyperlink ref="C217" r:id="rId332" xr:uid="{6F160E9C-28C2-9641-9DFC-22F25114A500}"/>
-    <hyperlink ref="B218" r:id="rId333" xr:uid="{73B6A897-CC12-624B-B420-3142BFB3B7E7}"/>
-    <hyperlink ref="C219" r:id="rId334" xr:uid="{97260B38-6E63-8949-A540-58D6E311FC48}"/>
-    <hyperlink ref="B220" r:id="rId335" xr:uid="{63962B13-F41B-C849-BD6B-055FC35A58D4}"/>
-    <hyperlink ref="B221" r:id="rId336" xr:uid="{76C9DF5E-2957-2841-B4F2-ABA46671CCA0}"/>
-    <hyperlink ref="B222" r:id="rId337" xr:uid="{89A49EA1-C764-B740-A236-82525B727186}"/>
-    <hyperlink ref="B223" r:id="rId338" xr:uid="{ECE997AF-CE38-B24F-ADBF-641D516BA06C}"/>
-    <hyperlink ref="C224" r:id="rId339" xr:uid="{E42A850B-432C-BD4F-ADAD-269074FD12D7}"/>
-    <hyperlink ref="B225" r:id="rId340" xr:uid="{C1923A14-8FC3-3048-929B-76B8E6CABE4E}"/>
-    <hyperlink ref="B226" r:id="rId341" xr:uid="{FB93A9DD-F604-164C-8539-EE9D683EAE3F}"/>
-    <hyperlink ref="B227" r:id="rId342" xr:uid="{3ED03127-35DA-8A49-93C9-896BA1D8DC06}"/>
-    <hyperlink ref="B228" r:id="rId343" xr:uid="{6AECACA9-7563-5844-88E8-65163C3C2045}"/>
-    <hyperlink ref="C229" r:id="rId344" xr:uid="{8922321F-CDC7-5A46-838D-8D1A2F011DBC}"/>
-    <hyperlink ref="B230" r:id="rId345" xr:uid="{97E5BE47-CB30-1E45-9F11-15A6DE53936E}"/>
-    <hyperlink ref="B231" r:id="rId346" xr:uid="{B055B99F-8704-CA44-985E-FEE3A9E3B3EB}"/>
-    <hyperlink ref="B232" r:id="rId347" xr:uid="{5FEA98AF-8D00-C041-8FAA-30E8369F763B}"/>
-    <hyperlink ref="C233" r:id="rId348" xr:uid="{6782F7DA-4236-7740-A30E-EFCC23B81659}"/>
-    <hyperlink ref="B234" r:id="rId349" xr:uid="{ECA5F0C7-3864-ED48-B6A1-19E564969867}"/>
-    <hyperlink ref="B150" r:id="rId350" xr:uid="{C9B92141-6E73-914D-864F-BCF52A0441AB}"/>
-    <hyperlink ref="B106" r:id="rId351" xr:uid="{D9B7A9AA-835A-D440-B1F8-5FD8BA13EDDD}"/>
-    <hyperlink ref="B107" r:id="rId352" xr:uid="{7D9A8CFA-B72E-A545-A9FF-EDF4FCCB10D2}"/>
-    <hyperlink ref="B108" r:id="rId353" xr:uid="{1FDFABF3-4AC9-E94F-8F18-8D411A8F2A41}"/>
-    <hyperlink ref="B127" r:id="rId354" xr:uid="{0B90C06A-4AA3-7D4C-9151-0A8E86D33CF7}"/>
-    <hyperlink ref="B130" r:id="rId355" xr:uid="{41F8EA90-1905-5C44-A76E-C2835343544D}"/>
-    <hyperlink ref="B134" r:id="rId356" xr:uid="{FCCEDAA3-5F09-8F4E-A216-B145A130752A}"/>
-    <hyperlink ref="B135" r:id="rId357" xr:uid="{F25B11F0-FA68-8449-B6D5-77D0823A038E}"/>
-    <hyperlink ref="B136" r:id="rId358" xr:uid="{4CFCEB5C-9EA6-444B-B4A2-DFCB393B2F22}"/>
-    <hyperlink ref="B137" r:id="rId359" xr:uid="{9A0771D2-A3EE-1A4B-9800-411D74964533}"/>
-    <hyperlink ref="B139" r:id="rId360" xr:uid="{2185F98B-0A23-8744-A78F-0879B84BE337}"/>
-    <hyperlink ref="B140" r:id="rId361" xr:uid="{C24EAB49-5746-464B-9358-7B4ED4CF07C0}"/>
-    <hyperlink ref="B141" r:id="rId362" xr:uid="{7A760695-4FA5-784E-A939-A62BC029D8EE}"/>
-    <hyperlink ref="B142" r:id="rId363" xr:uid="{FB8F38DD-E9D5-474F-BE8C-E340D4584463}"/>
-    <hyperlink ref="B143" r:id="rId364" xr:uid="{A5739124-C2FB-7D4A-A75F-F924EE1B685A}"/>
-    <hyperlink ref="C144" r:id="rId365" xr:uid="{344639F6-7829-3644-88B4-2E8EADF8B352}"/>
-    <hyperlink ref="C145" r:id="rId366" xr:uid="{B8DA1305-DB70-2A43-8A0A-5086AC200953}"/>
-    <hyperlink ref="C146" r:id="rId367" xr:uid="{A32E6704-71B6-C64F-8C44-8E45ABCB3DD5}"/>
-    <hyperlink ref="C147" r:id="rId368" xr:uid="{75414C14-6E49-8F4F-A100-00774DE6E7B3}"/>
-    <hyperlink ref="C148" r:id="rId369" xr:uid="{CD048E5C-7315-ED41-9DC1-30B18B0F6186}"/>
-    <hyperlink ref="C149" r:id="rId370" xr:uid="{CBD425AF-7CFB-D441-89AA-C4A1EFC7F571}"/>
-    <hyperlink ref="B201" r:id="rId371" xr:uid="{7197ACB3-C33E-734B-BBE9-D327D1DB5402}"/>
-    <hyperlink ref="B205" r:id="rId372" xr:uid="{718283FF-C075-6F45-8844-8AB4A96EDC21}"/>
-    <hyperlink ref="B206" r:id="rId373" xr:uid="{0927B0FA-382D-0B41-B89F-7381B38B9AB6}"/>
-    <hyperlink ref="B207" r:id="rId374" xr:uid="{FD06177F-42A0-854E-9FA5-F28B82F7F4A9}"/>
-    <hyperlink ref="B208" r:id="rId375" xr:uid="{98A13AC8-DF8D-984C-B71C-26F2324FFA33}"/>
-    <hyperlink ref="B209" r:id="rId376" xr:uid="{7D123A10-F21A-5841-8929-AD430797D8B7}"/>
-    <hyperlink ref="B210" r:id="rId377" xr:uid="{B8AD5374-49B4-B747-9070-F3CD48B43977}"/>
-    <hyperlink ref="B217" r:id="rId378" xr:uid="{CB04DAAE-22D3-404A-9B59-41734A925C2C}"/>
-    <hyperlink ref="B219" r:id="rId379" xr:uid="{53EA6710-D57A-7948-8604-F4386503E804}"/>
-    <hyperlink ref="B229" r:id="rId380" xr:uid="{57B4B706-4868-C545-80F2-74B709A3780A}"/>
-    <hyperlink ref="B233" r:id="rId381" xr:uid="{39FE5A64-9EF1-9042-9A70-7B7BEB2DFDBB}"/>
+    <hyperlink ref="C135" r:id="rId251" xr:uid="{BDA7CC67-1472-8248-946E-93B6F618685B}"/>
+    <hyperlink ref="C136" r:id="rId252" xr:uid="{EA63AAC0-2987-5B4D-8CA8-F8E8B820ED36}"/>
+    <hyperlink ref="C137" r:id="rId253" xr:uid="{A66AC424-A7F4-B84A-9280-820A43B4AEBA}"/>
+    <hyperlink ref="C138" r:id="rId254" xr:uid="{E7A6808E-50F2-0948-9C94-628B4F9ACF7D}"/>
+    <hyperlink ref="C139" r:id="rId255" xr:uid="{0B5221E8-DE05-0E4E-9EE3-DCADE66F2696}"/>
+    <hyperlink ref="C140" r:id="rId256" xr:uid="{EA1D837B-5F6A-B54C-9B61-2034B0CE85B3}"/>
+    <hyperlink ref="C141" r:id="rId257" xr:uid="{A3994F4F-3387-1942-A3D6-B8B67EB06BC1}"/>
+    <hyperlink ref="C142" r:id="rId258" xr:uid="{B8D152B1-8B72-E74D-88F6-C43A49A5AB2F}"/>
+    <hyperlink ref="B143" r:id="rId259" xr:uid="{6964114A-F58F-724D-A2B4-173388BA5302}"/>
+    <hyperlink ref="B144" r:id="rId260" xr:uid="{3BD56E0B-D3CE-AD4D-91FA-51D4543B137E}"/>
+    <hyperlink ref="B145" r:id="rId261" xr:uid="{23A75913-BCC4-4E47-9B47-B952CD9112B4}"/>
+    <hyperlink ref="B146" r:id="rId262" xr:uid="{60B2A7C5-DB9E-5F41-B146-74A96ECCE834}"/>
+    <hyperlink ref="C129" r:id="rId263" xr:uid="{F7F12410-9273-7F45-805B-07CE4BFEB9E8}"/>
+    <hyperlink ref="B147" r:id="rId264" xr:uid="{F234784D-26C2-A545-B685-EF602C8D974F}"/>
+    <hyperlink ref="B148" r:id="rId265" xr:uid="{0CF53428-4492-AE40-9C02-9FABA2BA0D3B}"/>
+    <hyperlink ref="B150" r:id="rId266" xr:uid="{6E42F66B-4B80-564E-8A39-545051468745}"/>
+    <hyperlink ref="B151" r:id="rId267" xr:uid="{D200C44B-A95E-434E-B96F-F097A5CB9796}"/>
+    <hyperlink ref="B152" r:id="rId268" xr:uid="{6C870BBD-0FCA-4E4D-8C04-64F66A4CDDBD}"/>
+    <hyperlink ref="B153" r:id="rId269" xr:uid="{13618F8B-EF5F-744B-92F0-4F8047208B03}"/>
+    <hyperlink ref="B154" r:id="rId270" xr:uid="{369A99E5-8534-484F-9378-38EA1F763D49}"/>
+    <hyperlink ref="B155" r:id="rId271" xr:uid="{F755E08D-37B2-7740-8B78-61FD6A0062F8}"/>
+    <hyperlink ref="B156" r:id="rId272" xr:uid="{DE03D456-C44C-C442-8758-FF0ADB5910C9}"/>
+    <hyperlink ref="B157" r:id="rId273" xr:uid="{DD51AED9-A8BF-E340-A7B8-574926029C7A}"/>
+    <hyperlink ref="B158" r:id="rId274" xr:uid="{4106DA73-80ED-0C48-9333-CF22AD9B453B}"/>
+    <hyperlink ref="B159" r:id="rId275" xr:uid="{24AA6FBD-DA03-1641-9CCE-C4125E436587}"/>
+    <hyperlink ref="B160" r:id="rId276" xr:uid="{671C41C7-BBE6-6244-AC5F-C2D5050A9976}"/>
+    <hyperlink ref="B161" r:id="rId277" xr:uid="{0A61AD93-54F4-B64C-A125-A39B41D20037}"/>
+    <hyperlink ref="B162" r:id="rId278" xr:uid="{B21EB3D6-55DF-A648-99FE-B9174BEB51CF}"/>
+    <hyperlink ref="B163" r:id="rId279" xr:uid="{EDD64D5C-42F2-1944-868E-02CE17E0C28C}"/>
+    <hyperlink ref="B165" r:id="rId280" xr:uid="{76E6FFD7-9F09-F545-9058-D27B73251ABF}"/>
+    <hyperlink ref="B166" r:id="rId281" xr:uid="{9ADE58D5-16AC-DC4F-A820-2981CD2C5EE1}"/>
+    <hyperlink ref="C167" r:id="rId282" xr:uid="{8D033399-8CBD-724D-80CD-C7397C3C2A0F}"/>
+    <hyperlink ref="B168" r:id="rId283" xr:uid="{01B1B80B-C304-4D4F-A53E-AB4D0EE61624}"/>
+    <hyperlink ref="B169" r:id="rId284" xr:uid="{F690EC01-0A49-E548-9E56-0EACEA75EA38}"/>
+    <hyperlink ref="B170" r:id="rId285" xr:uid="{7F51F9C1-398D-9749-A281-E22D1309A30E}"/>
+    <hyperlink ref="B171" r:id="rId286" xr:uid="{64214232-7C7F-8444-9AAC-0A4BBD3AF2D1}"/>
+    <hyperlink ref="B172" r:id="rId287" xr:uid="{7AF546D0-B342-424F-A68E-944E05062E8A}"/>
+    <hyperlink ref="B173" r:id="rId288" xr:uid="{0050ED55-AE7F-E64C-87FF-712ACBB46C7D}"/>
+    <hyperlink ref="B174" r:id="rId289" xr:uid="{83754876-42D8-E74F-91FA-9CECBBAC6924}"/>
+    <hyperlink ref="B175" r:id="rId290" xr:uid="{337A6E39-03DD-064F-BF1E-FA6674858C0B}"/>
+    <hyperlink ref="B176" r:id="rId291" xr:uid="{8D3B4445-BD15-E441-B13B-E90EAF62DA8E}"/>
+    <hyperlink ref="B177" r:id="rId292" xr:uid="{F8DCC388-ABD3-2544-8E1A-8EAF5A2DAA9C}"/>
+    <hyperlink ref="B178" r:id="rId293" xr:uid="{BC6EE541-680A-884F-958C-C07EA84B94D8}"/>
+    <hyperlink ref="B179" r:id="rId294" xr:uid="{DD1C41B7-F12D-0B4A-807D-2D572F6BC0DA}"/>
+    <hyperlink ref="B180" r:id="rId295" xr:uid="{456B4E6A-BAF0-1C4B-A5A2-33029913A11F}"/>
+    <hyperlink ref="B181" r:id="rId296" xr:uid="{AB596C81-A2E4-D84E-97FF-F4EDC38B3AB7}"/>
+    <hyperlink ref="B182" r:id="rId297" xr:uid="{6925BDA1-8306-C94C-B344-AC929606B70C}"/>
+    <hyperlink ref="B183" r:id="rId298" xr:uid="{F1F6DFAC-7F73-E242-80A6-0A54A6B92CBA}"/>
+    <hyperlink ref="C184" r:id="rId299" xr:uid="{2B979D45-F5FD-A54F-886F-C8E41EB241BE}"/>
+    <hyperlink ref="B185" r:id="rId300" xr:uid="{A4B83D25-A914-374B-AC70-67BC2B213C2A}"/>
+    <hyperlink ref="B186" r:id="rId301" xr:uid="{F533F9B9-2BCF-A847-AC92-C786DBA1CF4B}"/>
+    <hyperlink ref="B187" r:id="rId302" xr:uid="{6C8BEC30-39CE-A548-BBDD-73A01B452059}"/>
+    <hyperlink ref="B188" r:id="rId303" xr:uid="{85FCE497-9E96-6648-867F-752AA283D510}"/>
+    <hyperlink ref="B189" r:id="rId304" xr:uid="{43C3B803-5A07-A642-8293-EBD66D59834D}"/>
+    <hyperlink ref="C190" r:id="rId305" xr:uid="{31EDEE6A-D8E5-8C48-87E9-064EB36F385C}"/>
+    <hyperlink ref="B191" r:id="rId306" xr:uid="{F9240DAF-1152-804D-82D6-CD96D548238C}"/>
+    <hyperlink ref="B192" r:id="rId307" xr:uid="{DD79C80C-1BE5-F149-88DD-8DA5369DFCAD}"/>
+    <hyperlink ref="B193" r:id="rId308" xr:uid="{B0E436A7-E831-8E4C-9EAC-5207B2FC9DA3}"/>
+    <hyperlink ref="B194" r:id="rId309" xr:uid="{945AD53A-A851-EB4A-B3AC-9B72897828BE}"/>
+    <hyperlink ref="B195" r:id="rId310" xr:uid="{FAEF4F3C-0C71-C542-B31C-BDECF30F1ABE}"/>
+    <hyperlink ref="B196" r:id="rId311" xr:uid="{16789C92-8D31-CA42-A3C5-F457DE323071}"/>
+    <hyperlink ref="B197" r:id="rId312" xr:uid="{C9BB414A-D34A-A743-8C91-1506BC729AF1}"/>
+    <hyperlink ref="B198" r:id="rId313" xr:uid="{7E709984-032A-6D43-B8C0-35BB36F33A8B}"/>
+    <hyperlink ref="B199" r:id="rId314" xr:uid="{AF735B37-2761-6B44-8457-C70F018D475D}"/>
+    <hyperlink ref="C200" r:id="rId315" xr:uid="{F3E9CC02-E232-F247-910C-0F8F818F15FD}"/>
+    <hyperlink ref="B201" r:id="rId316" xr:uid="{CF20CF77-6D17-A640-BC1C-06D8AC56128F}"/>
+    <hyperlink ref="B202" r:id="rId317" xr:uid="{05A67C14-E63C-6643-A98B-DE5374A332F7}"/>
+    <hyperlink ref="B203" r:id="rId318" xr:uid="{2E28DB30-178A-5F43-BABB-5699190A802A}"/>
+    <hyperlink ref="C204" r:id="rId319" xr:uid="{D1AA51DE-D608-3D45-AD22-E8B64F1419E7}"/>
+    <hyperlink ref="C205" r:id="rId320" xr:uid="{9BABC60F-FE82-5248-9E79-B718EC0F659A}"/>
+    <hyperlink ref="C206" r:id="rId321" xr:uid="{03289203-0011-5743-AC70-D84C9B97DC6E}"/>
+    <hyperlink ref="C207" r:id="rId322" xr:uid="{1B79D66B-2C73-624F-A90B-DE414F9850D6}"/>
+    <hyperlink ref="C208" r:id="rId323" xr:uid="{43F13A60-CCD1-0C40-AB37-E9F9EE97732E}"/>
+    <hyperlink ref="C209" r:id="rId324" xr:uid="{1C156BC9-5818-4049-8EF2-B540C3E68E81}"/>
+    <hyperlink ref="B210" r:id="rId325" xr:uid="{53D53A00-1672-664D-91C8-7C5331F6CCA5}"/>
+    <hyperlink ref="B211" r:id="rId326" xr:uid="{515855E3-E3E4-F845-9DC8-E34325F7F3DA}"/>
+    <hyperlink ref="B212" r:id="rId327" xr:uid="{BA928391-E722-7746-BED2-1C83F80C0DBC}"/>
+    <hyperlink ref="B213" r:id="rId328" xr:uid="{102F6A53-9ABC-3E45-BD5C-B9BF66066C2A}"/>
+    <hyperlink ref="B214" r:id="rId329" xr:uid="{1285018C-691B-2E4B-A2D4-583D0B414C1F}"/>
+    <hyperlink ref="B215" r:id="rId330" xr:uid="{76AAE9CF-2707-B143-B652-46D8CE36A647}"/>
+    <hyperlink ref="C216" r:id="rId331" xr:uid="{6F160E9C-28C2-9641-9DFC-22F25114A500}"/>
+    <hyperlink ref="B217" r:id="rId332" xr:uid="{73B6A897-CC12-624B-B420-3142BFB3B7E7}"/>
+    <hyperlink ref="C218" r:id="rId333" xr:uid="{97260B38-6E63-8949-A540-58D6E311FC48}"/>
+    <hyperlink ref="B219" r:id="rId334" xr:uid="{63962B13-F41B-C849-BD6B-055FC35A58D4}"/>
+    <hyperlink ref="B220" r:id="rId335" xr:uid="{76C9DF5E-2957-2841-B4F2-ABA46671CCA0}"/>
+    <hyperlink ref="B221" r:id="rId336" xr:uid="{89A49EA1-C764-B740-A236-82525B727186}"/>
+    <hyperlink ref="B222" r:id="rId337" xr:uid="{ECE997AF-CE38-B24F-ADBF-641D516BA06C}"/>
+    <hyperlink ref="C223" r:id="rId338" xr:uid="{E42A850B-432C-BD4F-ADAD-269074FD12D7}"/>
+    <hyperlink ref="B224" r:id="rId339" xr:uid="{C1923A14-8FC3-3048-929B-76B8E6CABE4E}"/>
+    <hyperlink ref="B225" r:id="rId340" xr:uid="{FB93A9DD-F604-164C-8539-EE9D683EAE3F}"/>
+    <hyperlink ref="B226" r:id="rId341" xr:uid="{3ED03127-35DA-8A49-93C9-896BA1D8DC06}"/>
+    <hyperlink ref="B227" r:id="rId342" xr:uid="{6AECACA9-7563-5844-88E8-65163C3C2045}"/>
+    <hyperlink ref="C228" r:id="rId343" xr:uid="{8922321F-CDC7-5A46-838D-8D1A2F011DBC}"/>
+    <hyperlink ref="B229" r:id="rId344" xr:uid="{97E5BE47-CB30-1E45-9F11-15A6DE53936E}"/>
+    <hyperlink ref="B230" r:id="rId345" xr:uid="{B055B99F-8704-CA44-985E-FEE3A9E3B3EB}"/>
+    <hyperlink ref="B231" r:id="rId346" xr:uid="{5FEA98AF-8D00-C041-8FAA-30E8369F763B}"/>
+    <hyperlink ref="C232" r:id="rId347" xr:uid="{6782F7DA-4236-7740-A30E-EFCC23B81659}"/>
+    <hyperlink ref="B233" r:id="rId348" xr:uid="{ECA5F0C7-3864-ED48-B6A1-19E564969867}"/>
+    <hyperlink ref="B149" r:id="rId349" xr:uid="{C9B92141-6E73-914D-864F-BCF52A0441AB}"/>
+    <hyperlink ref="B106" r:id="rId350" xr:uid="{D9B7A9AA-835A-D440-B1F8-5FD8BA13EDDD}"/>
+    <hyperlink ref="B107" r:id="rId351" xr:uid="{7D9A8CFA-B72E-A545-A9FF-EDF4FCCB10D2}"/>
+    <hyperlink ref="B108" r:id="rId352" xr:uid="{1FDFABF3-4AC9-E94F-8F18-8D411A8F2A41}"/>
+    <hyperlink ref="B127" r:id="rId353" xr:uid="{0B90C06A-4AA3-7D4C-9151-0A8E86D33CF7}"/>
+    <hyperlink ref="B130" r:id="rId354" xr:uid="{41F8EA90-1905-5C44-A76E-C2835343544D}"/>
+    <hyperlink ref="B134" r:id="rId355" xr:uid="{FCCEDAA3-5F09-8F4E-A216-B145A130752A}"/>
+    <hyperlink ref="B135" r:id="rId356" xr:uid="{4CFCEB5C-9EA6-444B-B4A2-DFCB393B2F22}"/>
+    <hyperlink ref="B136" r:id="rId357" xr:uid="{9A0771D2-A3EE-1A4B-9800-411D74964533}"/>
+    <hyperlink ref="B138" r:id="rId358" xr:uid="{2185F98B-0A23-8744-A78F-0879B84BE337}"/>
+    <hyperlink ref="B139" r:id="rId359" xr:uid="{C24EAB49-5746-464B-9358-7B4ED4CF07C0}"/>
+    <hyperlink ref="B140" r:id="rId360" xr:uid="{7A760695-4FA5-784E-A939-A62BC029D8EE}"/>
+    <hyperlink ref="B141" r:id="rId361" xr:uid="{FB8F38DD-E9D5-474F-BE8C-E340D4584463}"/>
+    <hyperlink ref="B142" r:id="rId362" xr:uid="{A5739124-C2FB-7D4A-A75F-F924EE1B685A}"/>
+    <hyperlink ref="C143" r:id="rId363" xr:uid="{344639F6-7829-3644-88B4-2E8EADF8B352}"/>
+    <hyperlink ref="C144" r:id="rId364" xr:uid="{B8DA1305-DB70-2A43-8A0A-5086AC200953}"/>
+    <hyperlink ref="C145" r:id="rId365" xr:uid="{A32E6704-71B6-C64F-8C44-8E45ABCB3DD5}"/>
+    <hyperlink ref="C146" r:id="rId366" xr:uid="{75414C14-6E49-8F4F-A100-00774DE6E7B3}"/>
+    <hyperlink ref="C147" r:id="rId367" xr:uid="{CD048E5C-7315-ED41-9DC1-30B18B0F6186}"/>
+    <hyperlink ref="C148" r:id="rId368" xr:uid="{CBD425AF-7CFB-D441-89AA-C4A1EFC7F571}"/>
+    <hyperlink ref="B200" r:id="rId369" xr:uid="{7197ACB3-C33E-734B-BBE9-D327D1DB5402}"/>
+    <hyperlink ref="B204" r:id="rId370" xr:uid="{718283FF-C075-6F45-8844-8AB4A96EDC21}"/>
+    <hyperlink ref="B205" r:id="rId371" xr:uid="{0927B0FA-382D-0B41-B89F-7381B38B9AB6}"/>
+    <hyperlink ref="B206" r:id="rId372" xr:uid="{FD06177F-42A0-854E-9FA5-F28B82F7F4A9}"/>
+    <hyperlink ref="B207" r:id="rId373" xr:uid="{98A13AC8-DF8D-984C-B71C-26F2324FFA33}"/>
+    <hyperlink ref="B208" r:id="rId374" xr:uid="{7D123A10-F21A-5841-8929-AD430797D8B7}"/>
+    <hyperlink ref="B209" r:id="rId375" xr:uid="{B8AD5374-49B4-B747-9070-F3CD48B43977}"/>
+    <hyperlink ref="B216" r:id="rId376" xr:uid="{CB04DAAE-22D3-404A-9B59-41734A925C2C}"/>
+    <hyperlink ref="B218" r:id="rId377" xr:uid="{53EA6710-D57A-7948-8604-F4386503E804}"/>
+    <hyperlink ref="B228" r:id="rId378" xr:uid="{57B4B706-4868-C545-80F2-74B709A3780A}"/>
+    <hyperlink ref="B232" r:id="rId379" xr:uid="{39FE5A64-9EF1-9042-9A70-7B7BEB2DFDBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
clean up a few entries
</commit_message>
<xml_diff>
--- a/FOSS4Spec.xlsx
+++ b/FOSS4Spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanh/Documents/Professional/Research/R_Pkgs/FOSS4Spectroscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914042E0-B3EC-E043-A137-9D19706018B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40156B8-97B1-2841-853B-96637E627C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="500" windowWidth="23740" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="1100">
   <si>
     <t>name</t>
   </si>
@@ -3689,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187:XFD187"/>
+    <sheetView tabSelected="1" topLeftCell="B235" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G247" sqref="G247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11536,6 +11536,12 @@
       </c>
       <c r="E246" t="s">
         <v>1083</v>
+      </c>
+      <c r="F246" t="s">
+        <v>27</v>
+      </c>
+      <c r="G246" t="s">
+        <v>168</v>
       </c>
       <c r="J246" t="s">
         <v>1084</v>

</xml_diff>